<commit_message>
[LC] Update prompt for gpt to help me scale solution to similar problems.
</commit_message>
<xml_diff>
--- a/Leetcode/Problem-tracker.xlsx
+++ b/Leetcode/Problem-tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27930" windowHeight="12975"/>
+    <workbookView windowWidth="27945" windowHeight="12960"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
+  <si>
+    <t>Prompt</t>
+  </si>
+  <si>
+    <t>Problem Name: "Two sums" (LeetCode 1)
+Instructions:
+1. Provide the **problem pattern** and **solution approach**.
+2. Explain the **algorithm used** 
+3. List **when to use this pattern** and how it scales to similar problems.
+4. Format the output as:
+    - **Problem Pattern/Solution:** Describe the pattern &amp; solution strategy.
+    - **When to Use/Scale:** Provide 2-3 bullet points on when to apply this approach.</t>
+  </si>
   <si>
     <t>No.</t>
   </si>
@@ -43,7 +56,10 @@
     <t>Tag</t>
   </si>
   <si>
-    <t>Comment</t>
+    <t>Problem Pattern/Solution</t>
+  </si>
+  <si>
+    <t>When to use/scale</t>
   </si>
   <si>
     <t>Link</t>
@@ -61,7 +77,13 @@
     <t>Hash table</t>
   </si>
   <si>
-    <t>Hashmap+one pas; If sorted, two pointers can be used</t>
+    <t>Pattern: Array and sequence-based problem requiring pair lookup.
+Solution: Use a hash map (dictionary) to store seen elements and their indices. Perform one-pass lookup to find the complement (target - num). Runs in O(n) time with O(n) space.</t>
+  </si>
+  <si>
+    <t>1. Finding pairs, complements, subarrays, substrings efficiently.
+2. Unsorted input where quick lookups are required (if sorted, two-pointer method can be used).
+3. Order matters, indices matter (e.g., return index positions, track elements dynamically).</t>
   </si>
   <si>
     <t>https://leetcode.com/problems/two-sum/description/</t>
@@ -188,6 +210,21 @@
   </si>
   <si>
     <t>Generate Parentheses</t>
+  </si>
+  <si>
+    <t>Best Time to Buy and Sell Stock</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>Problem Pattern: Single-pass greedy approach; Maintain a min price tracker while iterating and compute max profit dynamically.
+Solution Approach: Iterate through prices, track the minimum price so far, and compute the maximum profit using max_profit = max(max_profit, price - min_price). This runs in O(n) time and O(1) space.</t>
+  </si>
+  <si>
+    <t>1. Finding max/min differences in a single pass (e.g., max temperature difference, longest price drop).
+2. When order matters (e.g., can't rearrange elements).
+3. When solving range-based max/min problems (e.g., max subarray sum, trapping rainwater).</t>
   </si>
 </sst>
 </file>
@@ -816,7 +853,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -831,9 +868,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1146,356 +1180,397 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="25.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.25" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="55.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="45.75" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="1"/>
+    <col min="5" max="5" width="46.25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="62.625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="45.75" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="3" t="s">
+    <row r="1" ht="165" customHeight="1" spans="1:7">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1">
+      <c r="F2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" ht="85.5" spans="1:8">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1">
-        <v>973</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
-        <v>23</v>
+        <v>973</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1">
-        <v>542</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1">
-        <v>733</v>
+        <v>542</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
-        <v>200</v>
+        <v>733</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1">
-        <v>235</v>
+        <v>200</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1">
-        <v>104</v>
+        <v>226</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1">
-        <v>232</v>
+        <v>104</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
-        <v>20</v>
+        <v>232</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1">
-        <v>225</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1">
-        <v>206</v>
+        <v>141</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
-        <v>54</v>
+        <v>206</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1">
-        <v>704</v>
+        <v>33</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1">
-        <v>78</v>
+        <v>704</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1">
+        <v>77</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3">
+      <c r="B23" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="C23" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" ht="99.75" spans="1:8">
+      <c r="A24" s="1">
+        <v>121</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>

<commit_message>
[LC] Update Trie notes and 208 Implement Trie.
</commit_message>
<xml_diff>
--- a/Leetcode/Problem-tracker.xlsx
+++ b/Leetcode/Problem-tracker.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
   <si>
     <t>Prompt</t>
   </si>
@@ -225,6 +225,48 @@
     <t>1. Finding max/min differences in a single pass (e.g., max temperature difference, longest price drop).
 2. When order matters (e.g., can't rearrange elements).
 3. When solving range-based max/min problems (e.g., max subarray sum, trapping rainwater).</t>
+  </si>
+  <si>
+    <t>Implement Trie (Prefix Tree)</t>
+  </si>
+  <si>
+    <t>2025.2.12</t>
+  </si>
+  <si>
+    <t>Trie</t>
+  </si>
+  <si>
+    <t>Problem Pattern: This problem follows the Tree-based Prefix Search Pattern, where a Trie (Prefix Tree) is used to efficiently store and retrieve strings.
+Solution Approach: A Trie is implemented using a nested dictionary (hash map) or a class-based tree structure where each node has links to its child characters and a flag for word completion. Insertions, searches, and prefix checks run in O(n) time, where n is the length of the word.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Efficient </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>prefix-based</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> searching (e.g., autocomplete, word search, dictionary lookups).
+2. Fast retrieval and storage of string-based data (e.g., IP routing, spell checking).
+3. When hash maps are insufficient due to key overlap (e.g., when prefixes must be efficiently queried).</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/implement-trie-prefix-tree/description/</t>
   </si>
 </sst>
 </file>
@@ -1180,10 +1222,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -1194,12 +1236,12 @@
     <col min="4" max="4" width="16.625" style="1" customWidth="1"/>
     <col min="5" max="5" width="46.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="62.625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="45.75" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.25" style="2" customWidth="1"/>
     <col min="8" max="8" width="23.5" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="165" customHeight="1" spans="1:7">
+    <row r="1" ht="165" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1209,8 +1251,6 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
@@ -1231,7 +1271,7 @@
       <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1257,7 +1297,7 @@
       <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -1565,12 +1605,38 @@
       </c>
       <c r="H24" s="1" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="25" ht="114" spans="1:7">
+      <c r="A25" s="1">
+        <v>208</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:G1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G25" r:id="rId1" display="https://leetcode.com/problems/implement-trie-prefix-tree/description/"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
@@ -1583,7 +1649,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1600,7 +1666,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
[LC] Update 5 question reviews for array.
</commit_message>
<xml_diff>
--- a/Leetcode/Problem-tracker.xlsx
+++ b/Leetcode/Problem-tracker.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
   <si>
     <t>Prompt</t>
   </si>
@@ -173,7 +173,7 @@
     <t>Linked List Cycle</t>
   </si>
   <si>
-    <t>2025.2.0</t>
+    <t>2025.1.31</t>
   </si>
   <si>
     <t>Linked List</t>
@@ -182,49 +182,108 @@
     <t>Reverse Linked List</t>
   </si>
   <si>
+    <t>2025.1.30</t>
+  </si>
+  <si>
     <t>Spiral Matrix</t>
   </si>
   <si>
+    <t>2025.1.29</t>
+  </si>
+  <si>
     <t>Matrix</t>
   </si>
   <si>
     <t>Set Matrix Zeros</t>
   </si>
   <si>
+    <t>2025.1.28</t>
+  </si>
+  <si>
     <t>Search in rotated sorted array</t>
   </si>
   <si>
+    <t>2025.1.27</t>
+  </si>
+  <si>
     <t>Search &amp; Sort</t>
   </si>
   <si>
     <t>Binary Search</t>
   </si>
   <si>
+    <t>2025.1.26</t>
+  </si>
+  <si>
     <t>Subsets</t>
   </si>
   <si>
+    <t>2025.1.25</t>
+  </si>
+  <si>
     <t>Recursion</t>
   </si>
   <si>
     <t>Combination</t>
   </si>
   <si>
+    <t>2025.1.24</t>
+  </si>
+  <si>
     <t>Generate Parentheses</t>
   </si>
   <si>
+    <t>2025.1.23</t>
+  </si>
+  <si>
     <t>Best Time to Buy and Sell Stock</t>
   </si>
   <si>
-    <t>Array</t>
+    <t>Array; Sub-array</t>
   </si>
   <si>
     <t>Problem Pattern: Single-pass greedy approach; Maintain a min price tracker while iterating and compute max profit dynamically.
 Solution Approach: Iterate through prices, track the minimum price so far, and compute the maximum profit using max_profit = max(max_profit, price - min_price). This runs in O(n) time and O(1) space.</t>
   </si>
   <si>
-    <t>1. Finding max/min differences in a single pass (e.g., max temperature difference, longest price drop).
+    <r>
+      <t xml:space="preserve">1. Finding max/min differences in a single pass (e.g., max temperature difference, longest price drop).
 2. When order matters (e.g., can't rearrange elements).
-3. When solving range-based max/min problems (e.g., max subarray sum, trapping rainwater).</t>
+3. When solving range-based max/min problems (e.g., </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>max subarray sum-contiguous</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">, trapping rainwater).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Just differences between two discrete points, not contiguous sum</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock/description/</t>
   </si>
   <si>
     <t>Implement Trie (Prefix Tree)</t>
@@ -241,6 +300,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. Efficient </t>
     </r>
     <r>
@@ -267,6 +332,307 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/implement-trie-prefix-tree/description/</t>
+  </si>
+  <si>
+    <t>Product of Array Except Self</t>
+  </si>
+  <si>
+    <t>Array; Prefix&amp;Suffix</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: This problem follows the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Prefix &amp; Suffix Product</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> Pattern, where we compute prefix and suffix products to solve the problem in O(n) time without division.
+Solution Approach: Use two passes: (1) Forward pass to compute prefix products, and (2) Backward pass to multiply suffix products. This avoids division and uses O(1) extra space (excluding output array).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Solved second time but not come up with the best solution using O(1) space</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When computing array transformations in O(n) without extra space (e.g., </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>sum/product modifications</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">).
+2. When a problem involves </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>modifying an array based on other elements</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> but without using division (e.g., cumulative sum/product).
+3. When </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>prefix/suffix computations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> are optimal over brute force (e.g., rainwater trapping, sum ranges).</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/product-of-array-except-self/description/</t>
+  </si>
+  <si>
+    <t>2025.2.12; 2024.11.3</t>
+  </si>
+  <si>
+    <t>Maximum Subarray</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: This problem follows the "Maximum Subarray Sum with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Dynamic Tracking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">" pattern. The key is to track a running sum and reset it when it becomes negative.
+Solution Approach: Kadane’s Algorithm iterates through the array while maintaining a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>current sum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>global maximum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> sum. If the sum becomes negative, reset it to zero to start a new subarray. This ensures an O(n) time complexity with O(1) space complexity.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Did not solve second time</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Finding the maximum sum of a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>contiguous subarray</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> efficiently in O(n).
+2. When deciding whether to extend or restart a sequence dynamically.
+3. Optimizing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>subarray-based problems</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> where negative values impact the total (e.g., stock prices, dynamic range calculations).</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-subarray/description/</t>
+  </si>
+  <si>
+    <t>2025.2.12; 2024.11.4</t>
+  </si>
+  <si>
+    <t>Contains Duplicate</t>
+  </si>
+  <si>
+    <t>Hash set</t>
+  </si>
+  <si>
+    <t>Problem Pattern: This problem follows the "Duplicate Detection" pattern, where a set is used to efficiently track previously seen elements.
+Solution Approach: Iterate through the array while inserting elements into a hash set. If an element is already in the set, return True (duplicate found). If the loop completes, return False. This runs in O(n) time and O(n) space.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When checking for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>duplicate elements</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> in an array efficiently.
+2. When </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>order doesn’t matter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>, but uniqueness is required.
+3. When fast lookups (O(1)) are needed instead of sorting (O(n log n)).</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/contains-duplicate/description/</t>
+  </si>
+  <si>
+    <t>2025.2.12; 2024.11.5</t>
   </si>
 </sst>
 </file>
@@ -279,7 +645,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -444,8 +810,15 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -454,6 +827,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -616,12 +1001,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -639,12 +1018,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -771,7 +1165,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -783,121 +1177,124 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -905,11 +1302,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1222,413 +1637,588 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="25.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="46.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="62.625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25.25" style="2" customWidth="1"/>
-    <col min="8" max="8" width="23.5" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="6.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.25" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="46.25" style="2" customWidth="1"/>
+    <col min="6" max="6" width="62.625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="25.25" style="3" customWidth="1"/>
+    <col min="8" max="8" width="23.5" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="165" customHeight="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="165" customHeight="1" spans="1:8">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="3" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:8">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" ht="85.5" spans="1:8">
-      <c r="A3" s="1">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1">
+    <row r="4" spans="1:8">
+      <c r="A4" s="9">
         <v>973</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1">
+      <c r="E4" s="6"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="9">
         <v>23</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1">
+      <c r="E5" s="6"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="9">
         <v>542</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1">
+      <c r="E6" s="6"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="9">
         <v>733</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1">
+      <c r="E7" s="6"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="9">
         <v>200</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1">
+      <c r="E8" s="6"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="9">
         <v>235</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1">
+      <c r="E9" s="6"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="9">
         <v>226</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1">
+      <c r="E10" s="6"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="9">
         <v>104</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1">
+      <c r="E11" s="6"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="9">
         <v>232</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1">
+      <c r="E12" s="6"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="9">
         <v>20</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1">
+      <c r="E13" s="6"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="9">
         <v>225</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="1">
+      <c r="E14" s="6"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="9">
         <v>141</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1">
+      <c r="E15" s="6"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="9">
         <v>206</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="C16" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1">
+      <c r="E16" s="6"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="9">
         <v>54</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="B17" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1">
+      <c r="C17" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="9">
         <v>73</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1">
+      <c r="B18" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="9">
         <v>33</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1">
+      <c r="B19" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="9">
         <v>704</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1">
+      <c r="B20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="9">
         <v>78</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="9">
+        <v>77</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="9">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" ht="99.75" spans="1:8">
+      <c r="A24" s="4">
+        <v>121</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" ht="114" spans="1:8">
+      <c r="A25" s="9">
+        <v>208</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" ht="142.5" spans="1:8">
+      <c r="A26" s="10">
+        <v>238</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" ht="142.5" spans="1:8">
+      <c r="A27" s="10">
         <v>53</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1">
-        <v>77</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" ht="99.75" spans="1:8">
-      <c r="A24" s="1">
-        <v>121</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" ht="114" spans="1:7">
-      <c r="A25" s="1">
-        <v>208</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G25" s="2" t="s">
+      <c r="B27" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>66</v>
       </c>
+      <c r="E27" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" ht="114" spans="1:8">
+      <c r="A28" s="4">
+        <v>217</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="4"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
[LC] Update notes for Interval and 56 Merge Intervals.
</commit_message>
<xml_diff>
--- a/Leetcode/Problem-tracker.xlsx
+++ b/Leetcode/Problem-tracker.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="99">
   <si>
     <t>Prompt</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. Finding max/min differences in a single pass (e.g., max temperature difference, longest price drop).
 2. When order matters (e.g., can't rearrange elements).
 3. When solving range-based max/min problems (e.g., </t>
@@ -341,6 +347,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the </t>
     </r>
     <r>
@@ -377,6 +389,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When computing array transformations in O(n) without extra space (e.g., </t>
     </r>
     <r>
@@ -450,6 +468,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Maximum Subarray Sum with </t>
     </r>
     <r>
@@ -524,6 +548,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. Finding the maximum sum of a </t>
     </r>
     <r>
@@ -585,6 +615,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When checking for </t>
     </r>
     <r>
@@ -633,6 +669,88 @@
   </si>
   <si>
     <t>2025.2.12; 2024.11.5</t>
+  </si>
+  <si>
+    <t>Merge Intervals</t>
+  </si>
+  <si>
+    <t>2025.2.13</t>
+  </si>
+  <si>
+    <t>Array; Intervals</t>
+  </si>
+  <si>
+    <r>
+      <t>Problem Pattern: This problem follows the "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Sorting + Merging Overlapping</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> Intervals" pattern. The key is to sort intervals by start time and then merge overlapping intervals greedily.
+Solution Approach: Sort the intervals by their start time, then iterate through the sorted list, merging overlapping intervals by updating the end time of the last merged interval. This runs in O(n log n) time due to sorting and O(n) space for the output list.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When dealing with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>overlapping intervals</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> that need merging.
+2. When handling scheduling problems like booking rooms, meeting times, or range merging.
+3. When </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>sorting simplifies</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> the problem by providing structure for greedy merging.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-intervals/description/</t>
   </si>
 </sst>
 </file>
@@ -1639,8 +1757,8 @@
   <sheetPr/>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -2210,14 +2328,28 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="4"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+    <row r="29" ht="128.25" spans="1:8">
+      <c r="A29" s="4">
+        <v>56</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="H29" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[LC/DATA200] Update lecture 7 notes and 3 questions review for array.
</commit_message>
<xml_diff>
--- a/Leetcode/Problem-tracker.xlsx
+++ b/Leetcode/Problem-tracker.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="113">
   <si>
     <t>Prompt</t>
   </si>
@@ -203,16 +203,47 @@
     <t>Search in rotated sorted array</t>
   </si>
   <si>
-    <t>2025.1.27</t>
+    <t>2025.2.13</t>
+  </si>
+  <si>
+    <t>Array; Binary Search</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: This problem follows the "Binary Search in Rotated Sorted Array" pattern. The key is to identify which half of the array is sorted and then decide whether to search in that half or the other.
+Solution Approach: Perform modified binary search: (1) Identify the sorted half of the array, (2) Determine if the target lies in the sorted half, (3) Adjust the search space accordingly. This runs in O(log n) time and O(1) space.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Solved second time in 15'23'' but not optimal in O(1) space complexity</t>
+    </r>
+  </si>
+  <si>
+    <t>1. When searching in a rotated sorted array efficiently using O(log n) binary search.
+2. When solving problems where array order is disrupted but retains some structure.
+3. When a normal binary search doesn’t work due to rotation or pivoted shifts.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/search-in-rotated-sorted-array/description/</t>
+  </si>
+  <si>
+    <t>2025.2.13; 2025.1.27; 2024.11.6</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>2025.1.26</t>
   </si>
   <si>
     <t>Search &amp; Sort</t>
-  </si>
-  <si>
-    <t>Binary Search</t>
-  </si>
-  <si>
-    <t>2025.1.26</t>
   </si>
   <si>
     <t>Subsets</t>
@@ -674,13 +705,16 @@
     <t>Merge Intervals</t>
   </si>
   <si>
-    <t>2025.2.13</t>
-  </si>
-  <si>
     <t>Array; Intervals</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t>Problem Pattern: This problem follows the "</t>
     </r>
     <r>
@@ -701,11 +735,18 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve"> Intervals" pattern. The key is to sort intervals by start time and then merge overlapping intervals greedily.
-Solution Approach: Sort the intervals by their start time, then iterate through the sorted list, merging overlapping intervals by updating the end time of the last merged interval. This runs in O(n log n) time due to sorting and O(n) space for the output list.</t>
-    </r>
-  </si>
-  <si>
-    <r>
+Solution Approach: Sort the intervals by their start time, then iterate through the sorted list, merging overlapping intervals by updating the end time of the last merged interval. This runs in O(n log n) time due to sorting and O(n) space for the output list.
+Solved in 18' first time</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When dealing with </t>
     </r>
     <r>
@@ -751,6 +792,251 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/merge-intervals/description/</t>
+  </si>
+  <si>
+    <t>Maximum Product Subarray</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: This problem follows the "Dynamic Range Tracking with Min/Max" pattern, where we track both the maximum and minimum product at each step to handle negative numbers.
+Solution Approach: Iterate through the array while maintaining two values: (1) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>max product</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> so far, and (2) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>min product</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> so far (to account for negative values flipping signs). If the current number is negative, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>swap max/min before updating</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">. This runs in O(n) time and O(1) space.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Not solved second time</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">1. When finding max/min values in a subarray while considering negative flips. - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>non-monotonic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+2. When multiplication is involved, making standard sum-based Kadane’s algorithm insufficient.
+3. When tracking both min/max dynamically is necessary for optimal subarrays.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-product-subarray/description/</t>
+  </si>
+  <si>
+    <t>3 Sums</t>
+  </si>
+  <si>
+    <t>Array; Sorting</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: This problem follows the "Sorting + Two Pointers" pattern, which is commonly used for sum problems where we need to find multiple numbers that satisfy a condition.
+Solution Approach: Sort the array, then </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>fix one number and use two pointers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> to find the remaining two numbers that sum to zero. This avoids duplicate results and ensures an efficient solution in O(n²) time complexity.
+why sort first:
+Once sorted, 
+Efficient duplicate handling </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>✅</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+The Two-Pointer Technique </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>✅</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+Early stopping to avoid unnecessary checks  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>✅</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Not solved second time</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When solving problems that involve </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>finding k numbers that sum to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> a target efficiently.
+2. When sorting allows structured searching instead of brute-force checking.
+3. When handling duplicate results needs a systematic approach (e.g., removing duplicate triplets).</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/3sum/description/</t>
+  </si>
+  <si>
+    <t>2025.2.13; 2024.11.6</t>
   </si>
 </sst>
 </file>
@@ -763,7 +1049,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -929,6 +1215,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1407,7 +1699,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1438,11 +1730,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1755,10 +2062,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -1770,7 +2077,7 @@
     <col min="5" max="5" width="46.25" style="2" customWidth="1"/>
     <col min="6" max="6" width="62.625" style="3" customWidth="1"/>
     <col min="7" max="7" width="25.25" style="3" customWidth="1"/>
-    <col min="8" max="8" width="23.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="44.25" style="2" customWidth="1"/>
     <col min="9" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
@@ -2110,8 +2417,8 @@
       <c r="G18" s="5"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="9">
+    <row r="19" ht="142.5" spans="1:8">
+      <c r="A19" s="10">
         <v>33</v>
       </c>
       <c r="B19" s="6" t="s">
@@ -2123,23 +2430,31 @@
       <c r="D19" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="6"/>
+      <c r="E19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="9">
         <v>704</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="5"/>
@@ -2151,13 +2466,13 @@
         <v>78</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="5"/>
@@ -2169,13 +2484,13 @@
         <v>77</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="5"/>
@@ -2187,13 +2502,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="5"/>
@@ -2205,22 +2520,22 @@
         <v>121</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>16</v>
@@ -2231,75 +2546,75 @@
         <v>208</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C25" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" ht="142.5" spans="1:8">
+      <c r="A26" s="12">
+        <v>238</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" ht="142.5" spans="1:8">
+      <c r="A27" s="12">
+        <v>53</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H25" s="6"/>
-    </row>
-    <row r="26" ht="142.5" spans="1:8">
-      <c r="A26" s="10">
-        <v>238</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" ht="142.5" spans="1:8">
-      <c r="A27" s="10">
-        <v>53</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="E27" s="5" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" ht="114" spans="1:8">
@@ -2307,50 +2622,110 @@
         <v>217</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C28" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" ht="142.5" spans="1:8">
+      <c r="A29" s="9">
+        <v>56</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" ht="156.75" spans="1:8">
+      <c r="A30" s="12">
+        <v>152</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D28" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" ht="128.25" spans="1:8">
-      <c r="A29" s="4">
-        <v>56</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="H29" s="6"/>
+      <c r="E30" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" ht="199.5" spans="1:8">
+      <c r="A31" s="14">
+        <v>15</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="H31" s="15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="16"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
[LC] Update 57 insert intervals.
</commit_message>
<xml_diff>
--- a/Leetcode/Problem-tracker.xlsx
+++ b/Leetcode/Problem-tracker.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="119">
   <si>
     <t>Prompt</t>
   </si>
@@ -210,6 +210,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Binary Search in Rotated Sorted Array" pattern. The key is to identify which half of the array is sorted and then decide whether to search in that half or the other.
 Solution Approach: Perform modified binary search: (1) Identify the sorted half of the array, (2) Determine if the target lies in the sorted half, (3) Adjust the search space accordingly. This runs in O(log n) time and O(1) space.
 </t>
@@ -798,6 +804,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Dynamic Range Tracking with Min/Max" pattern, where we track both the maximum and minimum product at each step to handle negative numbers.
 Solution Approach: Iterate through the array while maintaining two values: (1) </t>
     </r>
@@ -913,6 +925,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Sorting + Two Pointers" pattern, which is commonly used for sum problems where we need to find multiple numbers that satisfy a condition.
 Solution Approach: Sort the array, then </t>
     </r>
@@ -1008,6 +1026,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When solving problems that involve </t>
     </r>
     <r>
@@ -1037,6 +1061,81 @@
   </si>
   <si>
     <t>2025.2.13; 2024.11.6</t>
+  </si>
+  <si>
+    <t>Insert Intervals</t>
+  </si>
+  <si>
+    <t>2025.2.14</t>
+  </si>
+  <si>
+    <t>Intervals</t>
+  </si>
+  <si>
+    <r>
+      <t>Problem Pattern: This problem follows the "Merging Intervals with Insertion" pattern. The key is to insert an interval into an already sorted list of intervals while maintaining order and merging overlaps.
+Solution Approach: Iterate through the list while adding non-overlapping intervals directly. Once an overlap is found, merge it with the new interval. Continue until all remaining intervals are added. This runs in O(n) time complexity with O(n) space.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+Same issue like the previous 56 one, we should not have a function to check if overlap, cause if they two did overlap, it will be working well. But if there's not overlap, the inserted one could be in front of or behind the current interval, that will be another condition check.
+Not solved first time</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When inserting and merging intervals efficiently while maintaining order.
+2. When handling </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>scheduling problems</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> like booking times, meeting slots, or event ranges.
+3. When dealing with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ordered data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> where merging or insertion is required without full sorting.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/insert-interval/description/</t>
   </si>
 </sst>
 </file>
@@ -1699,7 +1798,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1733,23 +1832,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2064,8 +2151,8 @@
   <sheetPr/>
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -2436,7 +2523,7 @@
       <c r="F19" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="5" t="s">
         <v>58</v>
       </c>
       <c r="H19" s="6" t="s">
@@ -2566,10 +2653,10 @@
       <c r="H25" s="6"/>
     </row>
     <row r="26" ht="142.5" spans="1:8">
-      <c r="A26" s="12">
+      <c r="A26" s="11">
         <v>238</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="12" t="s">
         <v>81</v>
       </c>
       <c r="C26" s="6" t="s">
@@ -2592,10 +2679,10 @@
       </c>
     </row>
     <row r="27" ht="142.5" spans="1:8">
-      <c r="A27" s="12">
+      <c r="A27" s="11">
         <v>53</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="12" t="s">
         <v>87</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -2668,7 +2755,7 @@
       <c r="H29" s="6"/>
     </row>
     <row r="30" ht="156.75" spans="1:8">
-      <c r="A30" s="12">
+      <c r="A30" s="11">
         <v>152</v>
       </c>
       <c r="B30" s="6" t="s">
@@ -2692,40 +2779,54 @@
       <c r="H30" s="6"/>
     </row>
     <row r="31" ht="199.5" spans="1:8">
-      <c r="A31" s="14">
+      <c r="A31" s="11">
         <v>15</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F31" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="H31" s="15" t="s">
+      <c r="H31" s="6" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="16"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="15"/>
+    <row r="32" ht="228" spans="1:8">
+      <c r="A32" s="11">
+        <v>57</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H32" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
[LC/CS231n] Update notes for dp, update 70 climbing stairs, and create a notebook for cs231n.
</commit_message>
<xml_diff>
--- a/Leetcode/Problem-tracker.xlsx
+++ b/Leetcode/Problem-tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12960"/>
+    <workbookView windowWidth="22188" windowHeight="9767"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="125">
   <si>
     <t>Prompt</t>
   </si>
@@ -1073,6 +1073,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t>Problem Pattern: This problem follows the "Merging Intervals with Insertion" pattern. The key is to insert an interval into an already sorted list of intervals while maintaining order and merging overlaps.
 Solution Approach: Iterate through the list while adding non-overlapping intervals directly. Once an overlap is found, merge it with the new interval. Continue until all remaining intervals are added. This runs in O(n) time complexity with O(n) space.</t>
     </r>
@@ -1091,6 +1097,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When inserting and merging intervals efficiently while maintaining order.
 2. When handling </t>
     </r>
@@ -1136,6 +1148,40 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/insert-interval/description/</t>
+  </si>
+  <si>
+    <t>Climbing Stairs</t>
+  </si>
+  <si>
+    <t>2025.2.15</t>
+  </si>
+  <si>
+    <t>DP</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: This problem follows the "Dynamic Programming - Fibonacci Sequence" pattern. The key is recognizing that the number of ways to reach step n is the sum of ways to reach n-1 and n-2 because you can climb 1 or 2 steps at a time.
+Solution Approach: Use a bottom-up dynamic programming (DP) approach to compute the number of ways iteratively. The optimized solution runs in O(n) time with O(1) space by storing only the last two computed values.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Not solved first time, draw a decision tree helps a lot</t>
+    </r>
+  </si>
+  <si>
+    <t>1. When solving problems that follow the Fibonacci-like recurrence relation.
+2. When optimizing recursive backtracking using dynamic programming.
+3. When computing combinatorial step problems (e.g., number of paths in a grid).</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/climbing-stairs/description/</t>
   </si>
 </sst>
 </file>
@@ -1314,16 +1360,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -1798,7 +1844,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1837,6 +1883,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2149,20 +2204,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A30" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="6.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.6296296296296" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.25" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.6296296296296" style="2" customWidth="1"/>
     <col min="5" max="5" width="46.25" style="2" customWidth="1"/>
-    <col min="6" max="6" width="62.625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="62.6296296296296" style="3" customWidth="1"/>
     <col min="7" max="7" width="25.25" style="3" customWidth="1"/>
     <col min="8" max="8" width="44.25" style="2" customWidth="1"/>
     <col min="9" max="16384" width="9" style="2"/>
@@ -2208,7 +2263,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" ht="85.5" spans="1:8">
+    <row r="3" ht="82.8" spans="1:8">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -2504,7 +2559,7 @@
       <c r="G18" s="5"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" ht="142.5" spans="1:8">
+    <row r="19" ht="151.8" spans="1:8">
       <c r="A19" s="10">
         <v>33</v>
       </c>
@@ -2602,7 +2657,7 @@
       <c r="G23" s="5"/>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" ht="99.75" spans="1:8">
+    <row r="24" ht="96.6" spans="1:8">
       <c r="A24" s="4">
         <v>121</v>
       </c>
@@ -2628,7 +2683,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" ht="114" spans="1:8">
+    <row r="25" ht="124.2" spans="1:8">
       <c r="A25" s="9">
         <v>208</v>
       </c>
@@ -2652,7 +2707,7 @@
       </c>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" ht="142.5" spans="1:8">
+    <row r="26" ht="138" spans="1:8">
       <c r="A26" s="11">
         <v>238</v>
       </c>
@@ -2678,7 +2733,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" ht="142.5" spans="1:8">
+    <row r="27" ht="151.8" spans="1:8">
       <c r="A27" s="11">
         <v>53</v>
       </c>
@@ -2704,7 +2759,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" ht="114" spans="1:8">
+    <row r="28" ht="110.4" spans="1:8">
       <c r="A28" s="4">
         <v>217</v>
       </c>
@@ -2730,7 +2785,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" ht="142.5" spans="1:8">
+    <row r="29" ht="138" spans="1:8">
       <c r="A29" s="9">
         <v>56</v>
       </c>
@@ -2754,7 +2809,7 @@
       </c>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" ht="156.75" spans="1:8">
+    <row r="30" ht="151.8" spans="1:8">
       <c r="A30" s="11">
         <v>152</v>
       </c>
@@ -2778,7 +2833,7 @@
       </c>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" ht="199.5" spans="1:8">
+    <row r="31" ht="208.8" spans="1:8">
       <c r="A31" s="11">
         <v>15</v>
       </c>
@@ -2804,7 +2859,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="32" ht="228" spans="1:8">
+    <row r="32" ht="220.8" spans="1:8">
       <c r="A32" s="11">
         <v>57</v>
       </c>
@@ -2827,6 +2882,30 @@
         <v>118</v>
       </c>
       <c r="H32" s="6"/>
+    </row>
+    <row r="33" ht="189" customHeight="1" spans="1:8">
+      <c r="A33" s="13">
+        <v>70</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="H33" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2850,7 +2929,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2867,7 +2946,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
[LC] Update 4 reviews for array and string. Update 322 coin change.
</commit_message>
<xml_diff>
--- a/Leetcode/Problem-tracker.xlsx
+++ b/Leetcode/Problem-tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9767"/>
+    <workbookView windowWidth="22176" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="147">
   <si>
     <t>Prompt</t>
   </si>
@@ -715,12 +715,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <charset val="134"/>
-      </rPr>
       <t>Problem Pattern: This problem follows the "</t>
     </r>
     <r>
@@ -742,7 +736,17 @@
       </rPr>
       <t xml:space="preserve"> Intervals" pattern. The key is to sort intervals by start time and then merge overlapping intervals greedily.
 Solution Approach: Sort the intervals by their start time, then iterate through the sorted list, merging overlapping intervals by updating the end time of the last merged interval. This runs in O(n log n) time due to sorting and O(n) space for the output list.
-Solved in 18' first time</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Solved in 18' first time</t>
     </r>
   </si>
   <si>
@@ -1182,6 +1186,381 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/climbing-stairs/description/</t>
+  </si>
+  <si>
+    <t>Coin Change</t>
+  </si>
+  <si>
+    <t>2025.2.16</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: This problem follows the "Dynamic Programming - Unbounded Knapsack" pattern. The key is to find the minimum number of coins that sum up to a given amount using optimal substructure and overlapping subproblems.
+Solution Approach: Use bottom-up dynamic programming to compute the minimum coins required for each amount up to amount. Initialize dp[i] as inf and iteratively update it using dp[i] = min(dp[i], dp[i - coin] + 1). This runs in O(n * m) time, where n is the amount and m is the number of coin denominations.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Not solved first time, draw a decision tree then bottom-up helps a lot</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When solving problems that involve finding the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>minimum or maximum combination</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> of elements that sum to a target.
+2. When working with unbounded knapsack problems (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>each item can be used unlimited times</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>).
+3. When solving problems that require minimizing steps to reach a target (e.g., shortest path, minimum transformations).</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/coin-change/description/</t>
+  </si>
+  <si>
+    <t>Container With Most Water</t>
+  </si>
+  <si>
+    <t>Array; Two pointer</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: This problem follows the "Two Pointers with Greedy Optimization" pattern. The key insight is that maximizing the width while adjusting the height efficiently is the best approach.
+Solution Approach: Use two pointers (left and right) to find the container with the maximum water area. Move the pointer with the shorter height since it is the limiting factor in increasing the area. This runs in O(n) time complexity and O(1) space.
+        # Brute Force, try every container we could make. Nested for loop -&gt; O(N^2)
+        # Linear run time.
+        # Init two pointers all the way left/right because we wanna maximize the area and the width to be as big as possible. If left//right height is super tall, we ll instantly find the result
+        # Then update the shorter pointer to find higher height that may result in bigger area.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Not Solved second</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1. When solving problems that require maximizing/minimizing values</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> with two constraints </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">(e.g., width &amp; height).
+2. When a brute-force O(n²) approach is too slow, and an optimal greedy method exists.
+3. When dealing with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>left-right boundary</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> conditions that need </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>iterative narrowing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/container-with-most-water/description/</t>
+  </si>
+  <si>
+    <t>2025.2.16; 2024.11.10</t>
+  </si>
+  <si>
+    <t>Sliding Window Maximum</t>
+  </si>
+  <si>
+    <t>Queue; Sliding window</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: This problem follows the "Sliding Window with Monotonic Queue" pattern. The key is to efficiently maintain the maximum value within a moving window without recalculating from scratch.
+Solution Approach: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Use a deque (double-ended queue)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> to store indices of useful elements in a monotonic decreasing order. As the window moves, remove out-of-bound elements and keep track of the maximum efficiently. This runs in O(n) time complexity with O(k) space.        
+# Brute Force solution cost O(k(n-k))
+        # In every window, we do repeated comparison
+        # The value that is greater than values that are previously in our window, then we 
+        # can eliminate those values
+        # Compare the current visiting value with the newly added value, if added one is 
+        # smaller, pop right
+        # We wanna remove and add in both end in O(1) so we use deque
+        # Check if the front value is out of window, if so, popleft
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Not Solved second time</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When solving problems that involve tracking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>max/min values</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>in a dynamic range</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>.
+2. When a brute-force O(n*k) solution is too slow, and an O(n) approach is required.
+3. When a monotonic queue or deque can optimize range-based calculations (e.g., temperature, stock prices).</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sliding-window-maximum/description/</t>
+  </si>
+  <si>
+    <t>2025.2.16; 2024.11.11</t>
+  </si>
+  <si>
+    <t>Valid Anagram</t>
+  </si>
+  <si>
+    <t>Hashmap; String</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: This problem follows the "Character Frequency Counting" pattern. The key is to determine if two strings contain the same characters in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>same frequency</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">, regardless of order.
+Solution Approach: Use a hash map (dictionary) to count character occurrences in both strings and compare them. Alternatively, sorting both strings and checking equality also works but has a higher time complexity. The optimal solution runs in O(n) time using a hash map.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Solved in 2'40 second time. Alternatively</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+1.  return sorted(s) == sorted(t)
+2. return Counter(s) == Counter(t)
+3. Check values in dict
+# Check if any character has non-zero frequency
+        for val in count.values():
+            if val != 0:
+                return False</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When checking if two strings have the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>same characters in any order.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+2. When character </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>frequency counting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> is needed for comparison-based problems.
+3. When optimizing problems involving unordered string comparison.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-anagram/description/</t>
   </si>
 </sst>
 </file>
@@ -1360,16 +1739,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -1844,7 +2223,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1892,6 +2271,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2204,10 +2586,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="7"/>
@@ -2215,15 +2597,15 @@
     <col min="1" max="1" width="6.75" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.6296296296296" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.25" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.6296296296296" style="2" customWidth="1"/>
-    <col min="5" max="5" width="46.25" style="2" customWidth="1"/>
-    <col min="6" max="6" width="62.6296296296296" style="3" customWidth="1"/>
-    <col min="7" max="7" width="25.25" style="3" customWidth="1"/>
-    <col min="8" max="8" width="44.25" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.3611111111111" style="3" customWidth="1"/>
+    <col min="5" max="5" width="94.8981481481482" style="2" customWidth="1"/>
+    <col min="6" max="6" width="43.2592592592593" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18.2962962962963" style="3" customWidth="1"/>
+    <col min="8" max="8" width="32.6666666666667" style="2" customWidth="1"/>
     <col min="9" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="165" customHeight="1" spans="1:8">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2247,7 +2629,7 @@
       <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="7" t="s">
@@ -2263,7 +2645,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" ht="82.8" spans="1:8">
+    <row r="3" ht="96.6" spans="1:8">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -2273,7 +2655,7 @@
       <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="5" t="s">
@@ -2299,7 +2681,7 @@
       <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="6"/>
@@ -2317,7 +2699,7 @@
       <c r="C5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="6"/>
@@ -2335,7 +2717,7 @@
       <c r="C6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="6"/>
@@ -2353,7 +2735,7 @@
       <c r="C7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="6"/>
@@ -2371,7 +2753,7 @@
       <c r="C8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="6"/>
@@ -2389,7 +2771,7 @@
       <c r="C9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E9" s="6"/>
@@ -2407,7 +2789,7 @@
       <c r="C10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="6"/>
@@ -2425,7 +2807,7 @@
       <c r="C11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E11" s="6"/>
@@ -2443,7 +2825,7 @@
       <c r="C12" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>37</v>
       </c>
       <c r="E12" s="6"/>
@@ -2461,7 +2843,7 @@
       <c r="C13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>37</v>
       </c>
       <c r="E13" s="6"/>
@@ -2479,7 +2861,7 @@
       <c r="C14" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E14" s="6"/>
@@ -2497,7 +2879,7 @@
       <c r="C15" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E15" s="6"/>
@@ -2515,7 +2897,7 @@
       <c r="C16" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E16" s="6"/>
@@ -2533,7 +2915,7 @@
       <c r="C17" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E17" s="6"/>
@@ -2551,7 +2933,7 @@
       <c r="C18" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E18" s="6"/>
@@ -2559,7 +2941,7 @@
       <c r="G18" s="5"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" ht="151.8" spans="1:8">
+    <row r="19" ht="82.8" spans="1:8">
       <c r="A19" s="10">
         <v>33</v>
       </c>
@@ -2569,7 +2951,7 @@
       <c r="C19" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>55</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -2585,7 +2967,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" ht="27.6" spans="1:8">
       <c r="A20" s="9">
         <v>704</v>
       </c>
@@ -2595,7 +2977,7 @@
       <c r="C20" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>62</v>
       </c>
       <c r="E20" s="6"/>
@@ -2613,7 +2995,7 @@
       <c r="C21" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>65</v>
       </c>
       <c r="E21" s="6"/>
@@ -2631,7 +3013,7 @@
       <c r="C22" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>65</v>
       </c>
       <c r="E22" s="6"/>
@@ -2649,7 +3031,7 @@
       <c r="C23" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="5" t="s">
         <v>65</v>
       </c>
       <c r="E23" s="6"/>
@@ -2657,7 +3039,7 @@
       <c r="G23" s="5"/>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" ht="96.6" spans="1:8">
+    <row r="24" ht="138" spans="1:8">
       <c r="A24" s="4">
         <v>121</v>
       </c>
@@ -2667,7 +3049,7 @@
       <c r="C24" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="5" t="s">
         <v>71</v>
       </c>
       <c r="E24" s="5" t="s">
@@ -2683,7 +3065,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" ht="124.2" spans="1:8">
+    <row r="25" ht="96.6" spans="1:8">
       <c r="A25" s="9">
         <v>208</v>
       </c>
@@ -2693,7 +3075,7 @@
       <c r="C25" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="5" t="s">
         <v>77</v>
       </c>
       <c r="E25" s="5" t="s">
@@ -2707,7 +3089,7 @@
       </c>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" ht="138" spans="1:8">
+    <row r="26" ht="124.2" spans="1:8">
       <c r="A26" s="11">
         <v>238</v>
       </c>
@@ -2717,7 +3099,7 @@
       <c r="C26" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="5" t="s">
         <v>82</v>
       </c>
       <c r="E26" s="5" t="s">
@@ -2733,7 +3115,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" ht="151.8" spans="1:8">
+    <row r="27" ht="96.6" spans="1:8">
       <c r="A27" s="11">
         <v>53</v>
       </c>
@@ -2743,7 +3125,7 @@
       <c r="C27" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="5" t="s">
         <v>71</v>
       </c>
       <c r="E27" s="5" t="s">
@@ -2759,7 +3141,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" ht="110.4" spans="1:8">
+    <row r="28" ht="82.8" spans="1:8">
       <c r="A28" s="4">
         <v>217</v>
       </c>
@@ -2769,7 +3151,7 @@
       <c r="C28" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="5" t="s">
         <v>93</v>
       </c>
       <c r="E28" s="5" t="s">
@@ -2785,7 +3167,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" ht="138" spans="1:8">
+    <row r="29" ht="82.8" spans="1:8">
       <c r="A29" s="9">
         <v>56</v>
       </c>
@@ -2795,7 +3177,7 @@
       <c r="C29" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="5" t="s">
         <v>99</v>
       </c>
       <c r="E29" s="5" t="s">
@@ -2809,7 +3191,7 @@
       </c>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" ht="151.8" spans="1:8">
+    <row r="30" ht="110.4" spans="1:8">
       <c r="A30" s="11">
         <v>152</v>
       </c>
@@ -2819,7 +3201,7 @@
       <c r="C30" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="5" t="s">
         <v>71</v>
       </c>
       <c r="E30" s="5" t="s">
@@ -2833,7 +3215,7 @@
       </c>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" ht="208.8" spans="1:8">
+    <row r="31" ht="153.6" spans="1:8">
       <c r="A31" s="11">
         <v>15</v>
       </c>
@@ -2843,7 +3225,7 @@
       <c r="C31" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="5" t="s">
         <v>108</v>
       </c>
       <c r="E31" s="5" t="s">
@@ -2859,7 +3241,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="32" ht="220.8" spans="1:8">
+    <row r="32" ht="124.2" spans="1:8">
       <c r="A32" s="11">
         <v>57</v>
       </c>
@@ -2869,7 +3251,7 @@
       <c r="C32" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="5" t="s">
         <v>115</v>
       </c>
       <c r="E32" s="5" t="s">
@@ -2883,29 +3265,131 @@
       </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" ht="189" customHeight="1" spans="1:8">
-      <c r="A33" s="13">
+    <row r="33" ht="96.6" spans="1:8">
+      <c r="A33" s="11">
         <v>70</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="F33" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="G33" s="15" t="s">
+      <c r="G33" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="H33" s="14"/>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" ht="124.2" spans="1:8">
+      <c r="A34" s="13">
+        <v>322</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="H34" s="14"/>
+    </row>
+    <row r="35" ht="151.8" spans="1:8">
+      <c r="A35" s="13">
+        <v>11</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="G35" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="H35" s="14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" ht="193.2" spans="1:8">
+      <c r="A36" s="13">
+        <v>239</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="G36" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" ht="179.4" spans="1:8">
+      <c r="A37" s="16">
+        <v>242</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="H37" s="14" t="s">
+        <v>141</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
[LC] Update 198 House Robber.
</commit_message>
<xml_diff>
--- a/Leetcode/Problem-tracker.xlsx
+++ b/Leetcode/Problem-tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22176" windowHeight="9780"/>
+    <workbookView windowWidth="27945" windowHeight="12960"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="152">
   <si>
     <t>Prompt</t>
   </si>
@@ -715,6 +715,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t>Problem Pattern: This problem follows the "</t>
     </r>
     <r>
@@ -1164,6 +1170,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Dynamic Programming - Fibonacci Sequence" pattern. The key is recognizing that the number of ways to reach step n is the sum of ways to reach n-1 and n-2 because you can climb 1 or 2 steps at a time.
 Solution Approach: Use a bottom-up dynamic programming (DP) approach to compute the number of ways iteratively. The optimized solution runs in O(n) time with O(1) space by storing only the last two computed values.
 </t>
@@ -1195,6 +1207,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Dynamic Programming - Unbounded Knapsack" pattern. The key is to find the minimum number of coins that sum up to a given amount using optimal substructure and overlapping subproblems.
 Solution Approach: Use bottom-up dynamic programming to compute the minimum coins required for each amount up to amount. Initialize dp[i] as inf and iteratively update it using dp[i] = min(dp[i], dp[i - coin] + 1). This runs in O(n * m) time, where n is the amount and m is the number of coin denominations.
 </t>
@@ -1212,6 +1230,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When solving problems that involve finding the </t>
     </r>
     <r>
@@ -1266,6 +1290,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Two Pointers with Greedy Optimization" pattern. The key insight is that maximizing the width while adjusting the height efficiently is the best approach.
 Solution Approach: Use two pointers (left and right) to find the container with the maximum water area. Move the pointer with the shorter height since it is the limiting factor in increasing the area. This runs in O(n) time complexity and O(1) space.
         # Brute Force, try every container we could make. Nested for loop -&gt; O(N^2)
@@ -1287,6 +1317,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t>1. When solving problems that require maximizing/minimizing values</t>
     </r>
     <r>
@@ -1363,6 +1399,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Sliding Window with Monotonic Queue" pattern. The key is to efficiently maintain the maximum value within a moving window without recalculating from scratch.
 Solution Approach: </t>
     </r>
@@ -1407,6 +1449,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When solving problems that involve tracking </t>
     </r>
     <r>
@@ -1464,6 +1512,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Character Frequency Counting" pattern. The key is to determine if two strings contain the same characters in the </t>
     </r>
     <r>
@@ -1516,6 +1570,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When checking if two strings have the </t>
     </r>
     <r>
@@ -1561,6 +1621,82 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/valid-anagram/description/</t>
+  </si>
+  <si>
+    <t>House Robber</t>
+  </si>
+  <si>
+    <t>2025.2.17</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: This problem follows the "Dynamic Programming - Maximum Sum with Non-Adjacent Constraint" pattern. The key idea is to decide at each house whether to rob it (skip the previous one) or skip it (take the previous max sum).
+Solution Approach: Use bottom-up dynamic programming where dp[i] stores the maximum amount that can be robbed from the first i houses. Update dp[i] = max(dp[i-1], nums[i] + dp[i-2]). This runs in O(n) time with O(1) space using two variables.
+You have two choices at every house i:
+* Skip this house → Keep the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>max sum from i-1 (prev1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">. or I would say, dp[i-1]
+* Rob this house → Take nums[i] and add it to dp[i-2] (prev2).
+Transition Formula (DP Recurrence Relation):
+dp[i]=max(dp[i−1],nums[i]+dp[i−2])
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Solved first time in 20'37'', but not that efficient. Revised one is sufficient, same idea with official solution using prev1, prev2.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When solving problems where selecting an element </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>prevents selecting adjacent ones</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>.
+2. When optimizing maximum sum problems with sequence constraints.
+3. When transitioning from a brute-force approach to a dynamic programming solution.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/house-robber/description/</t>
   </si>
 </sst>
 </file>
@@ -2223,7 +2359,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2263,7 +2399,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2271,9 +2407,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2586,21 +2719,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="6.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6296296296296" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.6333333333333" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.25" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.3611111111111" style="3" customWidth="1"/>
-    <col min="5" max="5" width="94.8981481481482" style="2" customWidth="1"/>
-    <col min="6" max="6" width="43.2592592592593" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.2962962962963" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.3583333333333" style="3" customWidth="1"/>
+    <col min="5" max="5" width="94.9" style="2" customWidth="1"/>
+    <col min="6" max="6" width="43.2583333333333" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18.3" style="3" customWidth="1"/>
     <col min="8" max="8" width="32.6666666666667" style="2" customWidth="1"/>
     <col min="9" max="16384" width="9" style="2"/>
   </cols>
@@ -2645,7 +2778,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" ht="96.6" spans="1:8">
+    <row r="3" ht="85.5" spans="1:8">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -2941,7 +3074,7 @@
       <c r="G18" s="5"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" ht="82.8" spans="1:8">
+    <row r="19" ht="85.5" spans="1:8">
       <c r="A19" s="10">
         <v>33</v>
       </c>
@@ -2967,7 +3100,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" ht="27.6" spans="1:8">
+    <row r="20" spans="1:8">
       <c r="A20" s="9">
         <v>704</v>
       </c>
@@ -3039,7 +3172,7 @@
       <c r="G23" s="5"/>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" ht="138" spans="1:8">
+    <row r="24" ht="99.75" spans="1:8">
       <c r="A24" s="4">
         <v>121</v>
       </c>
@@ -3065,7 +3198,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" ht="96.6" spans="1:8">
+    <row r="25" ht="85.5" spans="1:8">
       <c r="A25" s="9">
         <v>208</v>
       </c>
@@ -3089,7 +3222,7 @@
       </c>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" ht="124.2" spans="1:8">
+    <row r="26" ht="114" spans="1:8">
       <c r="A26" s="11">
         <v>238</v>
       </c>
@@ -3115,7 +3248,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" ht="96.6" spans="1:8">
+    <row r="27" ht="99.75" spans="1:8">
       <c r="A27" s="11">
         <v>53</v>
       </c>
@@ -3141,7 +3274,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" ht="82.8" spans="1:8">
+    <row r="28" ht="85.5" spans="1:8">
       <c r="A28" s="4">
         <v>217</v>
       </c>
@@ -3167,7 +3300,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" ht="82.8" spans="1:8">
+    <row r="29" ht="85.5" spans="1:8">
       <c r="A29" s="9">
         <v>56</v>
       </c>
@@ -3191,7 +3324,7 @@
       </c>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" ht="110.4" spans="1:8">
+    <row r="30" ht="85.5" spans="1:8">
       <c r="A30" s="11">
         <v>152</v>
       </c>
@@ -3215,7 +3348,7 @@
       </c>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" ht="153.6" spans="1:8">
+    <row r="31" ht="142.5" spans="1:8">
       <c r="A31" s="11">
         <v>15</v>
       </c>
@@ -3241,7 +3374,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="32" ht="124.2" spans="1:8">
+    <row r="32" ht="128.25" spans="1:8">
       <c r="A32" s="11">
         <v>57</v>
       </c>
@@ -3265,7 +3398,7 @@
       </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" ht="96.6" spans="1:8">
+    <row r="33" ht="85.5" spans="1:8">
       <c r="A33" s="11">
         <v>70</v>
       </c>
@@ -3289,106 +3422,132 @@
       </c>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" ht="124.2" spans="1:8">
-      <c r="A34" s="13">
+    <row r="34" ht="114" spans="1:8">
+      <c r="A34" s="11">
         <v>322</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="F34" s="15" t="s">
+      <c r="F34" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="G34" s="15" t="s">
+      <c r="G34" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="H34" s="14"/>
-    </row>
-    <row r="35" ht="151.8" spans="1:8">
-      <c r="A35" s="13">
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" ht="156.75" spans="1:8">
+      <c r="A35" s="11">
         <v>11</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="F35" s="15" t="s">
+      <c r="F35" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="G35" s="15" t="s">
+      <c r="G35" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="H35" s="14" t="s">
+      <c r="H35" s="6" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="36" ht="193.2" spans="1:8">
-      <c r="A36" s="13">
+    <row r="36" ht="199.5" spans="1:8">
+      <c r="A36" s="11">
         <v>239</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="E36" s="15" t="s">
+      <c r="E36" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F36" s="15" t="s">
+      <c r="F36" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G36" s="15" t="s">
+      <c r="G36" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="H36" s="14" t="s">
+      <c r="H36" s="6" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="37" ht="179.4" spans="1:8">
-      <c r="A37" s="16">
+    <row r="37" ht="185.25" spans="1:8">
+      <c r="A37" s="4">
         <v>242</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E37" s="15" t="s">
+      <c r="E37" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="F37" s="15" t="s">
+      <c r="F37" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="G37" s="15" t="s">
+      <c r="G37" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="H37" s="14" t="s">
+      <c r="H37" s="6" t="s">
         <v>141</v>
+      </c>
+    </row>
+    <row r="38" ht="199.5" spans="1:8">
+      <c r="A38" s="13">
+        <v>198</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="H38" s="14" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -3413,7 +3572,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -3430,7 +3589,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
[LC] Update 300 Longest Increasing Sequence.
</commit_message>
<xml_diff>
--- a/Leetcode/Problem-tracker.xlsx
+++ b/Leetcode/Problem-tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12960"/>
+    <workbookView windowWidth="22176" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="158">
   <si>
     <t>Prompt</t>
   </si>
@@ -1630,6 +1630,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Dynamic Programming - Maximum Sum with Non-Adjacent Constraint" pattern. The key idea is to decide at each house whether to rob it (skip the previous one) or skip it (take the previous max sum).
 Solution Approach: Use bottom-up dynamic programming where dp[i] stores the maximum amount that can be robbed from the first i houses. Update dp[i] = max(dp[i-1], nums[i] + dp[i-2]). This runs in O(n) time with O(1) space using two variables.
 You have two choices at every house i:
@@ -1671,6 +1677,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When solving problems where selecting an element </t>
     </r>
     <r>
@@ -1697,6 +1709,100 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/house-robber/description/</t>
+  </si>
+  <si>
+    <t>Longest Increasing Subsequence</t>
+  </si>
+  <si>
+    <t>2025.2.18</t>
+  </si>
+  <si>
+    <t>DP; Subsequence</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: This problem follows the "Dynamic Programming - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Subsequence Optimization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">" pattern. The key is to find the longest increasing subsequence (LIS) in an unsorted array.
+Solution Approach: Use DP (O(n²)) or Binary Search (O(n log n)) to compute the LIS efficiently. The DP approach iterates through each element and checks for smaller elements before it, while the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>optimized binary search approach</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> uses a greedy strategy with a tail array to maintain the smallest possible increasing subsequence.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Not Solved first time. The DP idea is correct, but need sort of changes with the decision condition.
+Binary search idea is better on time complexity. try to implement next time</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When solving problems that involve </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>selecting a subsequence</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> while maintaining order.
+2. When a brute-force O(2ⁿ) approach is infeasible, and DP or Binary Search is needed.
+3. When optimizing sequence-based problems that require global order tracking.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-increasing-subsequence/description/</t>
   </si>
 </sst>
 </file>
@@ -1875,16 +1981,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -2399,7 +2505,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2719,21 +2825,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="6.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6333333333333" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.6296296296296" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.25" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.3583333333333" style="3" customWidth="1"/>
-    <col min="5" max="5" width="94.9" style="2" customWidth="1"/>
-    <col min="6" max="6" width="43.2583333333333" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.3" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.3611111111111" style="3" customWidth="1"/>
+    <col min="5" max="5" width="94.8981481481482" style="2" customWidth="1"/>
+    <col min="6" max="6" width="43.2592592592593" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18.2962962962963" style="3" customWidth="1"/>
     <col min="8" max="8" width="32.6666666666667" style="2" customWidth="1"/>
     <col min="9" max="16384" width="9" style="2"/>
   </cols>
@@ -2778,7 +2884,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" ht="85.5" spans="1:8">
+    <row r="3" ht="96.6" spans="1:8">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -3074,7 +3180,7 @@
       <c r="G18" s="5"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" ht="85.5" spans="1:8">
+    <row r="19" ht="82.8" spans="1:8">
       <c r="A19" s="10">
         <v>33</v>
       </c>
@@ -3100,7 +3206,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" ht="27.6" spans="1:8">
       <c r="A20" s="9">
         <v>704</v>
       </c>
@@ -3172,7 +3278,7 @@
       <c r="G23" s="5"/>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" ht="99.75" spans="1:8">
+    <row r="24" ht="138" spans="1:8">
       <c r="A24" s="4">
         <v>121</v>
       </c>
@@ -3198,7 +3304,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" ht="85.5" spans="1:8">
+    <row r="25" ht="96.6" spans="1:8">
       <c r="A25" s="9">
         <v>208</v>
       </c>
@@ -3222,7 +3328,7 @@
       </c>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" ht="114" spans="1:8">
+    <row r="26" ht="124.2" spans="1:8">
       <c r="A26" s="11">
         <v>238</v>
       </c>
@@ -3248,7 +3354,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" ht="99.75" spans="1:8">
+    <row r="27" ht="96.6" spans="1:8">
       <c r="A27" s="11">
         <v>53</v>
       </c>
@@ -3274,7 +3380,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" ht="85.5" spans="1:8">
+    <row r="28" ht="82.8" spans="1:8">
       <c r="A28" s="4">
         <v>217</v>
       </c>
@@ -3300,7 +3406,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" ht="85.5" spans="1:8">
+    <row r="29" ht="82.8" spans="1:8">
       <c r="A29" s="9">
         <v>56</v>
       </c>
@@ -3324,7 +3430,7 @@
       </c>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" ht="85.5" spans="1:8">
+    <row r="30" ht="110.4" spans="1:8">
       <c r="A30" s="11">
         <v>152</v>
       </c>
@@ -3348,7 +3454,7 @@
       </c>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" ht="142.5" spans="1:8">
+    <row r="31" ht="153.6" spans="1:8">
       <c r="A31" s="11">
         <v>15</v>
       </c>
@@ -3374,7 +3480,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="32" ht="128.25" spans="1:8">
+    <row r="32" ht="124.2" spans="1:8">
       <c r="A32" s="11">
         <v>57</v>
       </c>
@@ -3398,7 +3504,7 @@
       </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" ht="85.5" spans="1:8">
+    <row r="33" ht="96.6" spans="1:8">
       <c r="A33" s="11">
         <v>70</v>
       </c>
@@ -3422,7 +3528,7 @@
       </c>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" ht="114" spans="1:8">
+    <row r="34" ht="124.2" spans="1:8">
       <c r="A34" s="11">
         <v>322</v>
       </c>
@@ -3446,7 +3552,7 @@
       </c>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" ht="156.75" spans="1:8">
+    <row r="35" ht="151.8" spans="1:8">
       <c r="A35" s="11">
         <v>11</v>
       </c>
@@ -3472,7 +3578,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="36" ht="199.5" spans="1:8">
+    <row r="36" ht="193.2" spans="1:8">
       <c r="A36" s="11">
         <v>239</v>
       </c>
@@ -3498,7 +3604,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="37" ht="185.25" spans="1:8">
+    <row r="37" ht="179.4" spans="1:8">
       <c r="A37" s="4">
         <v>242</v>
       </c>
@@ -3524,31 +3630,55 @@
         <v>141</v>
       </c>
     </row>
-    <row r="38" ht="199.5" spans="1:8">
-      <c r="A38" s="13">
+    <row r="38" ht="193.2" spans="1:8">
+      <c r="A38" s="9">
         <v>198</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="E38" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="F38" s="15" t="s">
+      <c r="F38" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="G38" s="15" t="s">
+      <c r="G38" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="H38" s="14" t="s">
+      <c r="H38" s="6" t="s">
         <v>148</v>
       </c>
+    </row>
+    <row r="39" ht="110.4" spans="1:8">
+      <c r="A39" s="13">
+        <v>300</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="H39" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3572,7 +3702,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -3589,7 +3719,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
[LC] Update 371. Sum of Two Integers.
</commit_message>
<xml_diff>
--- a/Leetcode/Problem-tracker.xlsx
+++ b/Leetcode/Problem-tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22176" windowHeight="9780"/>
+    <workbookView windowWidth="22188" windowHeight="9767"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="164">
   <si>
     <t>Prompt</t>
   </si>
@@ -1721,6 +1721,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Dynamic Programming - </t>
     </r>
     <r>
@@ -1777,6 +1783,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When solving problems that involve </t>
     </r>
     <r>
@@ -1803,6 +1815,41 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/longest-increasing-subsequence/description/</t>
+  </si>
+  <si>
+    <t>Sum of Two Integers</t>
+  </si>
+  <si>
+    <t>2025.2.19</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: This problem follows the "Bitwise Manipulation for Arithmetic Operations" pattern. The key is to compute the sum of two integers without using + or - by using bitwise operations (XOR and AND with carry).
+Solution Approach: Use a loop-based bitwise addition method where: (1) XOR computes sum without carry, (2) AND + left shift computes the carry, and (3) repeat until carry becomes 0. This runs in O(1) time complexity (bounded by integer size).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Carry value identification: a &amp; b &lt;&lt; 1
+Not solved for first time</t>
+    </r>
+  </si>
+  <si>
+    <t>1. When simulating basic arithmetic using bitwise operations in low-level programming.
+2. When working with systems where + or - operations are restricted (e.g., hardware-level addition).
+3. When optimizing addition for unsigned/signed integers using bitwise tricks.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sum-of-two-integers/description/</t>
   </si>
 </sst>
 </file>
@@ -1981,16 +2028,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -2825,10 +2872,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="7"/>
@@ -3657,28 +3704,52 @@
       </c>
     </row>
     <row r="39" ht="110.4" spans="1:8">
-      <c r="A39" s="13">
+      <c r="A39" s="11">
         <v>300</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="D39" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E39" s="15" t="s">
+      <c r="E39" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="F39" s="15" t="s">
+      <c r="F39" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="G39" s="15" t="s">
+      <c r="G39" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="H39" s="14"/>
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" ht="131" customHeight="1" spans="1:8">
+      <c r="A40" s="13">
+        <v>371</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="H40" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
[LC] Update 191 number of bits and two string question reviews.
</commit_message>
<xml_diff>
--- a/Leetcode/Problem-tracker.xlsx
+++ b/Leetcode/Problem-tracker.xlsx
@@ -29,19 +29,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="181">
   <si>
     <t>Prompt</t>
   </si>
   <si>
-    <t>Problem Name: "Two sums" (LeetCode 1)
+    <t>Problem Name: "Leetcode {problem_number}. {problem_title}"
 Instructions:
-1. Provide the **problem pattern** and **solution approach**.
-2. Explain the **algorithm used** 
-3. List **when to use this pattern** and how it scales to similar problems.
-4. Format the output as:
-    - **Problem Pattern/Solution:** Describe the pattern &amp; solution strategy.
-    - **When to Use/Scale:** Provide 2-3 bullet points on when to apply this approach.</t>
+Provide the problem pattern and solution approach.
+Explain the algorithm used, including time and space complexity.
+List when to use this pattern and how it scales to similar problems.
+Format the output exactly as follows:
+### **LeetCode {problem_number}: {problem_title}**  
+| No. | Name | Last Viewed | Tag | Problem Pattern/Solution | When to Use/Scale |
+|----|------|------------|-----|--------------------------|--------------------|
+| {problem_number} | {problem_title} | {date} | {tags} | **Problem Pattern:** {Describe the problem pattern and general solution strategy.} &lt;br&gt; **Solution Approach:** {Explain the key idea behind the solution, including how it optimizes the problem.} | 1. {When to use this pattern, bullet point 1} &lt;br&gt; 2. {When to use this pattern, bullet point 2} &lt;br&gt; 3. {When to use this pattern, bullet point 3} |
+---
+## **🔹 Algorithm Used**
+- **{Algorithm Name} (`{Time Complexity}`)**
+  1. {Step 1 explanation}
+  2. {Step 2 explanation}
+  3. {Step 3 explanation}
+- **Time Complexity:** `{O(complexity)}`, explanation.  
+- **Space Complexity:** `{O(complexity)}`, explanation.  
+---
+## **🔹 Python Code**
+```python
+{Optimized Python code solution}
+Provide a structured solution for LeetCode 191: Number of 1 Bits, using the exact format specified above</t>
   </si>
   <si>
     <t>No.</t>
@@ -1827,6 +1842,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Bitwise Manipulation for Arithmetic Operations" pattern. The key is to compute the sum of two integers without using + or - by using bitwise operations (XOR and AND with carry).
 Solution Approach: Use a loop-based bitwise addition method where: (1) XOR computes sum without carry, (2) AND + left shift computes the carry, and (3) repeat until carry becomes 0. This runs in O(1) time complexity (bounded by integer size).
 </t>
@@ -1850,6 +1871,251 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/sum-of-two-integers/description/</t>
+  </si>
+  <si>
+    <t>Number of 1 Bits</t>
+  </si>
+  <si>
+    <t>2025.2.20</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: This problem follows the "Bitwise Counting" pattern. The key is to count how many 1s are present in the binary representation of an unsigned integer.
+Solution Approach: Use bitwise operations to efficiently count 1 bits. The optimal approach is Brian Kernighan’s Algorithm, which clears the least significant 1 in each iteration, reducing time complexity to O(k), where k is the number of 1 bits.
+Two solutions:
+1. n &amp; (n-1) is used to remove the right most 1
+2. check rightmost bit and then shift right
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Not solved first time</t>
+    </r>
+  </si>
+  <si>
+    <t>1. When counting set bits in an integer for bitwise optimizations.
+2. When working with binary representations and optimizing bitwise operations.
+3. When designing efficient bitwise operations for cryptography, hashing, and compression.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-of-1-bits/description/</t>
+  </si>
+  <si>
+    <t>Valid Palindrome</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: This problem follows the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Two Pointers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> pattern, where we use two indices to traverse the string from both ends to check for palindrome properties while ignoring non-alphanumeric characters.
+Solution Approach: Use two pointers, one starting from the left and one from the right, moving towards the center while skipping non-alphanumeric characters. If at any point the characters don’t match, return False. Otherwise, return True.
+Trick:
+1. string.isnumeric() to check if it's a digit
+2. string.isalpha() to check if it's a letter
+3. string.isalnum() to check if it's a digit or a letter.
+4. string.lower() to convert a letter to lowercase
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Solved second time in 4'45'', but not space efficient. It can be done in-place. But for the in-place solution, isalnum() and lower() are called multiple times inside the loop which can be slower than the array based solution</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When checking if a given string is a valid </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>palindrome</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> after preprocessing.
+2. When working with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>alphanumeric filtering</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> and case-insensitive comparisons.
+3. When solving problems requiring efficient in-place string manipulations.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-palindrome/description/</t>
+  </si>
+  <si>
+    <t>2025.2.20; 2025.11.13</t>
+  </si>
+  <si>
+    <t>Longest Substring Without Repeating Characters</t>
+  </si>
+  <si>
+    <t>String; Set</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: The problem follows the Sliding Window pattern where we </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>dynamically expand and shrink a window</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> to track unique characters efficiently.
+Solution Approach: Use a hash set (or dictionary) to track characters in the current substring. Expand the right pointer, and if a duplicate is found, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>shrink the left pointer until</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> the substring is unique again. Maintain the maximum length.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+Set is used for checking duplicates instantly
+Not solved second time</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When dealing with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>substring</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> problems requiring </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>unique</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> elements.
+2. When optimizing a brute-force approach (O(n^2)) to O(n).
+3. When implementing real-time processing for text parsing and tokenization.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-substring-without-repeating-characters/description/</t>
+  </si>
+  <si>
+    <t>2025.2.20; 2025.11.17</t>
   </si>
 </sst>
 </file>
@@ -2512,7 +2778,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2520,10 +2786,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2550,16 +2816,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2872,26 +3141,26 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="6.75" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.6296296296296" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.3611111111111" style="3" customWidth="1"/>
-    <col min="5" max="5" width="94.8981481481482" style="2" customWidth="1"/>
-    <col min="6" max="6" width="43.2592592592593" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.2962962962963" style="3" customWidth="1"/>
-    <col min="8" max="8" width="32.6666666666667" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="2"/>
+    <col min="3" max="3" width="12.25" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.3611111111111" style="2" customWidth="1"/>
+    <col min="5" max="5" width="94.8981481481482" style="3" customWidth="1"/>
+    <col min="6" max="6" width="43.2592592592593" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.2962962962963" style="2" customWidth="1"/>
+    <col min="8" max="8" width="32.6666666666667" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" ht="405" customHeight="1" spans="1:8">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2909,7 +3178,7 @@
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -2935,7 +3204,7 @@
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -2961,7 +3230,7 @@
       <c r="A4" s="9">
         <v>973</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -2979,7 +3248,7 @@
       <c r="A5" s="9">
         <v>23</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -2997,7 +3266,7 @@
       <c r="A6" s="9">
         <v>542</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -3015,7 +3284,7 @@
       <c r="A7" s="9">
         <v>733</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -3033,7 +3302,7 @@
       <c r="A8" s="9">
         <v>200</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -3051,7 +3320,7 @@
       <c r="A9" s="9">
         <v>235</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -3069,7 +3338,7 @@
       <c r="A10" s="9">
         <v>226</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -3083,11 +3352,11 @@
       <c r="G10" s="5"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" ht="27.6" spans="1:8">
       <c r="A11" s="9">
         <v>104</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -3101,11 +3370,11 @@
       <c r="G11" s="5"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" ht="27.6" spans="1:8">
       <c r="A12" s="9">
         <v>232</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -3123,7 +3392,7 @@
       <c r="A13" s="9">
         <v>20</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -3137,11 +3406,11 @@
       <c r="G13" s="5"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" ht="27.6" spans="1:8">
       <c r="A14" s="9">
         <v>225</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -3159,7 +3428,7 @@
       <c r="A15" s="9">
         <v>141</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -3177,7 +3446,7 @@
       <c r="A16" s="9">
         <v>206</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -3195,7 +3464,7 @@
       <c r="A17" s="9">
         <v>54</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -3213,7 +3482,7 @@
       <c r="A18" s="9">
         <v>73</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>51</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -3231,7 +3500,7 @@
       <c r="A19" s="10">
         <v>33</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C19" s="6" t="s">
@@ -3257,7 +3526,7 @@
       <c r="A20" s="9">
         <v>704</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>60</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -3275,7 +3544,7 @@
       <c r="A21" s="9">
         <v>78</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>63</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -3293,7 +3562,7 @@
       <c r="A22" s="9">
         <v>77</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>66</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -3311,7 +3580,7 @@
       <c r="A23" s="9">
         <v>22</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>68</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -3329,7 +3598,7 @@
       <c r="A24" s="4">
         <v>121</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -3355,7 +3624,7 @@
       <c r="A25" s="9">
         <v>208</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>75</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -3431,7 +3700,7 @@
       <c r="A28" s="4">
         <v>217</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>92</v>
       </c>
       <c r="C28" s="6" t="s">
@@ -3457,7 +3726,7 @@
       <c r="A29" s="9">
         <v>56</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>98</v>
       </c>
       <c r="C29" s="6" t="s">
@@ -3481,7 +3750,7 @@
       <c r="A30" s="11">
         <v>152</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>103</v>
       </c>
       <c r="C30" s="6" t="s">
@@ -3505,7 +3774,7 @@
       <c r="A31" s="11">
         <v>15</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="5" t="s">
         <v>107</v>
       </c>
       <c r="C31" s="6" t="s">
@@ -3531,7 +3800,7 @@
       <c r="A32" s="11">
         <v>57</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="5" t="s">
         <v>113</v>
       </c>
       <c r="C32" s="6" t="s">
@@ -3555,7 +3824,7 @@
       <c r="A33" s="11">
         <v>70</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C33" s="6" t="s">
@@ -3579,7 +3848,7 @@
       <c r="A34" s="11">
         <v>322</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="5" t="s">
         <v>125</v>
       </c>
       <c r="C34" s="6" t="s">
@@ -3603,7 +3872,7 @@
       <c r="A35" s="11">
         <v>11</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="5" t="s">
         <v>130</v>
       </c>
       <c r="C35" s="6" t="s">
@@ -3629,7 +3898,7 @@
       <c r="A36" s="11">
         <v>239</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="5" t="s">
         <v>136</v>
       </c>
       <c r="C36" s="6" t="s">
@@ -3655,7 +3924,7 @@
       <c r="A37" s="4">
         <v>242</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="5" t="s">
         <v>142</v>
       </c>
       <c r="C37" s="6" t="s">
@@ -3681,7 +3950,7 @@
       <c r="A38" s="9">
         <v>198</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="5" t="s">
         <v>147</v>
       </c>
       <c r="C38" s="6" t="s">
@@ -3707,7 +3976,7 @@
       <c r="A39" s="11">
         <v>300</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="5" t="s">
         <v>152</v>
       </c>
       <c r="C39" s="6" t="s">
@@ -3728,28 +3997,104 @@
       <c r="H39" s="6"/>
     </row>
     <row r="40" ht="131" customHeight="1" spans="1:8">
-      <c r="A40" s="13">
+      <c r="A40" s="11">
         <v>371</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="E40" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="F40" s="15" t="s">
+      <c r="F40" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="G40" s="15" t="s">
+      <c r="G40" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="H40" s="14"/>
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" ht="124.2" spans="1:8">
+      <c r="A41" s="13">
+        <v>191</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="G41" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="H41" s="15"/>
+    </row>
+    <row r="42" ht="179.4" spans="1:8">
+      <c r="A42" s="16">
+        <v>125</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="G42" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="H42" s="15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="43" ht="96.6" spans="1:8">
+      <c r="A43" s="13">
+        <v>3</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="G43" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="H43" s="15" t="s">
+        <v>180</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
[LC] Update math 50 and sqrt, review string 2 qurestions.
</commit_message>
<xml_diff>
--- a/Leetcode/Problem-tracker.xlsx
+++ b/Leetcode/Problem-tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9767"/>
+    <workbookView windowWidth="22176" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="197">
   <si>
     <t>Prompt</t>
   </si>
@@ -1880,6 +1880,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Bitwise Counting" pattern. The key is to count how many 1s are present in the binary representation of an unsigned integer.
 Solution Approach: Use bitwise operations to efficiently count 1 bits. The optimal approach is Brian Kernighan’s Algorithm, which clears the least significant 1 in each iteration, reducing time complexity to O(k), where k is the number of 1 bits.
 Two solutions:
@@ -1914,6 +1920,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the </t>
     </r>
     <r>
@@ -1955,6 +1967,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When checking if a given string is a valid </t>
     </r>
     <r>
@@ -2012,6 +2030,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: The problem follows the Sliding Window pattern where we </t>
     </r>
     <r>
@@ -2068,6 +2092,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When dealing with </t>
     </r>
     <r>
@@ -2116,6 +2146,241 @@
   </si>
   <si>
     <t>2025.2.20; 2025.11.17</t>
+  </si>
+  <si>
+    <t>Pow(x, n)</t>
+  </si>
+  <si>
+    <t>2025.2.21</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: This problem involves calculating the power of a number efficiently. A naive approach using repeated multiplication would be too </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>slow for large exponents</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">. Instead, we can use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Binary Exponentiation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">, which </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>reduces the number of multiplications</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> to O(log n).
+Solution Approach: We use Exponentiation by Squaring, which involves dividing the exponent by 2 at each step, recursively or iteratively computing the result, and multiplying it accordingly. This optimizes the process by significantly reducing the number of multiplications.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Not solved first time, it's better to decrement to check odd or even rather than incrementing to the target n</t>
+    </r>
+  </si>
+  <si>
+    <t>1. When efficiently computing large exponents.
+2. When dealing with scenarios requiring modular exponentiation in cryptography.
+3. When optimizing repeated multiplication in computational mathematics.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/powx-n/description/</t>
+  </si>
+  <si>
+    <t>Sqrt(x)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: The problem requires computing the integer square root of a given non-negative number without using built-in functions like sqrt(). The optimal approach is Binary Search, which reduces the search space logarithmically.
+Solution Approach: Use Binary Search between 0 and x, checking the square of the mid-value. If mid^2 is greater than x, move left; otherwise, move right. The final result will be the largest integer whose square is ≤ x.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Not solved first time</t>
+    </r>
+  </si>
+  <si>
+    <t>1. When computing integer square roots efficiently.
+2. When optimizing search problems using binary search.
+3. When solving mathematical problems with logarithmic complexity constraints.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sqrtx/description/</t>
+  </si>
+  <si>
+    <t>Longest Repeating Character Replacement</t>
+  </si>
+  <si>
+    <t>String; Sliding window; two pointers</t>
+  </si>
+  <si>
+    <r>
+      <t>Problem Pattern: This problem involves finding the longest substring where we can replace at most k characters to make all characters the same. The Sliding Window technique efficiently finds the maximum window that satisfies this condition.
+Solution Approach: Maintain a</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> sliding window with two pointers (left and right)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>track the frequency of characters</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">. If the total characters in the window minus the most frequent character count is greater than k, shrink the window. The maximum valid window size is the answer.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Not solved for the second time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+Count the frequency of each letter in every window;
+Check if window_size - max_frequency &gt; k, if so, keep moving right to plus one, otherwise, move left
+No need to clear up the entire hashmap, but decrement the frequency of the crossed-out element
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Expand as much as possible until unvalid, then shrink as much as possible until valid, then expand</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When finding the longest subarray with at most k modifications.
+2. When working with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>variable-length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> window problems.
+3. When optimizing character frequency-based constraints in a substring.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-repeating-character-replacement/description/</t>
+  </si>
+  <si>
+    <t>2025.2.21; 2024.11.22</t>
   </si>
 </sst>
 </file>
@@ -2294,16 +2559,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -2778,7 +3043,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2826,9 +3091,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -3141,10 +3403,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="7"/>
@@ -4021,79 +4283,153 @@
       <c r="H40" s="6"/>
     </row>
     <row r="41" ht="124.2" spans="1:8">
-      <c r="A41" s="13">
+      <c r="A41" s="11">
         <v>191</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="D41" s="14" t="s">
+      <c r="D41" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="E41" s="14" t="s">
+      <c r="E41" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="F41" s="14" t="s">
+      <c r="F41" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="G41" s="14" t="s">
+      <c r="G41" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="H41" s="15"/>
+      <c r="H41" s="6"/>
     </row>
     <row r="42" ht="179.4" spans="1:8">
-      <c r="A42" s="16">
+      <c r="A42" s="4">
         <v>125</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C42" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="D42" s="14" t="s">
+      <c r="D42" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="E42" s="14" t="s">
+      <c r="E42" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="F42" s="14" t="s">
+      <c r="F42" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="G42" s="14" t="s">
+      <c r="G42" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="H42" s="15" t="s">
+      <c r="H42" s="6" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="43" ht="96.6" spans="1:8">
-      <c r="A43" s="13">
+      <c r="A43" s="11">
         <v>3</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C43" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="D43" s="14" t="s">
+      <c r="D43" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="E43" s="14" t="s">
+      <c r="E43" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="F43" s="14" t="s">
+      <c r="F43" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="G43" s="14" t="s">
+      <c r="G43" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="H43" s="15" t="s">
+      <c r="H43" s="6" t="s">
         <v>180</v>
+      </c>
+    </row>
+    <row r="44" ht="110.4" spans="1:8">
+      <c r="A44" s="13">
+        <v>50</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="G44" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="H44" s="15"/>
+    </row>
+    <row r="45" ht="110.4" spans="1:8">
+      <c r="A45" s="13">
+        <v>69</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="G45" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="H45" s="15"/>
+    </row>
+    <row r="46" ht="208" customHeight="1" spans="1:8">
+      <c r="A46" s="13">
+        <v>424</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="G46" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="H46" s="15" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[LC] Update review for hashtable.
</commit_message>
<xml_diff>
--- a/Leetcode/Problem-tracker.xlsx
+++ b/Leetcode/Problem-tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22176" windowHeight="9780"/>
+    <workbookView windowWidth="22188" windowHeight="9767"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="227">
   <si>
     <t>Prompt</t>
   </si>
@@ -86,7 +86,7 @@
     <t>Two Sum</t>
   </si>
   <si>
-    <t>2025.2.11</t>
+    <t>2025.2.22</t>
   </si>
   <si>
     <t>Hash table</t>
@@ -104,10 +104,13 @@
     <t>https://leetcode.com/problems/two-sum/description/</t>
   </si>
   <si>
-    <t>2025.2.11; 2024.10.31</t>
+    <t>2025.2.22; 2025.2.11; 2024.10.31</t>
   </si>
   <si>
     <t>K Closet Points to Origin</t>
+  </si>
+  <si>
+    <t>2025.2.11</t>
   </si>
   <si>
     <t>Heap</t>
@@ -342,6 +345,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock/description/</t>
+  </si>
+  <si>
+    <t>2025.2.11; 2024.10.31</t>
   </si>
   <si>
     <t>Implement Trie (Prefix Tree)</t>
@@ -2158,6 +2164,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem involves calculating the power of a number efficiently. A naive approach using repeated multiplication would be too </t>
     </r>
     <r>
@@ -2243,6 +2255,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: The problem requires computing the integer square root of a given non-negative number without using built-in functions like sqrt(). The optimal approach is Binary Search, which reduces the search space logarithmically.
 Solution Approach: Use Binary Search between 0 and x, checking the square of the mid-value. If mid^2 is greater than x, move left; otherwise, move right. The final result will be the largest integer whose square is ≤ x.
 </t>
@@ -2274,6 +2292,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t>Problem Pattern: This problem involves finding the longest substring where we can replace at most k characters to make all characters the same. The Sliding Window technique efficiently finds the maximum window that satisfies this condition.
 Solution Approach: Maintain a</t>
     </r>
@@ -2352,6 +2376,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When finding the longest subarray with at most k modifications.
 2. When working with </t>
     </r>
@@ -2381,6 +2411,533 @@
   </si>
   <si>
     <t>2025.2.21; 2024.11.22</t>
+  </si>
+  <si>
+    <t>Overlap Rectangles</t>
+  </si>
+  <si>
+    <t>Geometry</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: The problem involves determining whether two axis-aligned rectangles overlap. This can be solved using coordinate comparisons.
+Solution Approach: The key idea is to check if one rectangle is completely to the left, right, above, or below the other. If none of these conditions hold, the rectangles must overlap.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Solved first time with formula</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When working with axis-aligned rectangle intersections.
+2. When solving computational geometry problems involving </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>bounding boxes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">.
+3. When implementing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>collision detection</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> in 2D simulations.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/rectangle-overlap/description/</t>
+  </si>
+  <si>
+    <t>Ransom Note</t>
+  </si>
+  <si>
+    <t>Hashtable</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: The problem involves checking if one string (ransomNote) can be formed using the characters from another string (magazine). This is a classic </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">character frequency counting </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>problem.
+Solution Approach: Use a hash table (dictionary) or an array to count character frequencies in magazine, then check if ransomNote can be formed using these frequencies.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+Solved second time, use hashtable solution but not that efficient</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+Alternative:
+1. sort two magazine and ransomNote, then go through every letter to check the length of index. O(nlogn)
+2. Use Counter function to count two strings, then perform cnt1 &amp; cnt2 == cnt1, if so, return true
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3. Use Counter function to count the magazine rather than a for loop, then check frequence in ransom</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When solving </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">character frequency </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>problems.
+2. When working with string manipulation involving counting occurrences.
+3. When optimizing character-based lookups in O(1) time.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/ransom-note/description/</t>
+  </si>
+  <si>
+    <t>2025.2.22; 2024.11.25</t>
+  </si>
+  <si>
+    <t>Group Anagram</t>
+  </si>
+  <si>
+    <t>Hash table; String; Sorting</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: Given a list of strings, group anagrams together. Anagrams have the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>same characters but in different orders</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">.
+Solution Approach: Use a hash table where the key is a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>canonical form (sorted string or frequency tuple</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>), and the value is a list of anagram words.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When dealing with problems involving </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>grouping by a common property</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>.
+2. When handling string rearrangements that need fast lookups.
+3. When optimizing solutions using dictionary-based hashing.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/group-anagrams/description/</t>
+  </si>
+  <si>
+    <t>2025.2.22; 2024.11.26</t>
+  </si>
+  <si>
+    <t>Insert Delete GetRandom O(1)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: Implement a data structure that supports insert(val), remove(val), and getRandom() in O(1) time.
+Solution Approach: Use a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>hash map (dict)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> for O(1) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>insert/remove lookups</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> and a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>list</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> (array) to store values for O(1)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> random access</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>.(</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>The hashmap and hashet does not support indexed access</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Solved second time, but not the most efficient. Most time-consuming part is conver a set to list-O(n)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When implementing data structures with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>fast insertion, deletion, and random access</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>.
+2. When designing randomized algorithms with efficient operations.
+3. When optimizing O(1) operations for performance-sensitive applications.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/insert-delete-getrandom-o1/description/</t>
+  </si>
+  <si>
+    <t>2025.2.22; 2024.12.15</t>
+  </si>
+  <si>
+    <t>First Missing Positive</t>
+  </si>
+  <si>
+    <t>Hash table; Array; Cyclic Sort</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: Find the smallest missing positive integer from an unsorted array in O(n) time and O(1) space.
+Solution Approach: Use Cyclic Sort (Indexing Sort) to place each number at its correct position (nums[i] = i+1 where possible), then scan the array for the first missing positive number.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Solved second time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> using set()+linear search, which cost O(n) time and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">space complexity
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Alternative:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Use cyclic sort which runs in O(n) time complexity and O(1) space complexity
+Cyclic Sort is a sorting algorithm used when numbers are in a known range (1 to n). Instead of using extra space, it places each number at its correct index using swaps, making it efficient for in-place sorting.
+Two looking out:
+1. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>The condition should be a while, until the current position is not valid. 
+2. Swap operation should be looking out</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When solving </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>in-place array</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> problems with a constrained space limit.
+2. When looking for the smallest missing element in a range.
+3. When </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>avoiding extra space</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> and optimizing runtime complexity to O(n).</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/first-missing-positive/description/</t>
+  </si>
+  <si>
+    <t>2025.2.22; 2024.12.18</t>
   </si>
 </sst>
 </file>
@@ -2393,7 +2950,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2411,6 +2968,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Cambria"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Cambria"/>
       <charset val="134"/>
     </font>
@@ -2559,6 +3122,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -2572,7 +3144,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2582,6 +3154,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2913,55 +3491,52 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2976,74 +3551,77 @@
     <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3077,13 +3655,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3091,6 +3672,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -3403,10 +3990,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="7"/>
@@ -3496,10 +4083,10 @@
         <v>17</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="5"/>
@@ -3511,13 +4098,13 @@
         <v>23</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="5"/>
@@ -3529,13 +4116,13 @@
         <v>542</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="5"/>
@@ -3547,13 +4134,13 @@
         <v>733</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="5"/>
@@ -3565,13 +4152,13 @@
         <v>200</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="5"/>
@@ -3583,13 +4170,13 @@
         <v>235</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="5"/>
@@ -3601,13 +4188,13 @@
         <v>226</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="5"/>
@@ -3619,13 +4206,13 @@
         <v>104</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="5"/>
@@ -3637,13 +4224,13 @@
         <v>232</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="5"/>
@@ -3655,13 +4242,13 @@
         <v>20</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="5"/>
@@ -3673,13 +4260,13 @@
         <v>225</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="5"/>
@@ -3691,13 +4278,13 @@
         <v>141</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="5"/>
@@ -3709,13 +4296,13 @@
         <v>206</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="5"/>
@@ -3727,13 +4314,13 @@
         <v>54</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="5"/>
@@ -3745,13 +4332,13 @@
         <v>73</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>50</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="5"/>
@@ -3763,25 +4350,25 @@
         <v>33</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" ht="27.6" spans="1:8">
@@ -3789,13 +4376,13 @@
         <v>704</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="5"/>
@@ -3807,13 +4394,13 @@
         <v>78</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="5"/>
@@ -3825,13 +4412,13 @@
         <v>77</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="5"/>
@@ -3843,13 +4430,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="5"/>
@@ -3861,25 +4448,25 @@
         <v>121</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" ht="96.6" spans="1:8">
@@ -3887,22 +4474,22 @@
         <v>208</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H25" s="6"/>
     </row>
@@ -3911,51 +4498,51 @@
         <v>238</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" ht="96.6" spans="1:8">
-      <c r="A27" s="11">
+      <c r="A27" s="13">
         <v>53</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" ht="82.8" spans="1:8">
@@ -3963,25 +4550,25 @@
         <v>217</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" ht="82.8" spans="1:8">
@@ -3989,197 +4576,197 @@
         <v>56</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H29" s="6"/>
     </row>
     <row r="30" ht="110.4" spans="1:8">
-      <c r="A30" s="11">
+      <c r="A30" s="13">
         <v>152</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H30" s="6"/>
     </row>
     <row r="31" ht="153.6" spans="1:8">
-      <c r="A31" s="11">
+      <c r="A31" s="13">
         <v>15</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" ht="124.2" spans="1:8">
-      <c r="A32" s="11">
+      <c r="A32" s="13">
         <v>57</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H32" s="6"/>
     </row>
     <row r="33" ht="96.6" spans="1:8">
-      <c r="A33" s="11">
+      <c r="A33" s="13">
         <v>70</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H33" s="6"/>
     </row>
     <row r="34" ht="124.2" spans="1:8">
-      <c r="A34" s="11">
+      <c r="A34" s="13">
         <v>322</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H34" s="6"/>
     </row>
     <row r="35" ht="151.8" spans="1:8">
-      <c r="A35" s="11">
+      <c r="A35" s="13">
         <v>11</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" ht="193.2" spans="1:8">
-      <c r="A36" s="11">
+      <c r="A36" s="13">
         <v>239</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" ht="179.4" spans="1:8">
@@ -4187,25 +4774,25 @@
         <v>242</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D37" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="H37" s="6" t="s">
         <v>143</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="38" ht="193.2" spans="1:8">
@@ -4213,96 +4800,96 @@
         <v>198</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F38" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="H38" s="6" t="s">
         <v>150</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="39" ht="110.4" spans="1:8">
-      <c r="A39" s="11">
+      <c r="A39" s="13">
         <v>300</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H39" s="6"/>
     </row>
     <row r="40" ht="131" customHeight="1" spans="1:8">
-      <c r="A40" s="11">
+      <c r="A40" s="13">
         <v>371</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H40" s="6"/>
     </row>
     <row r="41" ht="124.2" spans="1:8">
-      <c r="A41" s="11">
+      <c r="A41" s="13">
         <v>191</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H41" s="6"/>
     </row>
@@ -4311,125 +4898,253 @@
         <v>125</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="43" ht="96.6" spans="1:8">
-      <c r="A43" s="11">
+      <c r="A43" s="13">
         <v>3</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44" ht="110.4" spans="1:8">
       <c r="A44" s="13">
         <v>50</v>
       </c>
-      <c r="B44" s="14" t="s">
-        <v>181</v>
+      <c r="B44" s="5" t="s">
+        <v>183</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="E44" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="F44" s="14" t="s">
+      <c r="D44" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="G44" s="14" t="s">
+      <c r="E44" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="H44" s="15"/>
+      <c r="F44" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="H44" s="6"/>
     </row>
     <row r="45" ht="110.4" spans="1:8">
       <c r="A45" s="13">
         <v>69</v>
       </c>
-      <c r="B45" s="14" t="s">
-        <v>187</v>
+      <c r="B45" s="5" t="s">
+        <v>189</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="D45" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="E45" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="F45" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="G45" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E45" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="H45" s="15"/>
+      <c r="F45" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="H45" s="6"/>
     </row>
     <row r="46" ht="208" customHeight="1" spans="1:8">
       <c r="A46" s="13">
         <v>424</v>
       </c>
-      <c r="B46" s="14" t="s">
-        <v>191</v>
+      <c r="B46" s="5" t="s">
+        <v>193</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="E46" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="F46" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="D46" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="G46" s="14" t="s">
+      <c r="E46" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="H46" s="15" t="s">
+      <c r="F46" s="5" t="s">
         <v>196</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="47" ht="82.8" spans="1:8">
+      <c r="A47" s="14">
+        <v>836</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="G47" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="H47" s="16"/>
+    </row>
+    <row r="48" ht="156" customHeight="1" spans="1:8">
+      <c r="A48" s="17">
+        <v>383</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="G48" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="H48" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="49" ht="82.8" spans="1:8">
+      <c r="A49" s="17">
+        <v>49</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="G49" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="H49" s="16" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="50" ht="82.8" spans="1:8">
+      <c r="A50" s="18">
+        <v>380</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="F50" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="G50" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="H50" s="16" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="51" ht="179.4" spans="1:8">
+      <c r="A51" s="18">
+        <v>41</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="E51" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="G51" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="H51" s="16" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[LC] Update question review for hashtable.
</commit_message>
<xml_diff>
--- a/Leetcode/Problem-tracker.xlsx
+++ b/Leetcode/Problem-tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9767"/>
+    <workbookView windowWidth="27945" windowHeight="12960"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="237">
   <si>
     <t>Prompt</t>
   </si>
@@ -2420,6 +2420,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: The problem involves determining whether two axis-aligned rectangles overlap. This can be solved using coordinate comparisons.
 Solution Approach: The key idea is to check if one rectangle is completely to the left, right, above, or below the other. If none of these conditions hold, the rectangles must overlap.
 </t>
@@ -2437,6 +2443,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When working with axis-aligned rectangle intersections.
 2. When solving computational geometry problems involving </t>
     </r>
@@ -2491,6 +2503,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: The problem involves checking if one string (ransomNote) can be formed using the characters from another string (magazine). This is a classic </t>
     </r>
     <r>
@@ -2550,6 +2568,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When solving </t>
     </r>
     <r>
@@ -2588,6 +2612,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: Given a list of strings, group anagrams together. Anagrams have the </t>
     </r>
     <r>
@@ -2632,6 +2662,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When dealing with problems involving </t>
     </r>
     <r>
@@ -2667,6 +2703,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: Implement a data structure that supports insert(val), remove(val), and getRandom() in O(1) time.
 Solution Approach: Use a </t>
     </r>
@@ -2779,6 +2821,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When implementing data structures with </t>
     </r>
     <r>
@@ -2817,6 +2865,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: Find the smallest missing positive integer from an unsorted array in O(n) time and O(1) space.
 Solution Approach: Use Cyclic Sort (Indexing Sort) to place each number at its correct position (nums[i] = i+1 where possible), then scan the array for the first missing positive number.
 </t>
@@ -2890,6 +2944,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When solving </t>
     </r>
     <r>
@@ -2938,6 +2998,153 @@
   </si>
   <si>
     <t>2025.2.22; 2024.12.18</t>
+  </si>
+  <si>
+    <t>LRU Cache</t>
+  </si>
+  <si>
+    <t>2025.2.23</t>
+  </si>
+  <si>
+    <t>Hash table; Doubly linked list</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: The problem requires designing a data structure that supports </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>get() and put()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> operations in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>O(1) time complexity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">, while maintaining the Least Recently Used (LRU) eviction policy.
+Solution Approach: We use a HashMap + Doubly Linked List approach, where the HashMap stores key-node pairs for O(1) lookups, and the Doubly Linked List maintains the order of usage to efficiently remove and update the least recently used item.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Not solve second by using hashmap as cache map key&amp;value look up and queue dealing with constant insert/remove</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+Quick(O(1)) look up -&gt; hashmap
+Quick rearrange -&gt; linked list
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Most efficient alternative: OrderedDict
+Be familiar with move_to_end and popitem(last=False)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When implementing caching mechanisms to optimize data retrieval.
+2. When designing a system that maintains </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>recent access history</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">, such as browser history, database caching, or memory paging.
+3. When needing an efficient </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>O(1) time complexity solution for insert, delete, and access</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> operations while keeping track of the most recent elements.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/lru-cache/description/</t>
+  </si>
+  <si>
+    <t>2025.2.23; 2024.12.1</t>
+  </si>
+  <si>
+    <t>All O`one Data Structure</t>
+  </si>
+  <si>
+    <t>Not Solved in O(1) Time Complexity</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/all-oone-data-structure/description/</t>
   </si>
 </sst>
 </file>
@@ -3122,12 +3329,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Cambria"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
@@ -3138,9 +3342,12 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <i/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Cambria"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -3621,7 +3828,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3664,7 +3871,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3672,12 +3879,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -3990,21 +4191,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="6.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6296296296296" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.6333333333333" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.25" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.3611111111111" style="2" customWidth="1"/>
-    <col min="5" max="5" width="94.8981481481482" style="3" customWidth="1"/>
-    <col min="6" max="6" width="43.2592592592593" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.2962962962963" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.3583333333333" style="2" customWidth="1"/>
+    <col min="5" max="5" width="94.9" style="3" customWidth="1"/>
+    <col min="6" max="6" width="43.2583333333333" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.3" style="2" customWidth="1"/>
     <col min="8" max="8" width="32.6666666666667" style="3" customWidth="1"/>
     <col min="9" max="16384" width="9" style="3"/>
   </cols>
@@ -4049,7 +4250,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" ht="96.6" spans="1:8">
+    <row r="3" ht="85.5" spans="1:8">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -4201,7 +4402,7 @@
       <c r="G10" s="5"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" ht="27.6" spans="1:8">
+    <row r="11" spans="1:8">
       <c r="A11" s="9">
         <v>104</v>
       </c>
@@ -4219,7 +4420,7 @@
       <c r="G11" s="5"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" ht="27.6" spans="1:8">
+    <row r="12" spans="1:8">
       <c r="A12" s="9">
         <v>232</v>
       </c>
@@ -4255,7 +4456,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" ht="27.6" spans="1:8">
+    <row r="14" spans="1:8">
       <c r="A14" s="9">
         <v>225</v>
       </c>
@@ -4345,7 +4546,7 @@
       <c r="G18" s="5"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" ht="82.8" spans="1:8">
+    <row r="19" ht="85.5" spans="1:8">
       <c r="A19" s="10">
         <v>33</v>
       </c>
@@ -4371,7 +4572,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" ht="27.6" spans="1:8">
+    <row r="20" spans="1:8">
       <c r="A20" s="9">
         <v>704</v>
       </c>
@@ -4443,7 +4644,7 @@
       <c r="G23" s="5"/>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" ht="138" spans="1:8">
+    <row r="24" ht="99.75" spans="1:8">
       <c r="A24" s="4">
         <v>121</v>
       </c>
@@ -4469,7 +4670,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" ht="96.6" spans="1:8">
+    <row r="25" ht="85.5" spans="1:8">
       <c r="A25" s="9">
         <v>208</v>
       </c>
@@ -4493,7 +4694,7 @@
       </c>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" ht="124.2" spans="1:8">
+    <row r="26" ht="114" spans="1:8">
       <c r="A26" s="11">
         <v>238</v>
       </c>
@@ -4519,7 +4720,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" ht="96.6" spans="1:8">
+    <row r="27" ht="99.75" spans="1:8">
       <c r="A27" s="13">
         <v>53</v>
       </c>
@@ -4545,7 +4746,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" ht="82.8" spans="1:8">
+    <row r="28" ht="85.5" spans="1:8">
       <c r="A28" s="4">
         <v>217</v>
       </c>
@@ -4571,7 +4772,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" ht="82.8" spans="1:8">
+    <row r="29" ht="85.5" spans="1:8">
       <c r="A29" s="9">
         <v>56</v>
       </c>
@@ -4595,7 +4796,7 @@
       </c>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" ht="110.4" spans="1:8">
+    <row r="30" ht="85.5" spans="1:8">
       <c r="A30" s="13">
         <v>152</v>
       </c>
@@ -4619,7 +4820,7 @@
       </c>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" ht="153.6" spans="1:8">
+    <row r="31" ht="142.5" spans="1:8">
       <c r="A31" s="13">
         <v>15</v>
       </c>
@@ -4645,7 +4846,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="32" ht="124.2" spans="1:8">
+    <row r="32" ht="128.25" spans="1:8">
       <c r="A32" s="13">
         <v>57</v>
       </c>
@@ -4669,7 +4870,7 @@
       </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" ht="96.6" spans="1:8">
+    <row r="33" ht="85.5" spans="1:8">
       <c r="A33" s="13">
         <v>70</v>
       </c>
@@ -4693,7 +4894,7 @@
       </c>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" ht="124.2" spans="1:8">
+    <row r="34" ht="114" spans="1:8">
       <c r="A34" s="13">
         <v>322</v>
       </c>
@@ -4717,7 +4918,7 @@
       </c>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" ht="151.8" spans="1:8">
+    <row r="35" ht="156.75" spans="1:8">
       <c r="A35" s="13">
         <v>11</v>
       </c>
@@ -4743,7 +4944,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="36" ht="193.2" spans="1:8">
+    <row r="36" ht="199.5" spans="1:8">
       <c r="A36" s="13">
         <v>239</v>
       </c>
@@ -4769,7 +4970,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="37" ht="179.4" spans="1:8">
+    <row r="37" ht="185.25" spans="1:8">
       <c r="A37" s="4">
         <v>242</v>
       </c>
@@ -4795,7 +4996,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="38" ht="193.2" spans="1:8">
+    <row r="38" ht="199.5" spans="1:8">
       <c r="A38" s="9">
         <v>198</v>
       </c>
@@ -4821,7 +5022,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="39" ht="110.4" spans="1:8">
+    <row r="39" ht="99.75" spans="1:8">
       <c r="A39" s="13">
         <v>300</v>
       </c>
@@ -4869,7 +5070,7 @@
       </c>
       <c r="H40" s="6"/>
     </row>
-    <row r="41" ht="124.2" spans="1:8">
+    <row r="41" ht="128.25" spans="1:8">
       <c r="A41" s="13">
         <v>191</v>
       </c>
@@ -4893,7 +5094,7 @@
       </c>
       <c r="H41" s="6"/>
     </row>
-    <row r="42" ht="179.4" spans="1:8">
+    <row r="42" ht="171" spans="1:8">
       <c r="A42" s="4">
         <v>125</v>
       </c>
@@ -4919,7 +5120,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="43" ht="96.6" spans="1:8">
+    <row r="43" ht="85.5" spans="1:8">
       <c r="A43" s="13">
         <v>3</v>
       </c>
@@ -4945,7 +5146,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="44" ht="110.4" spans="1:8">
+    <row r="44" ht="99.75" spans="1:8">
       <c r="A44" s="13">
         <v>50</v>
       </c>
@@ -4969,7 +5170,7 @@
       </c>
       <c r="H44" s="6"/>
     </row>
-    <row r="45" ht="110.4" spans="1:8">
+    <row r="45" ht="85.5" spans="1:8">
       <c r="A45" s="13">
         <v>69</v>
       </c>
@@ -5019,132 +5220,182 @@
         <v>198</v>
       </c>
     </row>
-    <row r="47" ht="82.8" spans="1:8">
-      <c r="A47" s="14">
+    <row r="47" ht="85.5" spans="1:8">
+      <c r="A47" s="9">
         <v>836</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C47" s="16" t="s">
+      <c r="C47" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D47" s="15" t="s">
+      <c r="D47" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="E47" s="15" t="s">
+      <c r="E47" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="F47" s="15" t="s">
+      <c r="F47" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="G47" s="15" t="s">
+      <c r="G47" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="H47" s="16"/>
+      <c r="H47" s="6"/>
     </row>
     <row r="48" ht="156" customHeight="1" spans="1:8">
-      <c r="A48" s="17">
+      <c r="A48" s="4">
         <v>383</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="C48" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D48" s="15" t="s">
+      <c r="D48" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="E48" s="15" t="s">
+      <c r="E48" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="F48" s="15" t="s">
+      <c r="F48" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="G48" s="15" t="s">
+      <c r="G48" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="H48" s="16" t="s">
+      <c r="H48" s="6" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="49" ht="82.8" spans="1:8">
-      <c r="A49" s="17">
+    <row r="49" ht="85.5" spans="1:8">
+      <c r="A49" s="4">
         <v>49</v>
       </c>
-      <c r="B49" s="15" t="s">
+      <c r="B49" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="C49" s="16" t="s">
+      <c r="C49" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D49" s="15" t="s">
+      <c r="D49" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="E49" s="15" t="s">
+      <c r="E49" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="F49" s="15" t="s">
+      <c r="F49" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="G49" s="15" t="s">
+      <c r="G49" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="H49" s="16" t="s">
+      <c r="H49" s="6" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="50" ht="82.8" spans="1:8">
-      <c r="A50" s="18">
+    <row r="50" ht="85.5" spans="1:8">
+      <c r="A50" s="11">
         <v>380</v>
       </c>
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="C50" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D50" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E50" s="15" t="s">
+      <c r="E50" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="F50" s="15" t="s">
+      <c r="F50" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="G50" s="15" t="s">
+      <c r="G50" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="H50" s="16" t="s">
+      <c r="H50" s="6" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="51" ht="179.4" spans="1:8">
-      <c r="A51" s="18">
+    <row r="51" ht="156.75" spans="1:8">
+      <c r="A51" s="11">
         <v>41</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="C51" s="16" t="s">
+      <c r="C51" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D51" s="15" t="s">
+      <c r="D51" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="E51" s="15" t="s">
+      <c r="E51" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="F51" s="15" t="s">
+      <c r="F51" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="G51" s="15" t="s">
+      <c r="G51" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="H51" s="16" t="s">
+      <c r="H51" s="6" t="s">
         <v>226</v>
+      </c>
+    </row>
+    <row r="52" ht="156.75" spans="1:8">
+      <c r="A52" s="14">
+        <v>146</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="E52" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="G52" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="H52" s="16" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="53" ht="71.25" spans="1:8">
+      <c r="A53" s="14">
+        <v>432</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="E53" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="H53" s="16" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -5169,7 +5420,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -5186,7 +5437,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
[LC] Update leetcode 110 and 278 question.
</commit_message>
<xml_diff>
--- a/Leetcode/Problem-tracker.xlsx
+++ b/Leetcode/Problem-tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12960"/>
+    <workbookView windowWidth="22188" windowHeight="9767"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="272">
   <si>
     <t>No.</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t>Problem Pattern: This problem follows the "</t>
     </r>
     <r>
@@ -149,6 +155,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When working with image processing or flood-fill operations in a 2D grid.
 2. When using BFS/DFS to </t>
     </r>
@@ -212,6 +224,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Binary Search Tree (BST) Properties" pattern. The key idea is to use the BST property where for any node: left subtree &lt; node &lt; right subtree, allowing efficient searching.
 Solution Approach: Traverse the tree, moving left if both nodes are smaller than the root, right if both are larger, and return the current node if it lies between p and q. Runs in O(log n) time for balanced BSTs and O(n) in the worst case (skewed tree).
 </t>
@@ -243,6 +261,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Tree Traversal &amp; Modification" pattern. The key idea is to swap left and right subtrees recursively or iteratively.
 Solution Approach: Use recursion (DFS) or queue-based BFS (iterative approach) to traverse the tree and swap child nodes. Runs in O(n) time complexity with O(h) space for recursion (O(n) in worst case).
 </t>
@@ -289,6 +313,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Stack for Matching Pairs" pattern. The key is to use a stack to track opening parentheses and ensure that each closing parenthesis has a matching opening one in the correct order.
 Solution Approach: Iterate through the string, pushing opening brackets onto a stack, and popping from the stack when encountering a closing bracket. If the stack is empty at the end, the string is valid. This runs in O(n) time complexity with O(n) space.
 </t>
@@ -307,6 +337,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When validating balanced expressions with </t>
     </r>
     <r>
@@ -373,6 +409,55 @@
   </si>
   <si>
     <t>Linked List</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: This problem follows the "Cycle Detection in Linked Lists" pattern. The key idea is to determine whether a linked list contains a cycle using a slow and fast pointer (Floyd’s Cycle Detection Algorithm).
+Solution Approach: Use two pointers (slow moves one step, fast moves two steps). If they ever meet, a cycle exists. Runs in O(n) time complexity with O(1) space.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Not solved second time. Be aware of the stop condition is all about the fast</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>detecting cycles in linked lists</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> or graphs.
+2. When implementing algorithms that rely on slow-fast pointer techniques (e.g., finding cycle start).
+3. When detecting infinite loops in linked data structures.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/linked-list-cycle/description/</t>
+  </si>
+  <si>
+    <t>2025.2.25; 2025.1.31</t>
   </si>
   <si>
     <t>Reverse Linked List</t>
@@ -446,6 +531,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Divide &amp; Conquer (Binary Search)" pattern. The key idea is to repeatedly divide the sorted array in half and check the middle element to decide whether to search in the left or right half.
 Solution Approach: Use iterative or recursive binary search to achieve O(log n) time complexity.
 </t>
@@ -3380,6 +3471,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Merge Two Sorted Sequences" pattern. The key is to merge two already sorted linked lists into one sorted linked list while maintaining their order.
 Solution Approach: Use a dummy head with a </t>
     </r>
@@ -3416,6 +3513,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When </t>
     </r>
     <r>
@@ -3442,6 +3545,167 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/merge-two-sorted-lists/description/</t>
+  </si>
+  <si>
+    <t>Balanced Binary Tree</t>
+  </si>
+  <si>
+    <t>2025.2.25</t>
+  </si>
+  <si>
+    <t>Tree; DFS; Tree Traversal</t>
+  </si>
+  <si>
+    <t>Problem Pattern: This problem follows the "Tree Depth Calculation &amp; Height Checking" pattern. The key idea is to determine if the height difference between any two subtrees does not exceed 1.
+Solution Approach: Use postorder DFS traversal to compute subtree heights bottom-up, returning -1 if an imbalance is detected early. This runs in O(n) time complexity with O(h) space for recursion (O(log n) for balanced trees, O(n) worst case for skewed trees).
+Not Solved First Time
+How would you define the height of a tree:
+1. the max height of the left child and the right child
+2. if no children, then just 1
+bottom-up use postorder to check if subtree is balanced</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When checking whether a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>binary tree is balanced</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> (AVL tree condition).
+2. When </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>determining height constraints</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> in tree structures.
+3. When optimizing tree-based operations requiring balance (e.g., self-balancing BSTs).</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/balanced-binary-tree/description/</t>
+  </si>
+  <si>
+    <t>First Bad Version</t>
+  </si>
+  <si>
+    <r>
+      <t>Problem Pattern: This problem follows the "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Binary Search for First Occurrence</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>" pattern. The key idea is to efficiently find the first bad version by searching in a sorted sequence where isBadVersion(version) determines if a version is bad.
+Solution Approach: Use binary search to minimize API calls, narrowing the range by checking the middle version. Runs in O(log n) time complexity with O(1) space.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When searching for the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>first occurrence</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> of a condition </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>in a sorted list or a sequence</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+2. When optimizing API calls for large datasets (e.g., n = 2^31).
+3. When implementing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"lower bound" searches</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> (e.g., first failing test case, first threshold breach).</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/first-bad-version/description/</t>
   </si>
   <si>
     <t>Prompt</t>
@@ -3663,16 +3927,16 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -4206,22 +4470,22 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -4534,21 +4798,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="6.75" style="3" customWidth="1"/>
-    <col min="2" max="2" width="25.6333333333333" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.6296296296296" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.25" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.3583333333333" style="2" customWidth="1"/>
-    <col min="5" max="5" width="94.9" style="4" customWidth="1"/>
-    <col min="6" max="6" width="43.2583333333333" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.3" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.3611111111111" style="2" customWidth="1"/>
+    <col min="5" max="5" width="94.8981481481482" style="4" customWidth="1"/>
+    <col min="6" max="6" width="43.2592592592593" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.2962962962963" style="2" customWidth="1"/>
     <col min="8" max="8" width="32.6666666666667" style="4" customWidth="1"/>
     <col min="9" max="16384" width="9" style="4"/>
   </cols>
@@ -4579,7 +4843,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" ht="85.5" spans="1:8">
+    <row r="2" ht="96.6" spans="1:8">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -4659,7 +4923,7 @@
       <c r="G5" s="8"/>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" ht="85.5" spans="1:8">
+    <row r="6" ht="96.6" spans="1:8">
       <c r="A6" s="11">
         <v>733</v>
       </c>
@@ -4703,7 +4967,7 @@
       <c r="G7" s="8"/>
       <c r="H7" s="9"/>
     </row>
-    <row r="8" ht="85.5" spans="1:8">
+    <row r="8" ht="96.6" spans="1:8">
       <c r="A8" s="13">
         <v>235</v>
       </c>
@@ -4729,7 +4993,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" ht="85.5" spans="1:8">
+    <row r="9" ht="82.8" spans="1:8">
       <c r="A9" s="13">
         <v>226</v>
       </c>
@@ -4755,7 +5019,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" ht="27.6" spans="1:8">
       <c r="A10" s="10">
         <v>104</v>
       </c>
@@ -4773,11 +5037,11 @@
       <c r="G10" s="8"/>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" ht="27.6" spans="1:8">
       <c r="A11" s="10">
         <v>232</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="14" t="s">
         <v>45</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -4791,7 +5055,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="9"/>
     </row>
-    <row r="12" ht="99.75" spans="1:8">
+    <row r="12" ht="110.4" spans="1:8">
       <c r="A12" s="13">
         <v>20</v>
       </c>
@@ -4817,7 +5081,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" ht="27.6" spans="1:8">
       <c r="A13" s="10">
         <v>225</v>
       </c>
@@ -4835,11 +5099,11 @@
       <c r="G13" s="8"/>
       <c r="H13" s="9"/>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="10">
+    <row r="14" ht="96.6" spans="1:8">
+      <c r="A14" s="11">
         <v>141</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="15" t="s">
         <v>56</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -4848,20 +5112,28 @@
       <c r="D14" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9"/>
+      <c r="E14" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="10">
         <v>206</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>59</v>
+      <c r="B15" s="14" t="s">
+        <v>63</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>58</v>
@@ -4876,13 +5148,13 @@
         <v>54</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="8"/>
@@ -4894,69 +5166,69 @@
         <v>73</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="9"/>
     </row>
-    <row r="18" ht="85.5" spans="1:8">
-      <c r="A18" s="15">
+    <row r="18" ht="82.8" spans="1:8">
+      <c r="A18" s="13">
         <v>33</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" ht="99.75" spans="1:8">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" ht="110.4" spans="1:8">
       <c r="A19" s="13">
         <v>704</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -4964,13 +5236,13 @@
         <v>78</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="8"/>
@@ -4982,13 +5254,13 @@
         <v>77</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="8"/>
@@ -5000,418 +5272,418 @@
         <v>22</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C22" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>81</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="9"/>
     </row>
-    <row r="23" ht="99.75" spans="1:8">
+    <row r="23" ht="138" spans="1:8">
       <c r="A23" s="7">
         <v>121</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>16</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" ht="85.5" spans="1:8">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" ht="96.6" spans="1:8">
       <c r="A24" s="10">
         <v>208</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="H24" s="9"/>
     </row>
-    <row r="25" ht="114" spans="1:8">
+    <row r="25" ht="124.2" spans="1:8">
       <c r="A25" s="16">
         <v>238</v>
       </c>
-      <c r="B25" s="17" t="s">
-        <v>98</v>
+      <c r="B25" s="12" t="s">
+        <v>102</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" ht="99.75" spans="1:8">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" ht="96.6" spans="1:8">
       <c r="A26" s="11">
         <v>53</v>
       </c>
-      <c r="B26" s="17" t="s">
-        <v>104</v>
+      <c r="B26" s="12" t="s">
+        <v>108</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="27" ht="85.5" spans="1:8">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" ht="82.8" spans="1:8">
       <c r="A27" s="7">
         <v>217</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="28" ht="85.5" spans="1:8">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" ht="82.8" spans="1:8">
       <c r="A28" s="10">
         <v>56</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H28" s="9"/>
     </row>
-    <row r="29" ht="85.5" spans="1:8">
+    <row r="29" ht="110.4" spans="1:8">
       <c r="A29" s="11">
         <v>152</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="H29" s="9"/>
     </row>
-    <row r="30" ht="142.5" spans="1:8">
+    <row r="30" ht="153.6" spans="1:8">
       <c r="A30" s="11">
         <v>15</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="31" ht="128.25" spans="1:8">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" ht="124.2" spans="1:8">
       <c r="A31" s="11">
         <v>57</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="H31" s="9"/>
     </row>
-    <row r="32" ht="85.5" spans="1:8">
+    <row r="32" ht="96.6" spans="1:8">
       <c r="A32" s="11">
         <v>70</v>
       </c>
-      <c r="B32" s="8" t="s">
-        <v>136</v>
+      <c r="B32" s="14" t="s">
+        <v>140</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H32" s="9"/>
     </row>
-    <row r="33" ht="114" spans="1:8">
+    <row r="33" ht="124.2" spans="1:8">
       <c r="A33" s="11">
         <v>322</v>
       </c>
       <c r="B33" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>138</v>
-      </c>
       <c r="E33" s="8" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="H33" s="9"/>
     </row>
-    <row r="34" ht="156.75" spans="1:8">
+    <row r="34" ht="151.8" spans="1:8">
       <c r="A34" s="11">
         <v>11</v>
       </c>
       <c r="B34" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C34" s="9" t="s">
-        <v>143</v>
-      </c>
       <c r="D34" s="8" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="35" ht="199.5" spans="1:8">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" ht="193.2" spans="1:8">
       <c r="A35" s="11">
         <v>239</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="36" ht="185.25" spans="1:8">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" ht="179.4" spans="1:8">
       <c r="A36" s="7">
         <v>242</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="F36" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="H36" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="G36" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="37" ht="199.5" spans="1:8">
+    </row>
+    <row r="37" ht="193.2" spans="1:8">
       <c r="A37" s="10">
         <v>198</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="38" ht="99.75" spans="1:8">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" ht="110.4" spans="1:8">
       <c r="A38" s="11">
         <v>300</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="H38" s="9"/>
     </row>
@@ -5420,146 +5692,146 @@
         <v>371</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="H39" s="9"/>
     </row>
-    <row r="40" ht="128.25" spans="1:8">
+    <row r="40" ht="124.2" spans="1:8">
       <c r="A40" s="11">
         <v>191</v>
       </c>
       <c r="B40" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>177</v>
-      </c>
       <c r="E40" s="8" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="H40" s="9"/>
     </row>
-    <row r="41" ht="171" spans="1:8">
+    <row r="41" ht="179.4" spans="1:8">
       <c r="A41" s="7">
         <v>125</v>
       </c>
       <c r="B41" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="C41" s="9" t="s">
-        <v>182</v>
-      </c>
       <c r="D41" s="8" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="42" ht="85.5" spans="1:8">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="42" ht="96.6" spans="1:8">
       <c r="A42" s="11">
         <v>3</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="H42" s="9" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="43" ht="99.75" spans="1:8">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" ht="110.4" spans="1:8">
       <c r="A43" s="11">
         <v>50</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="H43" s="9"/>
     </row>
-    <row r="44" ht="85.5" spans="1:8">
+    <row r="44" ht="110.4" spans="1:8">
       <c r="A44" s="11">
         <v>69</v>
       </c>
       <c r="B44" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="C44" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>200</v>
-      </c>
       <c r="E44" s="8" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="H44" s="9"/>
     </row>
@@ -5568,48 +5840,48 @@
         <v>424</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="H45" s="9" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="46" ht="85.5" spans="1:8">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="46" ht="82.8" spans="1:8">
       <c r="A46" s="10">
         <v>836</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="H46" s="9"/>
     </row>
@@ -5618,59 +5890,59 @@
         <v>383</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="48" ht="85.5" spans="1:8">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="48" ht="82.8" spans="1:8">
       <c r="A48" s="7">
         <v>49</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="H48" s="9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="49" ht="85.5" spans="1:8">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="49" ht="82.8" spans="1:8">
       <c r="A49" s="16">
         <v>380</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>9</v>
@@ -5679,119 +5951,167 @@
         <v>10</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="50" ht="156.75" spans="1:8">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="50" ht="179.4" spans="1:8">
       <c r="A50" s="16">
         <v>41</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="H50" s="9" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="51" ht="156.75" spans="1:8">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="51" ht="151.8" spans="1:8">
       <c r="A51" s="11">
         <v>146</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="H51" s="9" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="52" ht="71.25" spans="1:8">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="52" ht="69" spans="1:8">
       <c r="A52" s="11">
         <v>432</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="F52" s="8"/>
       <c r="G52" s="8" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="H52" s="9" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="53" ht="85.5" spans="1:8">
-      <c r="A53" s="18">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="53" ht="82.8" spans="1:8">
+      <c r="A53" s="10">
         <v>21</v>
       </c>
-      <c r="B53" s="19" t="s">
-        <v>252</v>
-      </c>
-      <c r="C53" s="20" t="s">
+      <c r="B53" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="C53" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D53" s="19" t="s">
+      <c r="D53" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E53" s="19" t="s">
-        <v>253</v>
-      </c>
-      <c r="F53" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="G53" s="19" t="s">
-        <v>255</v>
-      </c>
-      <c r="H53" s="20" t="s">
+      <c r="E53" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="H53" s="9" t="s">
         <v>24</v>
       </c>
+    </row>
+    <row r="54" ht="138" spans="1:8">
+      <c r="A54" s="17">
+        <v>110</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="E54" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="F54" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="G54" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="H54" s="19"/>
+    </row>
+    <row r="55" ht="82.8" spans="1:8">
+      <c r="A55" s="20">
+        <v>278</v>
+      </c>
+      <c r="B55" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="C55" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E55" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="F55" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="G55" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="H55" s="19"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5812,19 +6132,19 @@
       <selection activeCell="D5" sqref="D5:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="195.125" customWidth="1"/>
+    <col min="1" max="1" width="195.12962962963" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" spans="1:1">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>256</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" ht="409" customHeight="1" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>257</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -5876,7 +6196,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
[LC] Update 2 question review and longest palindrome.
</commit_message>
<xml_diff>
--- a/Leetcode/Problem-tracker.xlsx
+++ b/Leetcode/Problem-tracker.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Must be reviewed every day" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="279">
   <si>
     <t>No.</t>
   </si>
@@ -303,10 +303,78 @@
     <t>Implement Queue using Stacks</t>
   </si>
   <si>
-    <t>2025.2.3</t>
+    <t>2025.2.26</t>
   </si>
   <si>
     <t>Stack</t>
+  </si>
+  <si>
+    <r>
+      <t>Problem Pattern: This problem follows the "Queue Simulation using Two Stacks" pattern. The key idea is to use two stacks (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>push_stack and pop_stack</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">) to simulate a queue’s FIFO (First-In-First-Out) behavior.
+Solution Approach: Push elements onto push_stack and transfer elements to pop_stack when needed to maintain order. Runs in O(1) for push, amortized O(1) for pop and peek, worst-case O(n).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Solved second time, but not the best solution</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When implementing a queue using only stack operations.
+2. When dealing with limited data structures in low-level programming.
+3. When </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>simulating FIFO behavior</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> using LIFO structures (stacks).</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/implement-queue-using-stacks/description/</t>
+  </si>
+  <si>
+    <t>2025.2.26; 2025.2.3</t>
   </si>
   <si>
     <t>Valid Parentheses</t>
@@ -405,13 +473,19 @@
     <t>Linked List Cycle</t>
   </si>
   <si>
-    <t>2025.1.31</t>
+    <t>2025.2.25</t>
   </si>
   <si>
     <t>Linked List</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Cycle Detection in Linked Lists" pattern. The key idea is to determine whether a linked list contains a cycle using a slow and fast pointer (Floyd’s Cycle Detection Algorithm).
 Solution Approach: Use two pointers (slow moves one step, fast moves two steps). If they ever meet, a cycle exists. Runs in O(n) time complexity with O(1) space.
 </t>
@@ -429,6 +503,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When </t>
     </r>
     <r>
@@ -1492,19 +1572,10 @@
     <t>Climbing Stairs</t>
   </si>
   <si>
-    <t>2025.2.15</t>
-  </si>
-  <si>
     <t>DP</t>
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Dynamic Programming - Fibonacci Sequence" pattern. The key is recognizing that the number of ways to reach step n is the sum of ways to reach n-1 and n-2 because you can climb 1 or 2 steps at a time.
 Solution Approach: Use a bottom-up dynamic programming (DP) approach to compute the number of ways iteratively. The optimized solution runs in O(n) time with O(1) space by storing only the last two computed values.
 </t>
@@ -1517,16 +1588,20 @@
         <rFont val="Cambria"/>
         <charset val="134"/>
       </rPr>
-      <t>Not solved first time, draw a decision tree helps a lot</t>
-    </r>
-  </si>
-  <si>
-    <t>1. When solving problems that follow the Fibonacci-like recurrence relation.
-2. When optimizing recursive backtracking using dynamic programming.
-3. When computing combinatorial step problems (e.g., number of paths in a grid).</t>
+      <t>Not solved first time, draw a decision tree helps a lot
+Not solved second</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Use this pattern when solving problems that require breaking down into smaller subproblems.
+2. Ideal for problems involving counting paths, sequences, or tiling.
+3. Scales to problems like "Jump Game," "House Robber," and "Decode Ways."</t>
   </si>
   <si>
     <t>https://leetcode.com/problems/climbing-stairs/description/</t>
+  </si>
+  <si>
+    <t>2025.2.26; 2025.2.15</t>
   </si>
   <si>
     <t>Coin Change</t>
@@ -3550,9 +3625,6 @@
     <t>Balanced Binary Tree</t>
   </si>
   <si>
-    <t>2025.2.25</t>
-  </si>
-  <si>
     <t>Tree; DFS; Tree Traversal</t>
   </si>
   <si>
@@ -3566,6 +3638,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When checking whether a </t>
     </r>
     <r>
@@ -3617,6 +3695,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t>Problem Pattern: This problem follows the "</t>
     </r>
     <r>
@@ -3642,6 +3726,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When searching for the </t>
     </r>
     <r>
@@ -3706,6 +3796,131 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/first-bad-version/description/</t>
+  </si>
+  <si>
+    <t>Longest Palindrome</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: The problem is about counting character frequencies and determining how they can form a palindrome. The key observation is that a palindrome can have at most one character with an odd frequency.
+Solution Approach: Use a hash set or dictionary to count the occurrences of each character. Add characters with even counts directly to the palindrome length. If a character </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>appears an odd number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> of times, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>add the largest even portion of it to the palindrome</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">, and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>reserve at most one odd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> character for the center.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Solved first time, but not most efficient a single odd number is only allowed to appera once, not matter where it comes from.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Use this pattern when determining the longest subsequence forming a specific structure (e.g., palindrome).
+2. Applies to problems where </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>character frequency</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>pairing rules</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> dictate the solution.
+3. Useful for string problems involving constraints on character arrangements.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-palindrome/description/</t>
   </si>
   <si>
     <t>Prompt</t>
@@ -3746,7 +3961,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3763,6 +3978,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Cambria"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
       <charset val="134"/>
@@ -3770,6 +3992,11 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Cambria"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Cambria"/>
       <charset val="134"/>
     </font>
@@ -3918,15 +4145,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -3939,8 +4157,17 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3949,13 +4176,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.8"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4293,140 +4526,158 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -4436,56 +4687,53 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -4798,1320 +5046,1354 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="6.75" style="3" customWidth="1"/>
-    <col min="2" max="2" width="25.6296296296296" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.3611111111111" style="2" customWidth="1"/>
-    <col min="5" max="5" width="94.8981481481482" style="4" customWidth="1"/>
-    <col min="6" max="6" width="43.2592592592593" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.2962962962963" style="2" customWidth="1"/>
-    <col min="8" max="8" width="32.6666666666667" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="4"/>
+    <col min="1" max="1" width="6.75" style="9" customWidth="1"/>
+    <col min="2" max="2" width="25.6296296296296" style="8" customWidth="1"/>
+    <col min="3" max="3" width="12.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.3611111111111" style="8" customWidth="1"/>
+    <col min="5" max="5" width="94.8981481481482" style="1" customWidth="1"/>
+    <col min="6" max="6" width="43.2592592592593" style="8" customWidth="1"/>
+    <col min="7" max="7" width="18.2962962962963" style="8" customWidth="1"/>
+    <col min="8" max="8" width="32.6666666666667" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="1" spans="1:8">
-      <c r="A1" s="5" t="s">
+    <row r="1" s="9" customFormat="1" spans="1:8">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" ht="96.6" spans="1:8">
-      <c r="A2" s="7">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="10">
+      <c r="A3" s="13">
         <v>973</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="10">
+      <c r="A4" s="13">
         <v>23</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="10">
+      <c r="A5" s="13">
         <v>542</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" ht="96.6" spans="1:8">
-      <c r="A6" s="11">
+      <c r="A6" s="14">
         <v>733</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="10">
+      <c r="A7" s="13">
         <v>200</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" ht="96.6" spans="1:8">
-      <c r="A8" s="13">
+      <c r="A8" s="16">
         <v>235</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="9" ht="82.8" spans="1:8">
-      <c r="A9" s="13">
+      <c r="A9" s="16">
         <v>226</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" ht="27.6" spans="1:8">
-      <c r="A10" s="10">
+      <c r="A10" s="13">
         <v>104</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="9"/>
-    </row>
-    <row r="11" ht="27.6" spans="1:8">
-      <c r="A11" s="10">
+      <c r="E10" s="4"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" ht="82.8" spans="1:8">
+      <c r="A11" s="14">
         <v>232</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9"/>
+      <c r="E11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="12" ht="110.4" spans="1:8">
-      <c r="A12" s="13">
+      <c r="A12" s="16">
         <v>20</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="9" t="s">
+      <c r="B12" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" ht="27.6" spans="1:8">
+      <c r="A13" s="13">
+        <v>225</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" ht="96.6" spans="1:8">
+      <c r="A14" s="14">
+        <v>141</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="13">
+        <v>206</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="13">
+        <v>54</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="13">
+        <v>73</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" ht="82.8" spans="1:8">
+      <c r="A18" s="16">
+        <v>33</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" ht="110.4" spans="1:8">
+      <c r="A19" s="16">
+        <v>704</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="13">
+        <v>78</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="13">
+        <v>77</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="13">
+        <v>22</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" ht="138" spans="1:8">
+      <c r="A23" s="12">
+        <v>121</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" ht="96.6" spans="1:8">
+      <c r="A24" s="13">
+        <v>208</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" ht="124.2" spans="1:8">
+      <c r="A25" s="19">
+        <v>238</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" ht="96.6" spans="1:8">
+      <c r="A26" s="20">
+        <v>53</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" ht="82.8" spans="1:8">
+      <c r="A27" s="12">
+        <v>217</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" ht="82.8" spans="1:8">
+      <c r="A28" s="13">
+        <v>56</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" ht="110.4" spans="1:8">
+      <c r="A29" s="20">
+        <v>152</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" ht="153.6" spans="1:8">
+      <c r="A30" s="20">
+        <v>15</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" ht="124.2" spans="1:8">
+      <c r="A31" s="20">
+        <v>57</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" ht="110.4" spans="1:8">
+      <c r="A32" s="21">
+        <v>70</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="33" ht="124.2" spans="1:8">
+      <c r="A33" s="20">
+        <v>322</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" ht="151.8" spans="1:8">
+      <c r="A34" s="20">
+        <v>11</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="35" ht="193.2" spans="1:8">
+      <c r="A35" s="20">
+        <v>239</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="36" ht="179.4" spans="1:8">
+      <c r="A36" s="12">
+        <v>242</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="37" ht="193.2" spans="1:8">
+      <c r="A37" s="13">
+        <v>198</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="38" ht="110.4" spans="1:8">
+      <c r="A38" s="20">
+        <v>300</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" ht="131" customHeight="1" spans="1:8">
+      <c r="A39" s="20">
+        <v>371</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" ht="124.2" spans="1:8">
+      <c r="A40" s="20">
+        <v>191</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" ht="179.4" spans="1:8">
+      <c r="A41" s="12">
+        <v>125</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42" ht="96.6" spans="1:8">
+      <c r="A42" s="20">
+        <v>3</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="43" ht="110.4" spans="1:8">
+      <c r="A43" s="20">
+        <v>50</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" ht="110.4" spans="1:8">
+      <c r="A44" s="20">
+        <v>69</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" ht="208" customHeight="1" spans="1:8">
+      <c r="A45" s="20">
+        <v>424</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="46" ht="82.8" spans="1:8">
+      <c r="A46" s="13">
+        <v>836</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" ht="156" customHeight="1" spans="1:8">
+      <c r="A47" s="12">
+        <v>383</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="48" ht="82.8" spans="1:8">
+      <c r="A48" s="12">
         <v>49</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" ht="27.6" spans="1:8">
-      <c r="A13" s="10">
-        <v>225</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9"/>
-    </row>
-    <row r="14" ht="96.6" spans="1:8">
-      <c r="A14" s="11">
-        <v>141</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G14" s="8" t="s">
+      <c r="B48" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="49" ht="82.8" spans="1:8">
+      <c r="A49" s="19">
+        <v>380</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="50" ht="179.4" spans="1:8">
+      <c r="A50" s="19">
+        <v>41</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="51" ht="151.8" spans="1:8">
+      <c r="A51" s="20">
+        <v>146</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="52" ht="69" spans="1:8">
+      <c r="A52" s="20">
+        <v>432</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="53" ht="82.8" spans="1:8">
+      <c r="A53" s="13">
+        <v>21</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" ht="138" spans="1:8">
+      <c r="A54" s="20">
+        <v>110</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="H14" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="10">
-        <v>206</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="10">
-        <v>54</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="10">
-        <v>73</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9"/>
-    </row>
-    <row r="18" ht="82.8" spans="1:8">
-      <c r="A18" s="13">
-        <v>33</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" ht="110.4" spans="1:8">
-      <c r="A19" s="13">
-        <v>704</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="G19" s="8" t="s">
+      <c r="D54" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" ht="82.8" spans="1:8">
+      <c r="A55" s="13">
+        <v>278</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D55" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="H19" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="10">
-        <v>78</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="9"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="10">
-        <v>77</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="9"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="10">
-        <v>22</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="9"/>
-    </row>
-    <row r="23" ht="138" spans="1:8">
-      <c r="A23" s="7">
-        <v>121</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" ht="96.6" spans="1:8">
-      <c r="A24" s="10">
-        <v>208</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="H24" s="9"/>
-    </row>
-    <row r="25" ht="124.2" spans="1:8">
-      <c r="A25" s="16">
-        <v>238</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="26" ht="96.6" spans="1:8">
-      <c r="A26" s="11">
-        <v>53</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="27" ht="82.8" spans="1:8">
-      <c r="A27" s="7">
-        <v>217</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" ht="82.8" spans="1:8">
-      <c r="A28" s="10">
-        <v>56</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="H28" s="9"/>
-    </row>
-    <row r="29" ht="110.4" spans="1:8">
-      <c r="A29" s="11">
-        <v>152</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="H29" s="9"/>
-    </row>
-    <row r="30" ht="153.6" spans="1:8">
-      <c r="A30" s="11">
-        <v>15</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="31" ht="124.2" spans="1:8">
-      <c r="A31" s="11">
-        <v>57</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="H31" s="9"/>
-    </row>
-    <row r="32" ht="96.6" spans="1:8">
-      <c r="A32" s="11">
-        <v>70</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="H32" s="9"/>
-    </row>
-    <row r="33" ht="124.2" spans="1:8">
-      <c r="A33" s="11">
-        <v>322</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="H33" s="9"/>
-    </row>
-    <row r="34" ht="151.8" spans="1:8">
-      <c r="A34" s="11">
-        <v>11</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="35" ht="193.2" spans="1:8">
-      <c r="A35" s="11">
-        <v>239</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="36" ht="179.4" spans="1:8">
-      <c r="A36" s="7">
-        <v>242</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="37" ht="193.2" spans="1:8">
-      <c r="A37" s="10">
-        <v>198</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="38" ht="110.4" spans="1:8">
-      <c r="A38" s="11">
-        <v>300</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="H38" s="9"/>
-    </row>
-    <row r="39" ht="131" customHeight="1" spans="1:8">
-      <c r="A39" s="11">
-        <v>371</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="G39" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="H39" s="9"/>
-    </row>
-    <row r="40" ht="124.2" spans="1:8">
-      <c r="A40" s="11">
-        <v>191</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="G40" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="H40" s="9"/>
-    </row>
-    <row r="41" ht="179.4" spans="1:8">
-      <c r="A41" s="7">
-        <v>125</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="H41" s="9" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="42" ht="96.6" spans="1:8">
-      <c r="A42" s="11">
-        <v>3</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="G42" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="43" ht="110.4" spans="1:8">
-      <c r="A43" s="11">
-        <v>50</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="G43" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="H43" s="9"/>
-    </row>
-    <row r="44" ht="110.4" spans="1:8">
-      <c r="A44" s="11">
-        <v>69</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="G44" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="H44" s="9"/>
-    </row>
-    <row r="45" ht="208" customHeight="1" spans="1:8">
-      <c r="A45" s="11">
-        <v>424</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="G45" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="H45" s="9" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="46" ht="82.8" spans="1:8">
-      <c r="A46" s="10">
-        <v>836</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="G46" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="H46" s="9"/>
-    </row>
-    <row r="47" ht="156" customHeight="1" spans="1:8">
-      <c r="A47" s="7">
-        <v>383</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="G47" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="H47" s="9" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="48" ht="82.8" spans="1:8">
-      <c r="A48" s="7">
-        <v>49</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="G48" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="H48" s="9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="49" ht="82.8" spans="1:8">
-      <c r="A49" s="16">
-        <v>380</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D49" s="8" t="s">
+      <c r="E55" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="H55" s="4"/>
+    </row>
+    <row r="56" ht="110.4" spans="1:8">
+      <c r="A56" s="23">
+        <v>409</v>
+      </c>
+      <c r="B56" s="24" t="s">
+        <v>273</v>
+      </c>
+      <c r="C56" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D56" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E49" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="G49" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="H49" s="9" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="50" ht="179.4" spans="1:8">
-      <c r="A50" s="16">
-        <v>41</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="E50" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="G50" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="H50" s="9" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="51" ht="151.8" spans="1:8">
-      <c r="A51" s="11">
-        <v>146</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="G51" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="H51" s="9" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="52" ht="69" spans="1:8">
-      <c r="A52" s="11">
-        <v>432</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>253</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="H52" s="9" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="53" ht="82.8" spans="1:8">
-      <c r="A53" s="10">
-        <v>21</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="G53" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="H53" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="54" ht="138" spans="1:8">
-      <c r="A54" s="17">
-        <v>110</v>
-      </c>
-      <c r="B54" s="18" t="s">
-        <v>260</v>
-      </c>
-      <c r="C54" s="19" t="s">
-        <v>261</v>
-      </c>
-      <c r="D54" s="18" t="s">
-        <v>262</v>
-      </c>
-      <c r="E54" s="18" t="s">
-        <v>263</v>
-      </c>
-      <c r="F54" s="18" t="s">
-        <v>264</v>
-      </c>
-      <c r="G54" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="H54" s="19"/>
-    </row>
-    <row r="55" ht="82.8" spans="1:8">
-      <c r="A55" s="20">
-        <v>278</v>
-      </c>
-      <c r="B55" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="C55" s="19" t="s">
-        <v>261</v>
-      </c>
-      <c r="D55" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E55" s="18" t="s">
-        <v>267</v>
-      </c>
-      <c r="F55" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="G55" s="18" t="s">
-        <v>269</v>
-      </c>
-      <c r="H55" s="19"/>
+      <c r="E56" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="F56" s="24" t="s">
+        <v>275</v>
+      </c>
+      <c r="G56" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="H56" s="25"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6128,8 +6410,8 @@
   <sheetPr/>
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D6"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -6138,44 +6420,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>270</v>
+      <c r="A1" s="7" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="2" ht="409" customHeight="1" spans="1:1">
-      <c r="A2" s="2" t="s">
-        <v>271</v>
+      <c r="A2" s="8" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="2"/>
+      <c r="A3" s="8"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="2"/>
+      <c r="A4" s="8"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="2"/>
+      <c r="A5" s="8"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="2"/>
+      <c r="A6" s="8"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="2"/>
+      <c r="A7" s="8"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="2"/>
+      <c r="A8" s="8"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="2"/>
+      <c r="A9" s="8"/>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="2"/>
+      <c r="A10" s="8"/>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="2"/>
+      <c r="A11" s="8"/>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="2"/>
+      <c r="A12" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6190,14 +6472,99 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="7"/>
+  <cols>
+    <col min="2" max="2" width="24.1111111111111" customWidth="1"/>
+    <col min="5" max="5" width="63.4444444444444" customWidth="1"/>
+    <col min="6" max="6" width="38" customWidth="1"/>
+    <col min="8" max="8" width="30.2222222222222" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="141" customHeight="1" spans="1:8">
+      <c r="A1" s="2">
+        <v>70</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="124.2" spans="1:8">
+      <c r="A2" s="2">
+        <v>733</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="110.4" spans="1:8">
+      <c r="A3" s="2">
+        <v>141</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>

<commit_message>
[LC] Update question review and Majority Element.
</commit_message>
<xml_diff>
--- a/Leetcode/Problem-tracker.xlsx
+++ b/Leetcode/Problem-tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9767"/>
+    <workbookView windowWidth="27945" windowHeight="12960" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="291">
   <si>
     <t>No.</t>
   </si>
@@ -310,6 +310,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t>Problem Pattern: This problem follows the "Queue Simulation using Two Stacks" pattern. The key idea is to use two stacks (</t>
     </r>
     <r>
@@ -346,6 +352,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When implementing a queue using only stack operations.
 2. When dealing with limited data structures in low-level programming.
 3. When </t>
@@ -543,7 +555,35 @@
     <t>Reverse Linked List</t>
   </si>
   <si>
-    <t>2025.1.30</t>
+    <t>2025.2.27</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: Given a singly linked list, reverse it in-place. The problem can be solved using an iterative approach with two pointers or a recursive approach.
+Solution Approach: Use a two-pointer approach (prev and cur) to reverse pointers one by one until reaching the end of the list. Alternatively, recursion can be used to reverse the list by going to the last node and rebuilding the list in reverse order.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Not solved second time, write down the entire process rather than assumption!!!!!</t>
+    </r>
+  </si>
+  <si>
+    <t>1. When needing to reverse a linked list in-place.
+2. Useful when traversing and modifying a linked list efficiently.
+3. Scales to problems like "Reverse Nodes in k-Group" and "Reorder List".</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-linked-list/description/</t>
+  </si>
+  <si>
+    <t>2025.2.27; 2025.1.31</t>
   </si>
   <si>
     <t>Spiral Matrix</t>
@@ -1576,6 +1616,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Dynamic Programming - Fibonacci Sequence" pattern. The key is recognizing that the number of ways to reach step n is the sum of ways to reach n-1 and n-2 because you can climb 1 or 2 steps at a time.
 Solution Approach: Use a bottom-up dynamic programming (DP) approach to compute the number of ways iteratively. The optimized solution runs in O(n) time with O(1) space by storing only the last two computed values.
 </t>
@@ -3802,6 +3848,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: The problem is about counting character frequencies and determining how they can form a palindrome. The key observation is that a palindrome can have at most one character with an odd frequency.
 Solution Approach: Use a hash set or dictionary to count the occurrences of each character. Add characters with even counts directly to the palindrome length. If a character </t>
     </r>
@@ -3876,6 +3928,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. Use this pattern when determining the longest subsequence forming a specific structure (e.g., palindrome).
 2. Applies to problems where </t>
     </r>
@@ -3921,6 +3979,147 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/longest-palindrome/description/</t>
+  </si>
+  <si>
+    <t>Majority Element</t>
+  </si>
+  <si>
+    <t>Array, Hash table, Vote</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Problem Pattern: The problem requires finding an element that appears more than ⌊n/2⌋ times in an array, meaning it must occupy the majority of positions.
+Solution Approach: Use the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Boyer-Moore Voting Algorithm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>, which efficiently finds the majority element in O(n) time and O(1) space. The algorithm maintains a counter that increases when encountering the current candidate and decreases when encountering a different element.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+Solved first time but not most space efficient
+The algorithm maintains a candidate and a count variable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">1. Use this pattern when finding a majority element with a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>guaranteed majority</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> (appearing more than n/2 times).
+2. Scales to problems involving </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>voting or element dominance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> in sequences.
+3. Similar patterns appear in "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Find All Duplicates</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> in an Array" and "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Top K Frequent Elements</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>."</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/majority-element/description/</t>
   </si>
   <si>
     <t>Prompt</t>
@@ -3949,6 +4148,15 @@
 ```python
 {Optimized Python code solution}
 Provide a structured solution for LeetCode 191: Number of 1 Bits, using the exact format specified above</t>
+  </si>
+  <si>
+    <t>2025.2.27; 2025.2.26; 2025.2.15</t>
+  </si>
+  <si>
+    <t>2025.2.27; 2025.2.24; 2025.2.8</t>
+  </si>
+  <si>
+    <t>2025.2.27; 2025.2.25; 2025.1.31</t>
   </si>
 </sst>
 </file>
@@ -3983,6 +4191,20 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Cambria"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -3991,22 +4213,8 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
       <name val="Cambria"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Cambria"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -4152,12 +4360,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <i/>
       <u/>
@@ -4166,8 +4368,14 @@
       <name val="Cambria"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4182,19 +4390,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4526,13 +4722,13 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4556,16 +4752,16 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -4574,89 +4770,89 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4675,7 +4871,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -4687,16 +4889,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4711,29 +4913,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -5046,53 +5236,53 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="6.75" style="9" customWidth="1"/>
-    <col min="2" max="2" width="25.6296296296296" style="8" customWidth="1"/>
+    <col min="1" max="1" width="6.75" style="11" customWidth="1"/>
+    <col min="2" max="2" width="25.6333333333333" style="10" customWidth="1"/>
     <col min="3" max="3" width="12.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3611111111111" style="8" customWidth="1"/>
-    <col min="5" max="5" width="94.8981481481482" style="1" customWidth="1"/>
-    <col min="6" max="6" width="43.2592592592593" style="8" customWidth="1"/>
-    <col min="7" max="7" width="18.2962962962963" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.3583333333333" style="10" customWidth="1"/>
+    <col min="5" max="5" width="94.9" style="1" customWidth="1"/>
+    <col min="6" max="6" width="43.2583333333333" style="10" customWidth="1"/>
+    <col min="7" max="7" width="18.3" style="10" customWidth="1"/>
     <col min="8" max="8" width="32.6666666666667" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="1" spans="1:8">
-      <c r="A1" s="10" t="s">
+    <row r="1" s="11" customFormat="1" spans="1:8">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" ht="96.6" spans="1:8">
-      <c r="A2" s="12">
+    <row r="2" ht="85.5" spans="1:8">
+      <c r="A2" s="14">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -5118,7 +5308,7 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="13">
+      <c r="A3" s="15">
         <v>973</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -5136,7 +5326,7 @@
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="13">
+      <c r="A4" s="15">
         <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -5154,7 +5344,7 @@
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="13">
+      <c r="A5" s="15">
         <v>542</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -5171,11 +5361,11 @@
       <c r="G5" s="5"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" ht="96.6" spans="1:8">
-      <c r="A6" s="14">
+    <row r="6" ht="85.5" spans="1:8">
+      <c r="A6" s="16">
         <v>733</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="17" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -5198,7 +5388,7 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="13">
+      <c r="A7" s="15">
         <v>200</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -5215,11 +5405,11 @@
       <c r="G7" s="5"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" ht="96.6" spans="1:8">
+    <row r="8" ht="85.5" spans="1:8">
       <c r="A8" s="16">
         <v>235</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="17" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -5241,11 +5431,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" ht="82.8" spans="1:8">
+    <row r="9" ht="85.5" spans="1:8">
       <c r="A9" s="16">
         <v>226</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="17" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -5267,8 +5457,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" ht="27.6" spans="1:8">
-      <c r="A10" s="13">
+    <row r="10" spans="1:8">
+      <c r="A10" s="15">
         <v>104</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -5285,8 +5475,8 @@
       <c r="G10" s="5"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" ht="82.8" spans="1:8">
-      <c r="A11" s="14">
+    <row r="11" ht="85.5" spans="1:8">
+      <c r="A11" s="16">
         <v>232</v>
       </c>
       <c r="B11" s="17" t="s">
@@ -5311,11 +5501,11 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" ht="110.4" spans="1:8">
+    <row r="12" ht="99.75" spans="1:8">
       <c r="A12" s="16">
         <v>20</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="17" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -5337,8 +5527,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" ht="27.6" spans="1:8">
-      <c r="A13" s="13">
+    <row r="13" spans="1:8">
+      <c r="A13" s="15">
         <v>225</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -5355,11 +5545,11 @@
       <c r="G13" s="5"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" ht="96.6" spans="1:8">
-      <c r="A14" s="14">
+    <row r="14" ht="71.25" spans="1:8">
+      <c r="A14" s="16">
         <v>141</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="17" t="s">
         <v>60</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -5381,11 +5571,11 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="13">
+    <row r="15" ht="85.5" spans="1:8">
+      <c r="A15" s="18">
         <v>206</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="19" t="s">
         <v>67</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -5394,23 +5584,31 @@
       <c r="D15" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="4"/>
+      <c r="E15" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="13">
+      <c r="A16" s="15">
         <v>54</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="5"/>
@@ -5418,87 +5616,87 @@
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="13">
+      <c r="A17" s="15">
         <v>73</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" ht="82.8" spans="1:8">
+    <row r="18" ht="85.5" spans="1:8">
       <c r="A18" s="16">
         <v>33</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" ht="110.4" spans="1:8">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" ht="99.75" spans="1:8">
       <c r="A19" s="16">
         <v>704</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>81</v>
+      <c r="B19" s="17" t="s">
+        <v>85</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="13">
+      <c r="A20" s="15">
         <v>78</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="5"/>
@@ -5506,17 +5704,17 @@
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="13">
+      <c r="A21" s="15">
         <v>77</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="5"/>
@@ -5524,683 +5722,683 @@
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="13">
+      <c r="A22" s="15">
         <v>22</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" ht="138" spans="1:8">
-      <c r="A23" s="12">
+    <row r="23" ht="99.75" spans="1:8">
+      <c r="A23" s="14">
         <v>121</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="H23" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" ht="85.5" spans="1:8">
+      <c r="A24" s="15">
+        <v>208</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" ht="114" spans="1:8">
+      <c r="A25" s="20">
+        <v>238</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" ht="99.75" spans="1:8">
+      <c r="A26" s="21">
+        <v>53</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="24" ht="96.6" spans="1:8">
-      <c r="A24" s="13">
-        <v>208</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="G24" s="5" t="s">
+      <c r="E26" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" ht="85.5" spans="1:8">
+      <c r="A27" s="14">
+        <v>217</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" ht="124.2" spans="1:8">
-      <c r="A25" s="19">
-        <v>238</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" ht="96.6" spans="1:8">
-      <c r="A26" s="20">
-        <v>53</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="27" ht="82.8" spans="1:8">
-      <c r="A27" s="12">
-        <v>217</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="D27" s="5" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="28" ht="82.8" spans="1:8">
-      <c r="A28" s="13">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" ht="85.5" spans="1:8">
+      <c r="A28" s="15">
         <v>56</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" ht="110.4" spans="1:8">
-      <c r="A29" s="20">
+    <row r="29" ht="85.5" spans="1:8">
+      <c r="A29" s="21">
         <v>152</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" ht="153.6" spans="1:8">
-      <c r="A30" s="20">
+    <row r="30" ht="142.5" spans="1:8">
+      <c r="A30" s="21">
         <v>15</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="31" ht="124.2" spans="1:8">
-      <c r="A31" s="20">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" ht="128.25" spans="1:8">
+      <c r="A31" s="21">
         <v>57</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" ht="110.4" spans="1:8">
-      <c r="A32" s="21">
+    <row r="32" ht="99.75" spans="1:8">
+      <c r="A32" s="22">
         <v>70</v>
       </c>
-      <c r="B32" s="22" t="s">
-        <v>144</v>
+      <c r="B32" s="23" t="s">
+        <v>148</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H32" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" ht="114" spans="1:8">
+      <c r="A33" s="21">
+        <v>322</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="33" ht="124.2" spans="1:8">
-      <c r="A33" s="20">
-        <v>322</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>145</v>
-      </c>
       <c r="E33" s="5" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" ht="151.8" spans="1:8">
-      <c r="A34" s="20">
+    <row r="34" ht="156.75" spans="1:8">
+      <c r="A34" s="21">
         <v>11</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>151</v>
-      </c>
       <c r="D34" s="5" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="35" ht="193.2" spans="1:8">
-      <c r="A35" s="20">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" ht="199.5" spans="1:8">
+      <c r="A35" s="21">
         <v>239</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="36" ht="179.4" spans="1:8">
-      <c r="A36" s="12">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="36" ht="185.25" spans="1:8">
+      <c r="A36" s="14">
         <v>242</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="F36" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="H36" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="G36" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="37" ht="193.2" spans="1:8">
-      <c r="A37" s="13">
+    </row>
+    <row r="37" ht="199.5" spans="1:8">
+      <c r="A37" s="15">
         <v>198</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="38" ht="110.4" spans="1:8">
-      <c r="A38" s="20">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="38" ht="99.75" spans="1:8">
+      <c r="A38" s="21">
         <v>300</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="H38" s="4"/>
     </row>
     <row r="39" ht="131" customHeight="1" spans="1:8">
-      <c r="A39" s="20">
+      <c r="A39" s="21">
         <v>371</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" ht="124.2" spans="1:8">
-      <c r="A40" s="20">
+    <row r="40" ht="128.25" spans="1:8">
+      <c r="A40" s="21">
         <v>191</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>185</v>
-      </c>
       <c r="E40" s="5" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" ht="179.4" spans="1:8">
-      <c r="A41" s="12">
+    <row r="41" ht="171" spans="1:8">
+      <c r="A41" s="14">
         <v>125</v>
       </c>
       <c r="B41" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>190</v>
-      </c>
       <c r="D41" s="5" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="42" ht="96.6" spans="1:8">
-      <c r="A42" s="20">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="42" ht="85.5" spans="1:8">
+      <c r="A42" s="21">
         <v>3</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="43" ht="110.4" spans="1:8">
-      <c r="A43" s="20">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="43" ht="99.75" spans="1:8">
+      <c r="A43" s="21">
         <v>50</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="G43" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" ht="85.5" spans="1:8">
+      <c r="A44" s="21">
+        <v>69</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="H43" s="4"/>
-    </row>
-    <row r="44" ht="110.4" spans="1:8">
-      <c r="A44" s="20">
-        <v>69</v>
-      </c>
-      <c r="B44" s="5" t="s">
+      <c r="D44" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>208</v>
-      </c>
       <c r="E44" s="5" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="H44" s="4"/>
     </row>
     <row r="45" ht="208" customHeight="1" spans="1:8">
-      <c r="A45" s="20">
+      <c r="A45" s="21">
         <v>424</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="46" ht="82.8" spans="1:8">
-      <c r="A46" s="13">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="46" ht="85.5" spans="1:8">
+      <c r="A46" s="15">
         <v>836</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="H46" s="4"/>
     </row>
     <row r="47" ht="156" customHeight="1" spans="1:8">
-      <c r="A47" s="12">
+      <c r="A47" s="14">
         <v>383</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="48" ht="82.8" spans="1:8">
-      <c r="A48" s="12">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="48" ht="85.5" spans="1:8">
+      <c r="A48" s="14">
         <v>49</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="49" ht="82.8" spans="1:8">
-      <c r="A49" s="19">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="49" ht="85.5" spans="1:8">
+      <c r="A49" s="20">
         <v>380</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>9</v>
@@ -6209,100 +6407,100 @@
         <v>10</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="50" ht="179.4" spans="1:8">
-      <c r="A50" s="19">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="50" ht="156.75" spans="1:8">
+      <c r="A50" s="20">
         <v>41</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="51" ht="151.8" spans="1:8">
-      <c r="A51" s="20">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="51" ht="156.75" spans="1:8">
+      <c r="A51" s="21">
         <v>146</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="G51" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="52" ht="71.25" spans="1:8">
+      <c r="A52" s="21">
+        <v>432</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="H51" s="4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="52" ht="69" spans="1:8">
-      <c r="A52" s="20">
-        <v>432</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>251</v>
-      </c>
       <c r="D52" s="5" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="F52" s="5"/>
       <c r="G52" s="5" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="53" ht="82.8" spans="1:8">
-      <c r="A53" s="13">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="53" ht="85.5" spans="1:8">
+      <c r="A53" s="15">
         <v>21</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>24</v>
@@ -6311,89 +6509,113 @@
         <v>62</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="54" ht="138" spans="1:8">
-      <c r="A54" s="20">
+    <row r="54" ht="142.5" spans="1:8">
+      <c r="A54" s="21">
         <v>110</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="H54" s="4"/>
     </row>
-    <row r="55" ht="82.8" spans="1:8">
-      <c r="A55" s="13">
+    <row r="55" ht="85.5" spans="1:8">
+      <c r="A55" s="15">
         <v>278</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="H55" s="4"/>
     </row>
-    <row r="56" ht="110.4" spans="1:8">
-      <c r="A56" s="23">
+    <row r="56" ht="99.75" spans="1:8">
+      <c r="A56" s="15">
         <v>409</v>
       </c>
-      <c r="B56" s="24" t="s">
-        <v>273</v>
-      </c>
-      <c r="C56" s="25" t="s">
+      <c r="B56" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D56" s="24" t="s">
+      <c r="D56" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E56" s="24" t="s">
-        <v>274</v>
-      </c>
-      <c r="F56" s="24" t="s">
-        <v>275</v>
-      </c>
-      <c r="G56" s="24" t="s">
-        <v>276</v>
-      </c>
-      <c r="H56" s="25"/>
+      <c r="E56" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="H56" s="4"/>
+    </row>
+    <row r="57" ht="99.75" spans="1:8">
+      <c r="A57" s="21">
+        <v>169</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="H57" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6414,50 +6636,50 @@
       <selection activeCell="A2" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="195.12962962963" customWidth="1"/>
+    <col min="1" max="1" width="195.133333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="7" t="s">
-        <v>277</v>
+    <row r="1" ht="14.25" spans="1:1">
+      <c r="A1" s="9" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="2" ht="409" customHeight="1" spans="1:1">
-      <c r="A2" s="8" t="s">
-        <v>278</v>
+      <c r="A2" s="10" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="8"/>
+      <c r="A3" s="10"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="8"/>
+      <c r="A4" s="10"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="8"/>
+      <c r="A5" s="10"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="8"/>
+      <c r="A6" s="10"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="8"/>
+      <c r="A7" s="10"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="8"/>
+      <c r="A8" s="10"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="8"/>
+      <c r="A9" s="10"/>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="8"/>
+      <c r="A10" s="10"/>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="8"/>
+      <c r="A11" s="10"/>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="8"/>
+      <c r="A12" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6472,18 +6694,18 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="24.1111111111111" customWidth="1"/>
-    <col min="5" max="5" width="63.4444444444444" customWidth="1"/>
+    <col min="2" max="2" width="24.1083333333333" customWidth="1"/>
+    <col min="5" max="5" width="63.4416666666667" customWidth="1"/>
     <col min="6" max="6" width="38" customWidth="1"/>
-    <col min="8" max="8" width="30.2222222222222" customWidth="1"/>
+    <col min="8" max="8" width="30.225" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="141" customHeight="1" spans="1:8">
@@ -6491,28 +6713,28 @@
         <v>70</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>148</v>
+        <v>151</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>152</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" s="1" customFormat="1" ht="124.2" spans="1:8">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="114" spans="1:8">
       <c r="A2" s="2">
         <v>733</v>
       </c>
@@ -6520,7 +6742,7 @@
         <v>23</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>25</v>
@@ -6531,22 +6753,22 @@
       <c r="F2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="6" t="s">
         <v>28</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" s="1" customFormat="1" ht="110.4" spans="1:8">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="121.5" spans="1:8">
       <c r="A3" s="2">
         <v>141</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>62</v>
@@ -6557,14 +6779,45 @@
       <c r="F3" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="6" t="s">
         <v>65</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>66</v>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="114" spans="1:8">
+      <c r="A4" s="7">
+        <v>206</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G1" r:id="rId1" display="https://leetcode.com/problems/climbing-stairs/description/"/>
+    <hyperlink ref="G2" r:id="rId2" display="https://leetcode.com/problems/flood-fill/description/"/>
+    <hyperlink ref="G3" r:id="rId3" display="https://leetcode.com/problems/linked-list-cycle/description/"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>

<commit_message>
[LC] Update binary addition and question review.
</commit_message>
<xml_diff>
--- a/Leetcode/Problem-tracker.xlsx
+++ b/Leetcode/Problem-tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12960" activeTab="2"/>
+    <workbookView windowWidth="27945" windowHeight="12960"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="297">
   <si>
     <t>No.</t>
   </si>
@@ -559,6 +559,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: Given a singly linked list, reverse it in-place. The problem can be solved using an iterative approach with two pointers or a recursive approach.
 Solution Approach: Use a two-pointer approach (prev and cur) to reverse pointers one by one until reaching the end of the list. Alternatively, recursion can be used to reverse the list by going to the last node and rebuilding the list in reverse order.
 </t>
@@ -4120,6 +4126,105 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/majority-element/description/</t>
+  </si>
+  <si>
+    <t>Add Binary</t>
+  </si>
+  <si>
+    <t>2025.3.1</t>
+  </si>
+  <si>
+    <r>
+      <t>Problem Pattern: This problem follows the "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Binary Addition</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> using Bit Manipulation or String Manipulation" pattern. The key idea is to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>simulate binary addition</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">, handling carry propagation manually as in elementary arithmetic.
+Solution Approach: Traverse both binary strings right to left, summing corresponding digits and carrying over values. Runs in O(max(n, m)) time complexity with O(max(n, m)) space.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Not Solved first time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+Think about addition in ten
+Built-in alternative: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>int(a, 2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> - Convert Binary String to Integer. bin(21) convert sum to binary. [2:] removes prefix</t>
+    </r>
+  </si>
+  <si>
+    <t>1. When performing binary arithmetic without built-in conversion.
+2. When handling binary numbers as strings due to constraints.
+3. When implementing bitwise operations on large numbers efficiently.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/add-binary/description/</t>
   </si>
   <si>
     <t>Prompt</t>
@@ -4150,13 +4255,16 @@
 Provide a structured solution for LeetCode 191: Number of 1 Bits, using the exact format specified above</t>
   </si>
   <si>
-    <t>2025.2.27; 2025.2.26; 2025.2.15</t>
-  </si>
-  <si>
-    <t>2025.2.27; 2025.2.24; 2025.2.8</t>
-  </si>
-  <si>
-    <t>2025.2.27; 2025.2.25; 2025.1.31</t>
+    <t>20255.3.1; 2025.2.28; 2025.2.27; 2025.2.26; 2025.2.15</t>
+  </si>
+  <si>
+    <t>2025.3.1; 2025.2.27; 2025.2.24; 2025.2.8</t>
+  </si>
+  <si>
+    <t>2025.3.1; 2025.2.27; 2025.2.25; 2025.1.31</t>
+  </si>
+  <si>
+    <t>2025.3.1; 2025.2.27; 2025.1.31</t>
   </si>
 </sst>
 </file>
@@ -4169,7 +4277,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4186,6 +4294,26 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Cambria"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Cambria"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Cambria"/>
       <charset val="134"/>
@@ -4199,12 +4327,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Cambria"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -4215,14 +4337,6 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4353,6 +4467,8 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <i/>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -4360,8 +4476,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <i/>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -4722,147 +4836,147 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4871,7 +4985,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4880,6 +4994,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -4889,10 +5012,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4907,23 +5030,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -5236,53 +5362,53 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="6.75" style="11" customWidth="1"/>
-    <col min="2" max="2" width="25.6333333333333" style="10" customWidth="1"/>
+    <col min="1" max="1" width="6.75" style="14" customWidth="1"/>
+    <col min="2" max="2" width="25.6333333333333" style="13" customWidth="1"/>
     <col min="3" max="3" width="12.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3583333333333" style="10" customWidth="1"/>
+    <col min="4" max="4" width="11.3583333333333" style="13" customWidth="1"/>
     <col min="5" max="5" width="94.9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="43.2583333333333" style="10" customWidth="1"/>
-    <col min="7" max="7" width="18.3" style="10" customWidth="1"/>
+    <col min="6" max="6" width="43.2583333333333" style="13" customWidth="1"/>
+    <col min="7" max="7" width="18.3" style="13" customWidth="1"/>
     <col min="8" max="8" width="32.6666666666667" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="1" spans="1:8">
-      <c r="A1" s="12" t="s">
+    <row r="1" s="14" customFormat="1" spans="1:8">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" ht="85.5" spans="1:8">
-      <c r="A2" s="14">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -5308,7 +5434,7 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="15">
+      <c r="A3" s="18">
         <v>973</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -5326,7 +5452,7 @@
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="15">
+      <c r="A4" s="18">
         <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -5344,7 +5470,7 @@
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="15">
+      <c r="A5" s="18">
         <v>542</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -5362,10 +5488,10 @@
       <c r="H5" s="4"/>
     </row>
     <row r="6" ht="85.5" spans="1:8">
-      <c r="A6" s="16">
+      <c r="A6" s="19">
         <v>733</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="20" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -5388,7 +5514,7 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="15">
+      <c r="A7" s="18">
         <v>200</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -5406,10 +5532,10 @@
       <c r="H7" s="4"/>
     </row>
     <row r="8" ht="85.5" spans="1:8">
-      <c r="A8" s="16">
+      <c r="A8" s="19">
         <v>235</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="20" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -5432,10 +5558,10 @@
       </c>
     </row>
     <row r="9" ht="85.5" spans="1:8">
-      <c r="A9" s="16">
+      <c r="A9" s="19">
         <v>226</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="20" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -5458,7 +5584,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="15">
+      <c r="A10" s="18">
         <v>104</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -5476,10 +5602,10 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" ht="85.5" spans="1:8">
-      <c r="A11" s="16">
+      <c r="A11" s="19">
         <v>232</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="20" t="s">
         <v>45</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -5502,10 +5628,10 @@
       </c>
     </row>
     <row r="12" ht="99.75" spans="1:8">
-      <c r="A12" s="16">
+      <c r="A12" s="19">
         <v>20</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="20" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -5528,7 +5654,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="15">
+      <c r="A13" s="18">
         <v>225</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -5546,10 +5672,10 @@
       <c r="H13" s="4"/>
     </row>
     <row r="14" ht="71.25" spans="1:8">
-      <c r="A14" s="16">
+      <c r="A14" s="19">
         <v>141</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="20" t="s">
         <v>60</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -5572,10 +5698,10 @@
       </c>
     </row>
     <row r="15" ht="85.5" spans="1:8">
-      <c r="A15" s="18">
+      <c r="A15" s="19">
         <v>206</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="20" t="s">
         <v>67</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -5598,7 +5724,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="15">
+      <c r="A16" s="18">
         <v>54</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -5616,7 +5742,7 @@
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="15">
+      <c r="A17" s="18">
         <v>73</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -5634,7 +5760,7 @@
       <c r="H17" s="4"/>
     </row>
     <row r="18" ht="85.5" spans="1:8">
-      <c r="A18" s="16">
+      <c r="A18" s="19">
         <v>33</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -5660,10 +5786,10 @@
       </c>
     </row>
     <row r="19" ht="99.75" spans="1:8">
-      <c r="A19" s="16">
+      <c r="A19" s="19">
         <v>704</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="20" t="s">
         <v>85</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -5686,7 +5812,7 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="15">
+      <c r="A20" s="18">
         <v>78</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -5704,7 +5830,7 @@
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="15">
+      <c r="A21" s="18">
         <v>77</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -5722,7 +5848,7 @@
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="15">
+      <c r="A22" s="18">
         <v>22</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -5740,7 +5866,7 @@
       <c r="H22" s="4"/>
     </row>
     <row r="23" ht="99.75" spans="1:8">
-      <c r="A23" s="14">
+      <c r="A23" s="17">
         <v>121</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -5766,7 +5892,7 @@
       </c>
     </row>
     <row r="24" ht="85.5" spans="1:8">
-      <c r="A24" s="15">
+      <c r="A24" s="18">
         <v>208</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -5790,10 +5916,10 @@
       <c r="H24" s="4"/>
     </row>
     <row r="25" ht="114" spans="1:8">
-      <c r="A25" s="20">
+      <c r="A25" s="21">
         <v>238</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="20" t="s">
         <v>110</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -5816,10 +5942,10 @@
       </c>
     </row>
     <row r="26" ht="99.75" spans="1:8">
-      <c r="A26" s="21">
+      <c r="A26" s="22">
         <v>53</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="20" t="s">
         <v>116</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -5842,7 +5968,7 @@
       </c>
     </row>
     <row r="27" ht="85.5" spans="1:8">
-      <c r="A27" s="14">
+      <c r="A27" s="17">
         <v>217</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -5868,7 +5994,7 @@
       </c>
     </row>
     <row r="28" ht="85.5" spans="1:8">
-      <c r="A28" s="15">
+      <c r="A28" s="18">
         <v>56</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -5892,7 +6018,7 @@
       <c r="H28" s="4"/>
     </row>
     <row r="29" ht="85.5" spans="1:8">
-      <c r="A29" s="21">
+      <c r="A29" s="22">
         <v>152</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -5916,7 +6042,7 @@
       <c r="H29" s="4"/>
     </row>
     <row r="30" ht="142.5" spans="1:8">
-      <c r="A30" s="21">
+      <c r="A30" s="22">
         <v>15</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -5942,7 +6068,7 @@
       </c>
     </row>
     <row r="31" ht="128.25" spans="1:8">
-      <c r="A31" s="21">
+      <c r="A31" s="22">
         <v>57</v>
       </c>
       <c r="B31" s="5" t="s">
@@ -5966,10 +6092,10 @@
       <c r="H31" s="4"/>
     </row>
     <row r="32" ht="99.75" spans="1:8">
-      <c r="A32" s="22">
+      <c r="A32" s="23">
         <v>70</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="24" t="s">
         <v>148</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -5992,7 +6118,7 @@
       </c>
     </row>
     <row r="33" ht="114" spans="1:8">
-      <c r="A33" s="21">
+      <c r="A33" s="22">
         <v>322</v>
       </c>
       <c r="B33" s="5" t="s">
@@ -6016,7 +6142,7 @@
       <c r="H33" s="4"/>
     </row>
     <row r="34" ht="156.75" spans="1:8">
-      <c r="A34" s="21">
+      <c r="A34" s="22">
         <v>11</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -6042,7 +6168,7 @@
       </c>
     </row>
     <row r="35" ht="199.5" spans="1:8">
-      <c r="A35" s="21">
+      <c r="A35" s="22">
         <v>239</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -6068,7 +6194,7 @@
       </c>
     </row>
     <row r="36" ht="185.25" spans="1:8">
-      <c r="A36" s="14">
+      <c r="A36" s="17">
         <v>242</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -6094,7 +6220,7 @@
       </c>
     </row>
     <row r="37" ht="199.5" spans="1:8">
-      <c r="A37" s="15">
+      <c r="A37" s="18">
         <v>198</v>
       </c>
       <c r="B37" s="5" t="s">
@@ -6120,7 +6246,7 @@
       </c>
     </row>
     <row r="38" ht="99.75" spans="1:8">
-      <c r="A38" s="21">
+      <c r="A38" s="22">
         <v>300</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -6144,7 +6270,7 @@
       <c r="H38" s="4"/>
     </row>
     <row r="39" ht="131" customHeight="1" spans="1:8">
-      <c r="A39" s="21">
+      <c r="A39" s="22">
         <v>371</v>
       </c>
       <c r="B39" s="5" t="s">
@@ -6168,7 +6294,7 @@
       <c r="H39" s="4"/>
     </row>
     <row r="40" ht="128.25" spans="1:8">
-      <c r="A40" s="21">
+      <c r="A40" s="22">
         <v>191</v>
       </c>
       <c r="B40" s="5" t="s">
@@ -6192,7 +6318,7 @@
       <c r="H40" s="4"/>
     </row>
     <row r="41" ht="171" spans="1:8">
-      <c r="A41" s="14">
+      <c r="A41" s="17">
         <v>125</v>
       </c>
       <c r="B41" s="5" t="s">
@@ -6218,7 +6344,7 @@
       </c>
     </row>
     <row r="42" ht="85.5" spans="1:8">
-      <c r="A42" s="21">
+      <c r="A42" s="22">
         <v>3</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -6244,7 +6370,7 @@
       </c>
     </row>
     <row r="43" ht="99.75" spans="1:8">
-      <c r="A43" s="21">
+      <c r="A43" s="22">
         <v>50</v>
       </c>
       <c r="B43" s="5" t="s">
@@ -6268,7 +6394,7 @@
       <c r="H43" s="4"/>
     </row>
     <row r="44" ht="85.5" spans="1:8">
-      <c r="A44" s="21">
+      <c r="A44" s="22">
         <v>69</v>
       </c>
       <c r="B44" s="5" t="s">
@@ -6292,7 +6418,7 @@
       <c r="H44" s="4"/>
     </row>
     <row r="45" ht="208" customHeight="1" spans="1:8">
-      <c r="A45" s="21">
+      <c r="A45" s="22">
         <v>424</v>
       </c>
       <c r="B45" s="5" t="s">
@@ -6318,7 +6444,7 @@
       </c>
     </row>
     <row r="46" ht="85.5" spans="1:8">
-      <c r="A46" s="15">
+      <c r="A46" s="18">
         <v>836</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -6342,7 +6468,7 @@
       <c r="H46" s="4"/>
     </row>
     <row r="47" ht="156" customHeight="1" spans="1:8">
-      <c r="A47" s="14">
+      <c r="A47" s="17">
         <v>383</v>
       </c>
       <c r="B47" s="5" t="s">
@@ -6368,7 +6494,7 @@
       </c>
     </row>
     <row r="48" ht="85.5" spans="1:8">
-      <c r="A48" s="14">
+      <c r="A48" s="17">
         <v>49</v>
       </c>
       <c r="B48" s="5" t="s">
@@ -6394,7 +6520,7 @@
       </c>
     </row>
     <row r="49" ht="85.5" spans="1:8">
-      <c r="A49" s="20">
+      <c r="A49" s="21">
         <v>380</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -6420,7 +6546,7 @@
       </c>
     </row>
     <row r="50" ht="156.75" spans="1:8">
-      <c r="A50" s="20">
+      <c r="A50" s="21">
         <v>41</v>
       </c>
       <c r="B50" s="5" t="s">
@@ -6446,7 +6572,7 @@
       </c>
     </row>
     <row r="51" ht="156.75" spans="1:8">
-      <c r="A51" s="21">
+      <c r="A51" s="22">
         <v>146</v>
       </c>
       <c r="B51" s="5" t="s">
@@ -6472,7 +6598,7 @@
       </c>
     </row>
     <row r="52" ht="71.25" spans="1:8">
-      <c r="A52" s="21">
+      <c r="A52" s="22">
         <v>432</v>
       </c>
       <c r="B52" s="5" t="s">
@@ -6496,7 +6622,7 @@
       </c>
     </row>
     <row r="53" ht="85.5" spans="1:8">
-      <c r="A53" s="15">
+      <c r="A53" s="18">
         <v>21</v>
       </c>
       <c r="B53" s="5" t="s">
@@ -6522,7 +6648,7 @@
       </c>
     </row>
     <row r="54" ht="142.5" spans="1:8">
-      <c r="A54" s="21">
+      <c r="A54" s="22">
         <v>110</v>
       </c>
       <c r="B54" s="5" t="s">
@@ -6546,7 +6672,7 @@
       <c r="H54" s="4"/>
     </row>
     <row r="55" ht="85.5" spans="1:8">
-      <c r="A55" s="15">
+      <c r="A55" s="18">
         <v>278</v>
       </c>
       <c r="B55" s="5" t="s">
@@ -6570,7 +6696,7 @@
       <c r="H55" s="4"/>
     </row>
     <row r="56" ht="99.75" spans="1:8">
-      <c r="A56" s="15">
+      <c r="A56" s="18">
         <v>409</v>
       </c>
       <c r="B56" s="5" t="s">
@@ -6594,7 +6720,7 @@
       <c r="H56" s="4"/>
     </row>
     <row r="57" ht="99.75" spans="1:8">
-      <c r="A57" s="21">
+      <c r="A57" s="22">
         <v>169</v>
       </c>
       <c r="B57" s="5" t="s">
@@ -6616,6 +6742,30 @@
         <v>285</v>
       </c>
       <c r="H57" s="4"/>
+    </row>
+    <row r="58" ht="99.75" spans="1:8">
+      <c r="A58" s="25">
+        <v>67</v>
+      </c>
+      <c r="B58" s="26" t="s">
+        <v>286</v>
+      </c>
+      <c r="C58" s="27" t="s">
+        <v>287</v>
+      </c>
+      <c r="D58" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="E58" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="F58" s="26" t="s">
+        <v>289</v>
+      </c>
+      <c r="G58" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="H58" s="27"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6642,44 +6792,44 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" spans="1:1">
-      <c r="A1" s="9" t="s">
-        <v>286</v>
+      <c r="A1" s="12" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="2" ht="409" customHeight="1" spans="1:1">
-      <c r="A2" s="10" t="s">
-        <v>287</v>
+      <c r="A2" s="13" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="10"/>
+      <c r="A3" s="13"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="10"/>
+      <c r="A4" s="13"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="10"/>
+      <c r="A5" s="13"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="10"/>
+      <c r="A6" s="13"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="10"/>
+      <c r="A7" s="13"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="10"/>
+      <c r="A8" s="13"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="10"/>
+      <c r="A9" s="13"/>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="10"/>
+      <c r="A10" s="13"/>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="10"/>
+      <c r="A11" s="13"/>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="10"/>
+      <c r="A12" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6696,8 +6846,8 @@
   <sheetPr/>
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="7"/>
@@ -6716,7 +6866,7 @@
         <v>148</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>68</v>
+        <v>287</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>149</v>
@@ -6731,18 +6881,18 @@
         <v>152</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="114" spans="1:8">
-      <c r="A2" s="2">
+      <c r="A2" s="7">
         <v>733</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>68</v>
+        <v>287</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>25</v>
@@ -6757,18 +6907,18 @@
         <v>28</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="121.5" spans="1:8">
-      <c r="A3" s="2">
+      <c r="A3" s="7">
         <v>141</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="8" t="s">
         <v>60</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>68</v>
+        <v>287</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>62</v>
@@ -6783,18 +6933,18 @@
         <v>65</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="4" s="1" customFormat="1" ht="114" spans="1:8">
-      <c r="A4" s="7">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="121.5" spans="1:8">
+      <c r="A4" s="9">
         <v>206</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>67</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>68</v>
+        <v>287</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>62</v>
@@ -6805,18 +6955,19 @@
       <c r="F4" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="11" t="s">
         <v>71</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>72</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G1" r:id="rId1" display="https://leetcode.com/problems/climbing-stairs/description/"/>
+    <hyperlink ref="G1" r:id="rId1" display="https://leetcode.com/problems/climbing-stairs/description/" tooltip="https://leetcode.com/problems/climbing-stairs/description/"/>
     <hyperlink ref="G2" r:id="rId2" display="https://leetcode.com/problems/flood-fill/description/"/>
     <hyperlink ref="G3" r:id="rId3" display="https://leetcode.com/problems/linked-list-cycle/description/"/>
+    <hyperlink ref="G4" r:id="rId4" display="https://leetcode.com/problems/reverse-linked-list/description/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
[LC] Update Diameter of Binary Tree and question review.
</commit_message>
<xml_diff>
--- a/Leetcode/Problem-tracker.xlsx
+++ b/Leetcode/Problem-tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12960"/>
+    <workbookView windowWidth="22188" windowHeight="9767"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="307">
   <si>
     <t>No.</t>
   </si>
@@ -82,10 +82,102 @@
     <t>K Closet Points to Origin</t>
   </si>
   <si>
-    <t>2025.2.11</t>
+    <t>2025.3.3</t>
   </si>
   <si>
     <t>Heap</t>
+  </si>
+  <si>
+    <r>
+      <t>Problem Pattern: This problem follows the "Find K Smallest/Largest Elements" pattern. The key idea is to efficiently find the K closest points to (0,0) based on Euclidean distance (x² + y²).
+Solution Approach: Use Heap (O(n log k)), Sorting (O(n log n)), or Quickselect (O(n) average case).</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+Solved second time, be familiar with the usage of heap.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+heap = []  //  heappush(heap, ())  //  heappop(heap)
+What i was doing: compare the max value of the heap then if smaller, push.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Alternative: push first, then if larger than k, pop
+TC: O(nlogk)
+SC: O(k)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When needing the top </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>K smallest or largest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> elements efficiently.
+2. When solving </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>nearest neighbor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> or distance-based ranking problems.
+3. When optimizing data retrieval with heaps or partitioning methods</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/k-closest-points-to-origin/description/</t>
+  </si>
+  <si>
+    <t>2025.3.3; 2025.2.11</t>
   </si>
   <si>
     <t>Merge K Sorted List</t>
@@ -726,6 +818,9 @@
   </si>
   <si>
     <t>Best Time to Buy and Sell Stock</t>
+  </si>
+  <si>
+    <t>2025.2.11</t>
   </si>
   <si>
     <t>Array; Sub-array</t>
@@ -4135,6 +4230,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t>Problem Pattern: This problem follows the "</t>
     </r>
     <r>
@@ -4225,6 +4326,97 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/add-binary/description/</t>
+  </si>
+  <si>
+    <t>Diameter of Binary Tree</t>
+  </si>
+  <si>
+    <t>Tree; DFS</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem Pattern: This problem follows the "Tree Depth Calculation &amp; Path Length" pattern. The key idea is to compute the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>longest path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> (diameter) between two nodes in a binary tree, which may or may not pass through the root.
+Solution Approach: Use postorder DFS traversal to compute subtree heights while keeping </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>track of the maximum path length</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> (left height + right height) encountered. Runs in O(n) time complexity with O(h) space for recursion (O(log n) for balanced trees, O(n) worst case for skewed trees).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Not Solved first time, stuck at local variable in recursion
+Heads up: the longest is not necessarily through the roor</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. When finding the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t>longest path between any two nodes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> in a tree.
+2. When solving problems involving tree height and depth calculations.
+3. When optimizing network routing or tree-based path analysis.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/diameter-of-binary-tree/description/</t>
   </si>
   <si>
     <t>Prompt</t>
@@ -4258,13 +4450,13 @@
     <t>20255.3.1; 2025.2.28; 2025.2.27; 2025.2.26; 2025.2.15</t>
   </si>
   <si>
-    <t>2025.3.1; 2025.2.27; 2025.2.24; 2025.2.8</t>
-  </si>
-  <si>
-    <t>2025.3.1; 2025.2.27; 2025.2.25; 2025.1.31</t>
-  </si>
-  <si>
-    <t>2025.3.1; 2025.2.27; 2025.1.31</t>
+    <t>2025.3.3; 2025.3.1; 2025.2.27; 2025.2.24; 2025.2.8</t>
+  </si>
+  <si>
+    <t>2025.3.3; 2025.3.1; 2025.2.27; 2025.2.25; 2025.1.31</t>
+  </si>
+  <si>
+    <t>2025.3.3; 2025.3.1; 2025.2.27; 2025.1.31</t>
   </si>
 </sst>
 </file>
@@ -4277,7 +4469,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4306,25 +4498,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Cambria"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Cambria"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -4337,6 +4514,14 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4467,8 +4652,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <i/>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -4476,6 +4659,8 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <i/>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -4836,7 +5021,7 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4845,124 +5030,124 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4988,21 +5173,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -5012,15 +5194,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5030,16 +5215,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5362,53 +5547,53 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="6.75" style="14" customWidth="1"/>
-    <col min="2" max="2" width="25.6333333333333" style="13" customWidth="1"/>
+    <col min="1" max="1" width="6.75" style="13" customWidth="1"/>
+    <col min="2" max="2" width="25.6296296296296" style="12" customWidth="1"/>
     <col min="3" max="3" width="12.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3583333333333" style="13" customWidth="1"/>
-    <col min="5" max="5" width="94.9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="43.2583333333333" style="13" customWidth="1"/>
-    <col min="7" max="7" width="18.3" style="13" customWidth="1"/>
+    <col min="4" max="4" width="11.3611111111111" style="12" customWidth="1"/>
+    <col min="5" max="5" width="94.8981481481482" style="1" customWidth="1"/>
+    <col min="6" max="6" width="43.2592592592593" style="12" customWidth="1"/>
+    <col min="7" max="7" width="18.2962962962963" style="12" customWidth="1"/>
     <col min="8" max="8" width="32.6666666666667" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="14" customFormat="1" spans="1:8">
-      <c r="A1" s="15" t="s">
+    <row r="1" s="13" customFormat="1" spans="1:8">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" ht="85.5" spans="1:8">
-      <c r="A2" s="17">
+    <row r="2" ht="96.6" spans="1:8">
+      <c r="A2" s="16">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -5433,8 +5618,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="18">
+    <row r="3" ht="124.2" spans="1:8">
+      <c r="A3" s="17">
         <v>973</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -5446,20 +5631,28 @@
       <c r="D3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="4"/>
+      <c r="E3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="18">
         <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>17</v>
@@ -5474,43 +5667,43 @@
         <v>542</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" ht="85.5" spans="1:8">
+    <row r="6" ht="96.6" spans="1:8">
       <c r="A6" s="19">
         <v>733</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -5518,209 +5711,209 @@
         <v>200</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" ht="85.5" spans="1:8">
+    <row r="8" ht="96.6" spans="1:8">
       <c r="A8" s="19">
         <v>235</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" ht="85.5" spans="1:8">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" ht="82.8" spans="1:8">
       <c r="A9" s="19">
         <v>226</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" ht="27.6" spans="1:8">
       <c r="A10" s="18">
         <v>104</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" ht="85.5" spans="1:8">
+    <row r="11" ht="82.8" spans="1:8">
       <c r="A11" s="19">
         <v>232</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" ht="99.75" spans="1:8">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" ht="110.4" spans="1:8">
       <c r="A12" s="19">
         <v>20</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" ht="27.6" spans="1:8">
       <c r="A13" s="18">
         <v>225</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" ht="71.25" spans="1:8">
+    <row r="14" ht="96.6" spans="1:8">
       <c r="A14" s="19">
         <v>141</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" ht="85.5" spans="1:8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" ht="82.8" spans="1:8">
       <c r="A15" s="19">
         <v>206</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -5728,13 +5921,13 @@
         <v>54</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="5"/>
@@ -5746,69 +5939,69 @@
         <v>73</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" ht="85.5" spans="1:8">
+    <row r="18" ht="82.8" spans="1:8">
       <c r="A18" s="19">
         <v>33</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" ht="99.75" spans="1:8">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" ht="110.4" spans="1:8">
       <c r="A19" s="19">
         <v>704</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -5816,13 +6009,13 @@
         <v>78</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="5"/>
@@ -5834,13 +6027,13 @@
         <v>77</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="5"/>
@@ -5852,420 +6045,420 @@
         <v>22</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>93</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" ht="99.75" spans="1:8">
-      <c r="A23" s="17">
+    <row r="23" ht="138" spans="1:8">
+      <c r="A23" s="16">
         <v>121</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>16</v>
+        <v>103</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" ht="85.5" spans="1:8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" ht="96.6" spans="1:8">
       <c r="A24" s="18">
         <v>208</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" ht="114" spans="1:8">
+    <row r="25" ht="124.2" spans="1:8">
       <c r="A25" s="21">
         <v>238</v>
       </c>
       <c r="B25" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>105</v>
-      </c>
       <c r="D25" s="5" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="26" ht="99.75" spans="1:8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" ht="96.6" spans="1:8">
       <c r="A26" s="22">
         <v>53</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="27" ht="85.5" spans="1:8">
-      <c r="A27" s="17">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" ht="82.8" spans="1:8">
+      <c r="A27" s="16">
         <v>217</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="28" ht="85.5" spans="1:8">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" ht="82.8" spans="1:8">
       <c r="A28" s="18">
         <v>56</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" ht="85.5" spans="1:8">
+    <row r="29" ht="110.4" spans="1:8">
       <c r="A29" s="22">
         <v>152</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" ht="142.5" spans="1:8">
+    <row r="30" ht="153.6" spans="1:8">
       <c r="A30" s="22">
         <v>15</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="31" ht="128.25" spans="1:8">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" ht="124.2" spans="1:8">
       <c r="A31" s="22">
         <v>57</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" ht="99.75" spans="1:8">
+    <row r="32" ht="110.4" spans="1:8">
       <c r="A32" s="23">
         <v>70</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="33" ht="114" spans="1:8">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="33" ht="124.2" spans="1:8">
       <c r="A33" s="22">
         <v>322</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>149</v>
-      </c>
       <c r="E33" s="5" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" ht="156.75" spans="1:8">
+    <row r="34" ht="151.8" spans="1:8">
       <c r="A34" s="22">
         <v>11</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="35" ht="199.5" spans="1:8">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" ht="193.2" spans="1:8">
       <c r="A35" s="22">
         <v>239</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="36" ht="185.25" spans="1:8">
-      <c r="A36" s="17">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="36" ht="179.4" spans="1:8">
+      <c r="A36" s="16">
         <v>242</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="G36" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="H36" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="H36" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="37" ht="199.5" spans="1:8">
+    </row>
+    <row r="37" ht="193.2" spans="1:8">
       <c r="A37" s="18">
         <v>198</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="38" ht="99.75" spans="1:8">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="38" ht="110.4" spans="1:8">
       <c r="A38" s="22">
         <v>300</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="H38" s="4"/>
     </row>
@@ -6274,146 +6467,146 @@
         <v>371</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" ht="128.25" spans="1:8">
+    <row r="40" ht="124.2" spans="1:8">
       <c r="A40" s="22">
         <v>191</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="C40" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>189</v>
-      </c>
       <c r="E40" s="5" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" ht="171" spans="1:8">
-      <c r="A41" s="17">
+    <row r="41" ht="179.4" spans="1:8">
+      <c r="A41" s="16">
         <v>125</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="42" ht="85.5" spans="1:8">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="42" ht="96.6" spans="1:8">
       <c r="A42" s="22">
         <v>3</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="43" ht="99.75" spans="1:8">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="43" ht="110.4" spans="1:8">
       <c r="A43" s="22">
         <v>50</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="H43" s="4"/>
     </row>
-    <row r="44" ht="85.5" spans="1:8">
+    <row r="44" ht="110.4" spans="1:8">
       <c r="A44" s="22">
         <v>69</v>
       </c>
       <c r="B44" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>211</v>
-      </c>
       <c r="D44" s="5" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="H44" s="4"/>
     </row>
@@ -6422,109 +6615,109 @@
         <v>424</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="46" ht="85.5" spans="1:8">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="46" ht="82.8" spans="1:8">
       <c r="A46" s="18">
         <v>836</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="H46" s="4"/>
     </row>
     <row r="47" ht="156" customHeight="1" spans="1:8">
-      <c r="A47" s="17">
+      <c r="A47" s="16">
         <v>383</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="48" ht="85.5" spans="1:8">
-      <c r="A48" s="17">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="48" ht="82.8" spans="1:8">
+      <c r="A48" s="16">
         <v>49</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="49" ht="85.5" spans="1:8">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="49" ht="82.8" spans="1:8">
       <c r="A49" s="21">
         <v>380</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>9</v>
@@ -6533,239 +6726,263 @@
         <v>10</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="50" ht="156.75" spans="1:8">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="50" ht="179.4" spans="1:8">
       <c r="A50" s="21">
         <v>41</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="51" ht="156.75" spans="1:8">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="51" ht="151.8" spans="1:8">
       <c r="A51" s="22">
         <v>146</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="52" ht="71.25" spans="1:8">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="52" ht="69" spans="1:8">
       <c r="A52" s="22">
         <v>432</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="F52" s="5"/>
       <c r="G52" s="5" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="53" ht="85.5" spans="1:8">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="53" ht="82.8" spans="1:8">
       <c r="A53" s="18">
         <v>21</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="54" ht="142.5" spans="1:8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" ht="138" spans="1:8">
       <c r="A54" s="22">
         <v>110</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="H54" s="4"/>
     </row>
-    <row r="55" ht="85.5" spans="1:8">
+    <row r="55" ht="82.8" spans="1:8">
       <c r="A55" s="18">
         <v>278</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="H55" s="4"/>
     </row>
-    <row r="56" ht="99.75" spans="1:8">
+    <row r="56" ht="110.4" spans="1:8">
       <c r="A56" s="18">
         <v>409</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="H56" s="4"/>
     </row>
-    <row r="57" ht="99.75" spans="1:8">
+    <row r="57" ht="110.4" spans="1:8">
       <c r="A57" s="22">
         <v>169</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="H57" s="4"/>
     </row>
-    <row r="58" ht="99.75" spans="1:8">
-      <c r="A58" s="25">
+    <row r="58" ht="124.2" spans="1:8">
+      <c r="A58" s="22">
         <v>67</v>
       </c>
-      <c r="B58" s="26" t="s">
-        <v>286</v>
-      </c>
-      <c r="C58" s="27" t="s">
-        <v>287</v>
-      </c>
-      <c r="D58" s="26" t="s">
-        <v>189</v>
-      </c>
-      <c r="E58" s="26" t="s">
-        <v>288</v>
-      </c>
-      <c r="F58" s="26" t="s">
-        <v>289</v>
-      </c>
-      <c r="G58" s="26" t="s">
-        <v>290</v>
-      </c>
-      <c r="H58" s="27"/>
+      <c r="B58" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="H58" s="4"/>
+    </row>
+    <row r="59" ht="110.4" spans="1:8">
+      <c r="A59" s="25">
+        <v>543</v>
+      </c>
+      <c r="B59" s="26" t="s">
+        <v>296</v>
+      </c>
+      <c r="C59" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D59" s="26" t="s">
+        <v>297</v>
+      </c>
+      <c r="E59" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="F59" s="26" t="s">
+        <v>299</v>
+      </c>
+      <c r="G59" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="H59" s="27"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6786,50 +7003,50 @@
       <selection activeCell="A2" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="195.133333333333" customWidth="1"/>
+    <col min="1" max="1" width="195.12962962963" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" spans="1:1">
-      <c r="A1" s="12" t="s">
-        <v>291</v>
+    <row r="1" spans="1:1">
+      <c r="A1" s="11" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="2" ht="409" customHeight="1" spans="1:1">
-      <c r="A2" s="13" t="s">
-        <v>292</v>
+      <c r="A2" s="12" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="13"/>
+      <c r="A3" s="12"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="13"/>
+      <c r="A4" s="12"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="13"/>
+      <c r="A5" s="12"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="13"/>
+      <c r="A6" s="12"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="13"/>
+      <c r="A7" s="12"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="13"/>
+      <c r="A8" s="12"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="13"/>
+      <c r="A9" s="12"/>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="13"/>
+      <c r="A10" s="12"/>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="13"/>
+      <c r="A11" s="12"/>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="13"/>
+      <c r="A12" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6846,16 +7063,16 @@
   <sheetPr/>
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="24.1083333333333" customWidth="1"/>
-    <col min="5" max="5" width="63.4416666666667" customWidth="1"/>
+    <col min="2" max="2" width="24.1111111111111" customWidth="1"/>
+    <col min="5" max="5" width="63.4444444444444" customWidth="1"/>
     <col min="6" max="6" width="38" customWidth="1"/>
-    <col min="8" max="8" width="30.225" customWidth="1"/>
+    <col min="8" max="8" width="30.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="141" customHeight="1" spans="1:8">
@@ -6863,103 +7080,103 @@
         <v>70</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="2" s="1" customFormat="1" ht="114" spans="1:8">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="124.2" spans="1:8">
       <c r="A2" s="7">
         <v>733</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>287</v>
+        <v>16</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="3" s="1" customFormat="1" ht="121.5" spans="1:8">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="129.6" spans="1:8">
       <c r="A3" s="7">
         <v>141</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>287</v>
+        <v>16</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="4" s="1" customFormat="1" ht="121.5" spans="1:8">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="129.6" spans="1:8">
       <c r="A4" s="9">
         <v>206</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>287</v>
+        <v>16</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>71</v>
+        <v>74</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>296</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[DATA200] Update notes for lecture 22
</commit_message>
<xml_diff>
--- a/Leetcode/Problem-tracker.xlsx
+++ b/Leetcode/Problem-tracker.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9767"/>
+    <workbookView windowWidth="27945" windowHeight="12960"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="prompt" sheetId="2" r:id="rId2"/>
     <sheet name="Must be reviewed every day" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t>Problem Pattern: This problem follows the "Find K Smallest/Largest Elements" pattern. The key idea is to efficiently find the K closest points to (0,0) based on Euclidean distance (x² + y²).
 Solution Approach: Use Heap (O(n log k)), Sorting (O(n log n)), or Quickselect (O(n) average case).</t>
     </r>
@@ -130,6 +136,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When needing the top </t>
     </r>
     <r>
@@ -4335,6 +4347,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Tree Depth Calculation &amp; Path Length" pattern. The key idea is to compute the </t>
     </r>
     <r>
@@ -4391,6 +4409,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">1. When finding the </t>
     </r>
     <r>
@@ -5151,7 +5175,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5171,12 +5195,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5210,9 +5228,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5226,15 +5241,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -5553,47 +5559,47 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="6.75" style="13" customWidth="1"/>
-    <col min="2" max="2" width="25.6296296296296" style="12" customWidth="1"/>
+    <col min="1" max="1" width="6.75" style="11" customWidth="1"/>
+    <col min="2" max="2" width="25.6333333333333" style="10" customWidth="1"/>
     <col min="3" max="3" width="12.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3611111111111" style="12" customWidth="1"/>
-    <col min="5" max="5" width="94.8981481481482" style="1" customWidth="1"/>
-    <col min="6" max="6" width="43.2592592592593" style="12" customWidth="1"/>
-    <col min="7" max="7" width="18.2962962962963" style="12" customWidth="1"/>
+    <col min="4" max="4" width="11.3583333333333" style="10" customWidth="1"/>
+    <col min="5" max="5" width="94.9" style="1" customWidth="1"/>
+    <col min="6" max="6" width="43.2583333333333" style="10" customWidth="1"/>
+    <col min="7" max="7" width="18.3" style="10" customWidth="1"/>
     <col min="8" max="8" width="32.6666666666667" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="13" customFormat="1" spans="1:8">
-      <c r="A1" s="14" t="s">
+    <row r="1" s="11" customFormat="1" spans="1:8">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" ht="96.6" spans="1:8">
-      <c r="A2" s="16">
+    <row r="2" ht="85.5" spans="1:8">
+      <c r="A2" s="14">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -5618,8 +5624,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" ht="124.2" spans="1:8">
-      <c r="A3" s="17">
+    <row r="3" ht="128.25" spans="1:8">
+      <c r="A3" s="15">
         <v>973</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -5645,7 +5651,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="18">
+      <c r="A4" s="16">
         <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -5663,7 +5669,7 @@
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="18">
+      <c r="A5" s="16">
         <v>542</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -5680,11 +5686,11 @@
       <c r="G5" s="5"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" ht="96.6" spans="1:8">
-      <c r="A6" s="19">
+    <row r="6" ht="85.5" spans="1:8">
+      <c r="A6" s="15">
         <v>733</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="17" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -5707,7 +5713,7 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="18">
+      <c r="A7" s="16">
         <v>200</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -5724,11 +5730,11 @@
       <c r="G7" s="5"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" ht="96.6" spans="1:8">
-      <c r="A8" s="19">
+    <row r="8" ht="85.5" spans="1:8">
+      <c r="A8" s="15">
         <v>235</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="17" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -5750,11 +5756,11 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" ht="82.8" spans="1:8">
-      <c r="A9" s="19">
+    <row r="9" ht="85.5" spans="1:8">
+      <c r="A9" s="15">
         <v>226</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -5776,8 +5782,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" ht="27.6" spans="1:8">
-      <c r="A10" s="18">
+    <row r="10" spans="1:8">
+      <c r="A10" s="16">
         <v>104</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -5794,11 +5800,11 @@
       <c r="G10" s="5"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" ht="82.8" spans="1:8">
-      <c r="A11" s="19">
+    <row r="11" ht="85.5" spans="1:8">
+      <c r="A11" s="15">
         <v>232</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="17" t="s">
         <v>49</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -5820,11 +5826,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" ht="110.4" spans="1:8">
-      <c r="A12" s="19">
+    <row r="12" ht="99.75" spans="1:8">
+      <c r="A12" s="15">
         <v>20</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="17" t="s">
         <v>56</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -5846,8 +5852,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" ht="27.6" spans="1:8">
-      <c r="A13" s="18">
+    <row r="13" spans="1:8">
+      <c r="A13" s="16">
         <v>225</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -5864,11 +5870,11 @@
       <c r="G13" s="5"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" ht="96.6" spans="1:8">
-      <c r="A14" s="19">
+    <row r="14" ht="71.25" spans="1:8">
+      <c r="A14" s="15">
         <v>141</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="17" t="s">
         <v>64</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -5890,11 +5896,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" ht="82.8" spans="1:8">
-      <c r="A15" s="19">
+    <row r="15" ht="85.5" spans="1:8">
+      <c r="A15" s="15">
         <v>206</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="17" t="s">
         <v>71</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -5917,7 +5923,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="18">
+      <c r="A16" s="16">
         <v>54</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -5935,7 +5941,7 @@
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="18">
+      <c r="A17" s="16">
         <v>73</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -5952,8 +5958,8 @@
       <c r="G17" s="5"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" ht="82.8" spans="1:8">
-      <c r="A18" s="19">
+    <row r="18" ht="85.5" spans="1:8">
+      <c r="A18" s="15">
         <v>33</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -5978,11 +5984,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" ht="110.4" spans="1:8">
-      <c r="A19" s="19">
+    <row r="19" ht="99.75" spans="1:8">
+      <c r="A19" s="15">
         <v>704</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="17" t="s">
         <v>89</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -6005,7 +6011,7 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="18">
+      <c r="A20" s="16">
         <v>78</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -6023,7 +6029,7 @@
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="18">
+      <c r="A21" s="16">
         <v>77</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -6041,7 +6047,7 @@
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="18">
+      <c r="A22" s="16">
         <v>22</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -6058,8 +6064,8 @@
       <c r="G22" s="5"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" ht="138" spans="1:8">
-      <c r="A23" s="16">
+    <row r="23" ht="99.75" spans="1:8">
+      <c r="A23" s="14">
         <v>121</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -6084,8 +6090,8 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24" ht="96.6" spans="1:8">
-      <c r="A24" s="18">
+    <row r="24" ht="85.5" spans="1:8">
+      <c r="A24" s="16">
         <v>208</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -6108,11 +6114,11 @@
       </c>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" ht="124.2" spans="1:8">
-      <c r="A25" s="21">
+    <row r="25" ht="114" spans="1:8">
+      <c r="A25" s="18">
         <v>238</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="17" t="s">
         <v>115</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -6134,11 +6140,11 @@
         <v>120</v>
       </c>
     </row>
-    <row r="26" ht="96.6" spans="1:8">
-      <c r="A26" s="22">
+    <row r="26" ht="99.75" spans="1:8">
+      <c r="A26" s="19">
         <v>53</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="17" t="s">
         <v>121</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -6160,8 +6166,8 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" ht="82.8" spans="1:8">
-      <c r="A27" s="16">
+    <row r="27" ht="85.5" spans="1:8">
+      <c r="A27" s="14">
         <v>217</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -6186,8 +6192,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="28" ht="82.8" spans="1:8">
-      <c r="A28" s="18">
+    <row r="28" ht="85.5" spans="1:8">
+      <c r="A28" s="16">
         <v>56</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -6210,8 +6216,8 @@
       </c>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" ht="110.4" spans="1:8">
-      <c r="A29" s="22">
+    <row r="29" ht="85.5" spans="1:8">
+      <c r="A29" s="19">
         <v>152</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -6234,8 +6240,8 @@
       </c>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" ht="153.6" spans="1:8">
-      <c r="A30" s="22">
+    <row r="30" ht="142.5" spans="1:8">
+      <c r="A30" s="19">
         <v>15</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -6260,8 +6266,8 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" ht="124.2" spans="1:8">
-      <c r="A31" s="22">
+    <row r="31" ht="128.25" spans="1:8">
+      <c r="A31" s="19">
         <v>57</v>
       </c>
       <c r="B31" s="5" t="s">
@@ -6284,11 +6290,11 @@
       </c>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" ht="110.4" spans="1:8">
-      <c r="A32" s="23">
+    <row r="32" ht="99.75" spans="1:8">
+      <c r="A32" s="20">
         <v>70</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="21" t="s">
         <v>153</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -6310,8 +6316,8 @@
         <v>158</v>
       </c>
     </row>
-    <row r="33" ht="124.2" spans="1:8">
-      <c r="A33" s="22">
+    <row r="33" ht="114" spans="1:8">
+      <c r="A33" s="19">
         <v>322</v>
       </c>
       <c r="B33" s="5" t="s">
@@ -6334,8 +6340,8 @@
       </c>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" ht="151.8" spans="1:8">
-      <c r="A34" s="22">
+    <row r="34" ht="156.75" spans="1:8">
+      <c r="A34" s="19">
         <v>11</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -6360,8 +6366,8 @@
         <v>169</v>
       </c>
     </row>
-    <row r="35" ht="193.2" spans="1:8">
-      <c r="A35" s="22">
+    <row r="35" ht="199.5" spans="1:8">
+      <c r="A35" s="19">
         <v>239</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -6386,8 +6392,8 @@
         <v>175</v>
       </c>
     </row>
-    <row r="36" ht="179.4" spans="1:8">
-      <c r="A36" s="16">
+    <row r="36" ht="185.25" spans="1:8">
+      <c r="A36" s="14">
         <v>242</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -6412,8 +6418,8 @@
         <v>175</v>
       </c>
     </row>
-    <row r="37" ht="193.2" spans="1:8">
-      <c r="A37" s="18">
+    <row r="37" ht="199.5" spans="1:8">
+      <c r="A37" s="16">
         <v>198</v>
       </c>
       <c r="B37" s="5" t="s">
@@ -6438,8 +6444,8 @@
         <v>182</v>
       </c>
     </row>
-    <row r="38" ht="110.4" spans="1:8">
-      <c r="A38" s="22">
+    <row r="38" ht="99.75" spans="1:8">
+      <c r="A38" s="19">
         <v>300</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -6463,7 +6469,7 @@
       <c r="H38" s="4"/>
     </row>
     <row r="39" ht="131" customHeight="1" spans="1:8">
-      <c r="A39" s="22">
+      <c r="A39" s="19">
         <v>371</v>
       </c>
       <c r="B39" s="5" t="s">
@@ -6486,8 +6492,8 @@
       </c>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" ht="124.2" spans="1:8">
-      <c r="A40" s="22">
+    <row r="40" ht="128.25" spans="1:8">
+      <c r="A40" s="19">
         <v>191</v>
       </c>
       <c r="B40" s="5" t="s">
@@ -6510,8 +6516,8 @@
       </c>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" ht="179.4" spans="1:8">
-      <c r="A41" s="16">
+    <row r="41" ht="171" spans="1:8">
+      <c r="A41" s="14">
         <v>125</v>
       </c>
       <c r="B41" s="5" t="s">
@@ -6536,8 +6542,8 @@
         <v>208</v>
       </c>
     </row>
-    <row r="42" ht="96.6" spans="1:8">
-      <c r="A42" s="22">
+    <row r="42" ht="85.5" spans="1:8">
+      <c r="A42" s="19">
         <v>3</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -6562,8 +6568,8 @@
         <v>214</v>
       </c>
     </row>
-    <row r="43" ht="110.4" spans="1:8">
-      <c r="A43" s="22">
+    <row r="43" ht="99.75" spans="1:8">
+      <c r="A43" s="19">
         <v>50</v>
       </c>
       <c r="B43" s="5" t="s">
@@ -6586,8 +6592,8 @@
       </c>
       <c r="H43" s="4"/>
     </row>
-    <row r="44" ht="110.4" spans="1:8">
-      <c r="A44" s="22">
+    <row r="44" ht="85.5" spans="1:8">
+      <c r="A44" s="19">
         <v>69</v>
       </c>
       <c r="B44" s="5" t="s">
@@ -6611,7 +6617,7 @@
       <c r="H44" s="4"/>
     </row>
     <row r="45" ht="208" customHeight="1" spans="1:8">
-      <c r="A45" s="22">
+      <c r="A45" s="19">
         <v>424</v>
       </c>
       <c r="B45" s="5" t="s">
@@ -6636,8 +6642,8 @@
         <v>230</v>
       </c>
     </row>
-    <row r="46" ht="82.8" spans="1:8">
-      <c r="A46" s="18">
+    <row r="46" ht="85.5" spans="1:8">
+      <c r="A46" s="16">
         <v>836</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -6661,7 +6667,7 @@
       <c r="H46" s="4"/>
     </row>
     <row r="47" ht="156" customHeight="1" spans="1:8">
-      <c r="A47" s="16">
+      <c r="A47" s="14">
         <v>383</v>
       </c>
       <c r="B47" s="5" t="s">
@@ -6686,8 +6692,8 @@
         <v>241</v>
       </c>
     </row>
-    <row r="48" ht="82.8" spans="1:8">
-      <c r="A48" s="16">
+    <row r="48" ht="85.5" spans="1:8">
+      <c r="A48" s="14">
         <v>49</v>
       </c>
       <c r="B48" s="5" t="s">
@@ -6712,8 +6718,8 @@
         <v>247</v>
       </c>
     </row>
-    <row r="49" ht="82.8" spans="1:8">
-      <c r="A49" s="21">
+    <row r="49" ht="85.5" spans="1:8">
+      <c r="A49" s="18">
         <v>380</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -6738,8 +6744,8 @@
         <v>252</v>
       </c>
     </row>
-    <row r="50" ht="179.4" spans="1:8">
-      <c r="A50" s="21">
+    <row r="50" ht="156.75" spans="1:8">
+      <c r="A50" s="18">
         <v>41</v>
       </c>
       <c r="B50" s="5" t="s">
@@ -6764,8 +6770,8 @@
         <v>258</v>
       </c>
     </row>
-    <row r="51" ht="151.8" spans="1:8">
-      <c r="A51" s="22">
+    <row r="51" ht="156.75" spans="1:8">
+      <c r="A51" s="19">
         <v>146</v>
       </c>
       <c r="B51" s="5" t="s">
@@ -6790,8 +6796,8 @@
         <v>265</v>
       </c>
     </row>
-    <row r="52" ht="69" spans="1:8">
-      <c r="A52" s="22">
+    <row r="52" ht="71.25" spans="1:8">
+      <c r="A52" s="19">
         <v>432</v>
       </c>
       <c r="B52" s="5" t="s">
@@ -6814,8 +6820,8 @@
         <v>265</v>
       </c>
     </row>
-    <row r="53" ht="82.8" spans="1:8">
-      <c r="A53" s="18">
+    <row r="53" ht="85.5" spans="1:8">
+      <c r="A53" s="16">
         <v>21</v>
       </c>
       <c r="B53" s="5" t="s">
@@ -6840,8 +6846,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" ht="138" spans="1:8">
-      <c r="A54" s="22">
+    <row r="54" ht="142.5" spans="1:8">
+      <c r="A54" s="19">
         <v>110</v>
       </c>
       <c r="B54" s="5" t="s">
@@ -6864,8 +6870,8 @@
       </c>
       <c r="H54" s="4"/>
     </row>
-    <row r="55" ht="82.8" spans="1:8">
-      <c r="A55" s="18">
+    <row r="55" ht="85.5" spans="1:8">
+      <c r="A55" s="16">
         <v>278</v>
       </c>
       <c r="B55" s="5" t="s">
@@ -6888,8 +6894,8 @@
       </c>
       <c r="H55" s="4"/>
     </row>
-    <row r="56" ht="110.4" spans="1:8">
-      <c r="A56" s="18">
+    <row r="56" ht="99.75" spans="1:8">
+      <c r="A56" s="16">
         <v>409</v>
       </c>
       <c r="B56" s="5" t="s">
@@ -6912,8 +6918,8 @@
       </c>
       <c r="H56" s="4"/>
     </row>
-    <row r="57" ht="110.4" spans="1:8">
-      <c r="A57" s="22">
+    <row r="57" ht="99.75" spans="1:8">
+      <c r="A57" s="19">
         <v>169</v>
       </c>
       <c r="B57" s="5" t="s">
@@ -6936,8 +6942,8 @@
       </c>
       <c r="H57" s="4"/>
     </row>
-    <row r="58" ht="124.2" spans="1:8">
-      <c r="A58" s="22">
+    <row r="58" ht="99.75" spans="1:8">
+      <c r="A58" s="19">
         <v>67</v>
       </c>
       <c r="B58" s="5" t="s">
@@ -6960,29 +6966,29 @@
       </c>
       <c r="H58" s="4"/>
     </row>
-    <row r="59" ht="110.4" spans="1:8">
-      <c r="A59" s="25">
+    <row r="59" ht="99.75" spans="1:8">
+      <c r="A59" s="19">
         <v>543</v>
       </c>
-      <c r="B59" s="26" t="s">
+      <c r="B59" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="C59" s="27" t="s">
+      <c r="C59" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D59" s="26" t="s">
+      <c r="D59" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="E59" s="26" t="s">
+      <c r="E59" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="F59" s="26" t="s">
+      <c r="F59" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="G59" s="26" t="s">
+      <c r="G59" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="H59" s="27"/>
+      <c r="H59" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -7000,53 +7006,53 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A12"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="195.12962962963" customWidth="1"/>
+    <col min="1" max="1" width="195.133333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="11" t="s">
+    <row r="1" ht="14.25" spans="1:1">
+      <c r="A1" s="9" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="2" ht="409" customHeight="1" spans="1:1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="10" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="12"/>
+      <c r="A3" s="10"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="12"/>
+      <c r="A4" s="10"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="12"/>
+      <c r="A5" s="10"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="12"/>
+      <c r="A6" s="10"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="12"/>
+      <c r="A7" s="10"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="12"/>
+      <c r="A8" s="10"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="12"/>
+      <c r="A9" s="10"/>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="12"/>
+      <c r="A10" s="10"/>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="12"/>
+      <c r="A11" s="10"/>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="12"/>
+      <c r="A12" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7063,16 +7069,16 @@
   <sheetPr/>
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="24.1111111111111" customWidth="1"/>
-    <col min="5" max="5" width="63.4444444444444" customWidth="1"/>
+    <col min="2" max="2" width="24.1083333333333" customWidth="1"/>
+    <col min="5" max="5" width="63.4416666666667" customWidth="1"/>
     <col min="6" max="6" width="38" customWidth="1"/>
-    <col min="8" max="8" width="30.2222222222222" customWidth="1"/>
+    <col min="8" max="8" width="30.225" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="141" customHeight="1" spans="1:8">
@@ -7101,11 +7107,11 @@
         <v>303</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="124.2" spans="1:8">
-      <c r="A2" s="7">
+    <row r="2" s="1" customFormat="1" ht="114" spans="1:8">
+      <c r="A2" s="2">
         <v>733</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -7127,11 +7133,11 @@
         <v>304</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="129.6" spans="1:8">
-      <c r="A3" s="7">
+    <row r="3" s="1" customFormat="1" ht="121.5" spans="1:8">
+      <c r="A3" s="2">
         <v>141</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -7153,11 +7159,11 @@
         <v>305</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="129.6" spans="1:8">
-      <c r="A4" s="9">
+    <row r="4" s="1" customFormat="1" ht="121.5" spans="1:8">
+      <c r="A4" s="7">
         <v>206</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>71</v>
       </c>
       <c r="C4" s="4" t="s">

</xml_diff>